<commit_message>
DA 16 | Day 5
</commit_message>
<xml_diff>
--- a/Batch/16/Curriculum/Day_5_Lookup.xlsx
+++ b/Batch/16/Curriculum/Day_5_Lookup.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28613"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\Acciojob\Modules\Excel\Batch\16\Curriculum\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAC17A1D-8B64-42BF-B6DF-24596683782F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF1E85CD-2DF9-40FB-A9EB-11D5C68ADC19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="30" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="30" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Vlookup" sheetId="1" r:id="rId1"/>
@@ -44,8 +44,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="86">
   <si>
     <t>VLookup</t>
   </si>
@@ -287,22 +309,25 @@
     <t>Returns the number of columns covered in the array {1,2,3;4,5,6}. Note that comma denotes column and semi-colon denotes row</t>
   </si>
   <si>
-    <t>Order</t>
-  </si>
-  <si>
-    <t>Limitation Of the Vlookup</t>
-  </si>
-  <si>
-    <t>Index Match</t>
-  </si>
-  <si>
-    <t>xlookup</t>
-  </si>
-  <si>
     <t>=INDEX(B2:C7,MATCH(C11,C2:C7,0),1)</t>
   </si>
   <si>
     <t>=INDEX(B2:C7,MATCH(C12,C2:C7,0),MATCH("Student name",B2:C2,0))</t>
+  </si>
+  <si>
+    <t>Aman</t>
+  </si>
+  <si>
+    <t>Bobby</t>
+  </si>
+  <si>
+    <t>Rahul</t>
+  </si>
+  <si>
+    <t>Sachin</t>
+  </si>
+  <si>
+    <t>Zhuxin</t>
   </si>
 </sst>
 </file>
@@ -314,11 +339,18 @@
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -553,114 +585,115 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="4" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -718,25 +751,25 @@
   </xdr:oneCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>115088</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>154363</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>172643</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>154723</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>531886</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>182194</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>201003</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>112023</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
-      <mc:Choice Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2">
           <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="15" name="Ink 14">
+            <xdr14:cNvPr id="11" name="Ink 10">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00445FBB-26E6-0FD9-E881-F73AB3A0DA75}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{88E65A19-DBDB-7F86-9464-E9218F7F1D0F}"/>
                 </a:ext>
               </a:extLst>
             </xdr14:cNvPr>
@@ -744,18 +777,18 @@
           </xdr14:nvContentPartPr>
           <xdr14:nvPr macro=""/>
           <xdr14:xfrm>
-            <a:off x="10310122" y="3097260"/>
-            <a:ext cx="416798" cy="211762"/>
+            <a:off x="12515729" y="3281551"/>
+            <a:ext cx="1289602" cy="325162"/>
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:pic>
           <xdr:nvPicPr>
-            <xdr:cNvPr id="15" name="Ink 14">
+            <xdr:cNvPr id="11" name="Ink 10">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00445FBB-26E6-0FD9-E881-F73AB3A0DA75}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{88E65A19-DBDB-7F86-9464-E9218F7F1D0F}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -769,8 +802,593 @@
           </xdr:blipFill>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="10304003" y="3091138"/>
-              <a:ext cx="429036" cy="224007"/>
+              <a:off x="12509610" y="3275340"/>
+              <a:ext cx="1301839" cy="337584"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>101547</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>60635</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>181107</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>171544</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="12" name="Ink 11">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B9BBB487-1956-2BE7-92F9-0EA6DC541EEE}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="13075254" y="4474980"/>
+            <a:ext cx="79560" cy="294840"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="12" name="Ink 11">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B9BBB487-1956-2BE7-92F9-0EA6DC541EEE}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="13069134" y="4468860"/>
+              <a:ext cx="91800" cy="307080"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>277587</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>85864</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>343827</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>135573</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="13" name="Ink 12">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{493E9B8A-8552-C1FE-A330-6401759111A7}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="13251294" y="4684140"/>
+            <a:ext cx="66240" cy="233640"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="13" name="Ink 12">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{493E9B8A-8552-C1FE-A330-6401759111A7}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="13245174" y="4678020"/>
+              <a:ext cx="78480" cy="245880"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>467307</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>86613</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>524629</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>125882</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="14" name="Ink 13">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A3BB58C-1182-2B8D-21B8-EF92ECD4E956}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="13441014" y="4868820"/>
+            <a:ext cx="52560" cy="223200"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="14" name="Ink 13">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A3BB58C-1182-2B8D-21B8-EF92ECD4E956}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="13434894" y="4862700"/>
+              <a:ext cx="64800" cy="235440"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>84726</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>17575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>581248</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>68282</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId10">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="20" name="Ink 19">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CC0058D3-CB1D-9462-41CD-28791673EA30}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="13689054" y="4799782"/>
+            <a:ext cx="496522" cy="234638"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="20" name="Ink 19">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CC0058D3-CB1D-9462-41CD-28791673EA30}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="13682933" y="4793664"/>
+              <a:ext cx="508764" cy="246874"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>122365</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>161592</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>135506</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>144423</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId12">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="30" name="Ink 29">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3CEB4BD6-AD96-F094-9726-57FC7AF84F3B}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="14987934" y="3288420"/>
+            <a:ext cx="643762" cy="166762"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="30" name="Ink 29">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3CEB4BD6-AD96-F094-9726-57FC7AF84F3B}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="14981817" y="3282120"/>
+              <a:ext cx="655997" cy="179362"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>201925</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>55090</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>392268</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>104881</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId14">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="38" name="Ink 37">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3CC7097A-5545-1D44-EA69-D5599357D6BE}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="15067494" y="3549780"/>
+            <a:ext cx="816202" cy="233722"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="38" name="Ink 37">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3CC7097A-5545-1D44-EA69-D5599357D6BE}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="15061373" y="3543533"/>
+              <a:ext cx="828443" cy="246217"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>123626</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>36428</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>48846</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>30419</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId16">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="49" name="Ink 48">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D5F55533-80A7-61F2-41D0-7775A269AD1F}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="15619816" y="3898980"/>
+            <a:ext cx="555840" cy="177922"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="49" name="Ink 48">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D5F55533-80A7-61F2-41D0-7775A269AD1F}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="15613696" y="3892679"/>
+              <a:ext cx="568080" cy="190525"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>181405</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>19230</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>572807</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>65617</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId18">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="50" name="Ink 49">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{832AD57E-D120-821E-AFC0-8BD486053AFA}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="15046974" y="3881782"/>
+            <a:ext cx="391402" cy="230318"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="50" name="Ink 49">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{832AD57E-D120-821E-AFC0-8BD486053AFA}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="15040779" y="3875674"/>
+              <a:ext cx="403793" cy="242535"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>46515</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>99730</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>133995</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>49777</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId20">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="51" name="Ink 50">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8919A8FC-F893-DE9B-9077-FD00554996B1}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="16173325" y="3594420"/>
+            <a:ext cx="87480" cy="501840"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="51" name="Ink 50">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8919A8FC-F893-DE9B-9077-FD00554996B1}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="16167205" y="3588300"/>
+              <a:ext cx="99720" cy="514080"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -784,24 +1402,24 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>208246</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>97541</xdr:rowOff>
+      <xdr:colOff>626214</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>26679</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>483728</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>36452</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>421295</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>27150</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
-      <mc:Choice Requires="xdr14">
-        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId22">
           <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="31" name="Ink 30">
+            <xdr14:cNvPr id="74" name="Ink 73">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6CFFA9A4-8048-2E5F-16B7-5796DD2BDFFD}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AEA6F868-B0D4-AFFA-B8D8-A93166E74796}"/>
                 </a:ext>
               </a:extLst>
             </xdr14:cNvPr>
@@ -809,358 +1427,33 @@
           </xdr14:nvContentPartPr>
           <xdr14:nvPr macro=""/>
           <xdr14:xfrm>
-            <a:off x="10403280" y="3408300"/>
-            <a:ext cx="275482" cy="122842"/>
+            <a:off x="17383645" y="3705300"/>
+            <a:ext cx="1051560" cy="184402"/>
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:pic>
           <xdr:nvPicPr>
-            <xdr:cNvPr id="31" name="Ink 30">
+            <xdr:cNvPr id="74" name="Ink 73">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6CFFA9A4-8048-2E5F-16B7-5796DD2BDFFD}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AEA6F868-B0D4-AFFA-B8D8-A93166E74796}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvPicPr/>
           </xdr:nvPicPr>
           <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId23"/>
             <a:stretch>
               <a:fillRect/>
             </a:stretch>
           </xdr:blipFill>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="10397166" y="3401933"/>
-              <a:ext cx="287710" cy="135576"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-        </xdr:pic>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>113727</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>11112</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>40126</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>65363</xdr:rowOff>
-    </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
-      <mc:Choice Requires="xdr14">
-        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6">
-          <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="46" name="Ink 45">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{99987E72-8A05-E937-947C-4BE692B37B47}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr14:cNvPr>
-            <xdr14:cNvContentPartPr/>
-          </xdr14:nvContentPartPr>
-          <xdr14:nvPr macro=""/>
-          <xdr14:xfrm>
-            <a:off x="9047520" y="3137940"/>
-            <a:ext cx="1187640" cy="601282"/>
-          </xdr14:xfrm>
-        </xdr:contentPart>
-      </mc:Choice>
-      <mc:Fallback xmlns="">
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="46" name="Ink 45">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{99987E72-8A05-E937-947C-4BE692B37B47}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvPicPr/>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="9041400" y="3131819"/>
-              <a:ext cx="1199880" cy="613524"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-        </xdr:pic>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>252526</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>130330</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>352606</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>57721</xdr:rowOff>
-    </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
-      <mc:Choice Requires="xdr14">
-        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8">
-          <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="47" name="Ink 46">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B02AA164-0A12-10AB-ED82-A81C177EB13B}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr14:cNvPr>
-            <xdr14:cNvContentPartPr/>
-          </xdr14:nvContentPartPr>
-          <xdr14:nvPr macro=""/>
-          <xdr14:xfrm>
-            <a:off x="10447560" y="3625020"/>
-            <a:ext cx="100080" cy="106560"/>
-          </xdr14:xfrm>
-        </xdr:contentPart>
-      </mc:Choice>
-      <mc:Fallback xmlns="">
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="47" name="Ink 46">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B02AA164-0A12-10AB-ED82-A81C177EB13B}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvPicPr/>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="10441440" y="3618900"/>
-              <a:ext cx="112320" cy="118800"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-        </xdr:pic>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>230747</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>170012</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>455027</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>68161</xdr:rowOff>
-    </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
-      <mc:Choice Requires="xdr14">
-        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId10">
-          <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="53" name="Ink 52">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{41F2FAAD-369D-8C87-42D9-27C7B431AA65}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr14:cNvPr>
-            <xdr14:cNvContentPartPr/>
-          </xdr14:nvContentPartPr>
-          <xdr14:nvPr macro=""/>
-          <xdr14:xfrm>
-            <a:off x="11056402" y="3664702"/>
-            <a:ext cx="224280" cy="82080"/>
-          </xdr14:xfrm>
-        </xdr:contentPart>
-      </mc:Choice>
-      <mc:Fallback xmlns="">
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="53" name="Ink 52">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{41F2FAAD-369D-8C87-42D9-27C7B431AA65}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvPicPr/>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="11050141" y="3658555"/>
-              <a:ext cx="236801" cy="94374"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-        </xdr:pic>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>487606</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>162010</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>74867</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>65559</xdr:rowOff>
-    </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
-      <mc:Choice Requires="xdr14">
-        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId12">
-          <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="54" name="Ink 53">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C72905D1-488F-1FEF-97FA-F710193DD2F7}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr14:cNvPr>
-            <xdr14:cNvContentPartPr/>
-          </xdr14:nvContentPartPr>
-          <xdr14:nvPr macro=""/>
-          <xdr14:xfrm>
-            <a:off x="10682640" y="3656700"/>
-            <a:ext cx="217882" cy="87480"/>
-          </xdr14:xfrm>
-        </xdr:contentPart>
-      </mc:Choice>
-      <mc:Fallback xmlns="">
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="54" name="Ink 53">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C72905D1-488F-1FEF-97FA-F710193DD2F7}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvPicPr/>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="10676518" y="3650580"/>
-              <a:ext cx="230127" cy="99720"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-        </xdr:pic>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>137686</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>54730</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>58046</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>103470</xdr:rowOff>
-    </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
-      <mc:Choice Requires="xdr14">
-        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId14">
-          <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="55" name="Ink 54">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1ABE107C-2012-2A40-B6AB-8394E6FA02A2}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr14:cNvPr>
-            <xdr14:cNvContentPartPr/>
-          </xdr14:nvContentPartPr>
-          <xdr14:nvPr macro=""/>
-          <xdr14:xfrm>
-            <a:off x="10332720" y="3549420"/>
-            <a:ext cx="1176840" cy="411840"/>
-          </xdr14:xfrm>
-        </xdr:contentPart>
-      </mc:Choice>
-      <mc:Fallback xmlns="">
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="55" name="Ink 54">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1ABE107C-2012-2A40-B6AB-8394E6FA02A2}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvPicPr/>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="10326600" y="3543300"/>
-              <a:ext cx="1189080" cy="424080"/>
+              <a:off x="17377525" y="3699018"/>
+              <a:ext cx="1063800" cy="196966"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -1174,24 +1467,24 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>247026</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>116046</xdr:rowOff>
+      <xdr:colOff>264397</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>19119</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>128048</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>180597</xdr:rowOff>
+      <xdr:colOff>397974</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>104108</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
-      <mc:Choice Requires="xdr14">
-        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId16">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId24">
           <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="61" name="Ink 60">
+            <xdr14:cNvPr id="77" name="Ink 76">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{06A0CF6F-CF1D-3EB4-3AEB-49EDC74B0811}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E452D0E-D936-2C2F-16B2-9C9A67E3D8CB}"/>
                 </a:ext>
               </a:extLst>
             </xdr14:cNvPr>
@@ -1199,33 +1492,33 @@
           </xdr14:nvContentPartPr>
           <xdr14:nvPr macro=""/>
           <xdr14:xfrm>
-            <a:off x="9811440" y="4346460"/>
-            <a:ext cx="511642" cy="248482"/>
+            <a:off x="16391207" y="3697740"/>
+            <a:ext cx="764198" cy="268920"/>
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:pic>
           <xdr:nvPicPr>
-            <xdr:cNvPr id="61" name="Ink 60">
+            <xdr:cNvPr id="77" name="Ink 76">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{06A0CF6F-CF1D-3EB4-3AEB-49EDC74B0811}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E452D0E-D936-2C2F-16B2-9C9A67E3D8CB}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvPicPr/>
           </xdr:nvPicPr>
           <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId25"/>
             <a:stretch>
               <a:fillRect/>
             </a:stretch>
           </xdr:blipFill>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="9805319" y="4340347"/>
-              <a:ext cx="523884" cy="260708"/>
+              <a:off x="16385088" y="3691620"/>
+              <a:ext cx="776437" cy="281160"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -1238,25 +1531,25 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>365206</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>95526</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>11955</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>142872</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>537646</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>36904</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>134715</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>30332</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
-      <mc:Choice Requires="xdr14">
-        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId18">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId26">
           <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="62" name="Ink 61">
+            <xdr14:cNvPr id="78" name="Ink 77">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1C7AB7BB-F31F-1AA5-1169-385D8EBBDAE7}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CAB3C2FF-03A8-DCDB-1688-7881250AFEDA}"/>
                 </a:ext>
               </a:extLst>
             </xdr14:cNvPr>
@@ -1264,33 +1557,163 @@
           </xdr14:nvContentPartPr>
           <xdr14:nvPr macro=""/>
           <xdr14:xfrm>
-            <a:off x="10560240" y="4325940"/>
-            <a:ext cx="172440" cy="309240"/>
+            <a:off x="16138765" y="3269700"/>
+            <a:ext cx="122760" cy="250560"/>
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:pic>
           <xdr:nvPicPr>
-            <xdr:cNvPr id="62" name="Ink 61">
+            <xdr:cNvPr id="78" name="Ink 77">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1C7AB7BB-F31F-1AA5-1169-385D8EBBDAE7}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CAB3C2FF-03A8-DCDB-1688-7881250AFEDA}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvPicPr/>
           </xdr:nvPicPr>
           <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19"/>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId27"/>
             <a:stretch>
               <a:fillRect/>
             </a:stretch>
           </xdr:blipFill>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="10554120" y="4319820"/>
-              <a:ext cx="184680" cy="321480"/>
+              <a:off x="16132645" y="3263580"/>
+              <a:ext cx="135000" cy="262800"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>312637</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>164194</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>364216</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>19254</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId28">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="89" name="Ink 88">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0E392E2D-CBE1-2026-ED3C-E81D2E87FD05}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="16439447" y="3291022"/>
+            <a:ext cx="682200" cy="218160"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="89" name="Ink 88">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0E392E2D-CBE1-2026-ED3C-E81D2E87FD05}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId29"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="16433324" y="3284902"/>
+              <a:ext cx="694446" cy="230400"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>289237</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>8609</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>315599</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>179166</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId30">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="90" name="Ink 89">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{35F7170B-B4AF-2C30-706E-7A458EA48CB4}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="13262944" y="5526540"/>
+            <a:ext cx="21600" cy="175320"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="90" name="Ink 89">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{35F7170B-B4AF-2C30-706E-7A458EA48CB4}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId31"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="13256824" y="5520420"/>
+              <a:ext cx="33840" cy="187560"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -1304,24 +1727,24 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>67431</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>56583</xdr:rowOff>
+      <xdr:colOff>149656</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>48929</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>243831</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>127090</xdr:rowOff>
+      <xdr:colOff>321736</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>19160</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
-      <mc:Choice Requires="xdr14">
-        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId20">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId32">
           <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="68" name="Ink 67">
+            <xdr14:cNvPr id="91" name="Ink 90">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{76DB95CD-FB1F-99D5-C96F-A7B92E7E6170}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C00506A-4A36-0C82-2688-7FF9BDD827FA}"/>
                 </a:ext>
               </a:extLst>
             </xdr14:cNvPr>
@@ -1329,33 +1752,33 @@
           </xdr14:nvContentPartPr>
           <xdr14:nvPr macro=""/>
           <xdr14:xfrm>
-            <a:off x="7109362" y="3367342"/>
-            <a:ext cx="176400" cy="254438"/>
+            <a:off x="13753984" y="5566860"/>
+            <a:ext cx="172080" cy="149400"/>
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:pic>
           <xdr:nvPicPr>
-            <xdr:cNvPr id="68" name="Ink 67">
+            <xdr:cNvPr id="91" name="Ink 90">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{76DB95CD-FB1F-99D5-C96F-A7B92E7E6170}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C00506A-4A36-0C82-2688-7FF9BDD827FA}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvPicPr/>
           </xdr:nvPicPr>
           <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21"/>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId33"/>
             <a:stretch>
               <a:fillRect/>
             </a:stretch>
           </xdr:blipFill>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="7103242" y="3361224"/>
-              <a:ext cx="188640" cy="266674"/>
+              <a:off x="13747864" y="5560740"/>
+              <a:ext cx="184320" cy="161640"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -1368,25 +1791,25 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>285951</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>66332</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>191516</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>75958</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>441471</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>143401</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>316518</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>132589</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
-      <mc:Choice Requires="xdr14">
-        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId22">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId34">
           <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="72" name="Ink 71">
+            <xdr14:cNvPr id="94" name="Ink 93">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D3033A2E-4379-25F6-D1A7-9179A59C4957}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C7EDF0D0-5518-A161-7A86-A8725317B17A}"/>
                 </a:ext>
               </a:extLst>
             </xdr14:cNvPr>
@@ -1394,33 +1817,228 @@
           </xdr14:nvContentPartPr>
           <xdr14:nvPr macro=""/>
           <xdr14:xfrm>
-            <a:off x="7327882" y="3561022"/>
-            <a:ext cx="155520" cy="261000"/>
+            <a:off x="14426464" y="5777820"/>
+            <a:ext cx="120240" cy="235800"/>
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:pic>
           <xdr:nvPicPr>
-            <xdr:cNvPr id="72" name="Ink 71">
+            <xdr:cNvPr id="94" name="Ink 93">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D3033A2E-4379-25F6-D1A7-9179A59C4957}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C7EDF0D0-5518-A161-7A86-A8725317B17A}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvPicPr/>
           </xdr:nvPicPr>
           <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId23"/>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId35"/>
             <a:stretch>
               <a:fillRect/>
             </a:stretch>
           </xdr:blipFill>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="7321762" y="3554902"/>
-              <a:ext cx="167760" cy="273240"/>
+              <a:off x="14420344" y="5771700"/>
+              <a:ext cx="132480" cy="248040"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>329036</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>72027</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>427038</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>178698</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId36">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="95" name="Ink 94">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F4226905-E9BB-74CF-A2AD-C395B2DF0B4D}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="14563984" y="5957820"/>
+            <a:ext cx="93240" cy="285840"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="95" name="Ink 94">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F4226905-E9BB-74CF-A2AD-C395B2DF0B4D}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId37"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="14557864" y="5951700"/>
+              <a:ext cx="105480" cy="298080"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>458276</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>51896</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>545118</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>181607</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId38">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="96" name="Ink 95">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9BC518C1-4E07-ED42-10B8-C85083146B9C}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="14693224" y="6121620"/>
+            <a:ext cx="82080" cy="308880"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="96" name="Ink 95">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9BC518C1-4E07-ED42-10B8-C85083146B9C}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId39"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="14687104" y="6115500"/>
+              <a:ext cx="94320" cy="321120"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>163617</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>21018</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>503457</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>93407</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId40">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="100" name="Ink 99">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B5CF8111-329E-C632-C0C2-1066437BB166}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="15029186" y="6090742"/>
+            <a:ext cx="339840" cy="256320"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="100" name="Ink 99">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B5CF8111-329E-C632-C0C2-1066437BB166}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId41"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="15023060" y="6084622"/>
+              <a:ext cx="352093" cy="268560"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -1434,24 +2052,68 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>214130</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>6130</xdr:rowOff>
+      <xdr:colOff>124810</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>124810</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>50429</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>14079</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>466871</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>171342</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
-      <mc:Choice Requires="xdr14">
-        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId24">
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="101" name="Picture 100">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F5C9482B-B54E-96CF-8206-97556F0E6848}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId42"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13098517" y="6746327"/>
+          <a:ext cx="2233923" cy="414394"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>242114</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>151140</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>516074</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>105531</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId43">
           <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="75" name="Ink 74">
+            <xdr14:cNvPr id="102" name="Ink 101">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9D92B215-0EBF-413F-AE9A-7C7CB001E97E}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CAD8BBCE-4052-D4F7-E3E8-C65AED59E341}"/>
                 </a:ext>
               </a:extLst>
             </xdr14:cNvPr>
@@ -1459,98 +2121,33 @@
           </xdr14:nvContentPartPr>
           <xdr14:nvPr macro=""/>
           <xdr14:xfrm>
-            <a:off x="6625440" y="3500820"/>
-            <a:ext cx="466920" cy="191880"/>
+            <a:off x="15738304" y="5485140"/>
+            <a:ext cx="273960" cy="133560"/>
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:pic>
           <xdr:nvPicPr>
-            <xdr:cNvPr id="75" name="Ink 74">
+            <xdr:cNvPr id="102" name="Ink 101">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9D92B215-0EBF-413F-AE9A-7C7CB001E97E}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CAD8BBCE-4052-D4F7-E3E8-C65AED59E341}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvPicPr/>
           </xdr:nvPicPr>
           <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId25"/>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId44"/>
             <a:stretch>
               <a:fillRect/>
             </a:stretch>
           </xdr:blipFill>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="6619320" y="3494700"/>
-              <a:ext cx="479160" cy="204120"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-        </xdr:pic>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>506631</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>105130</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>91290</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>149799</xdr:rowOff>
-    </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
-      <mc:Choice Requires="xdr14">
-        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId26">
-          <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="76" name="Ink 75">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{70A9DFBC-4CC5-A251-2F8E-BE34190CA6F2}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr14:cNvPr>
-            <xdr14:cNvContentPartPr/>
-          </xdr14:nvContentPartPr>
-          <xdr14:nvPr macro=""/>
-          <xdr14:xfrm>
-            <a:off x="7548562" y="3599820"/>
-            <a:ext cx="215280" cy="228600"/>
-          </xdr14:xfrm>
-        </xdr:contentPart>
-      </mc:Choice>
-      <mc:Fallback xmlns="">
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="76" name="Ink 75">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{70A9DFBC-4CC5-A251-2F8E-BE34190CA6F2}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvPicPr/>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId27"/>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="7542452" y="3593700"/>
-              <a:ext cx="227500" cy="240840"/>
+              <a:off x="15732184" y="5479020"/>
+              <a:ext cx="286200" cy="145800"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -1564,24 +2161,24 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>45310</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>67023</xdr:rowOff>
+      <xdr:colOff>430295</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>162382</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>209830</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>113770</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>87314</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>122120</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
-      <mc:Choice Requires="xdr14">
-        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId28">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId45">
           <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="82" name="Ink 81">
+            <xdr14:cNvPr id="106" name="Ink 105">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AE9E1C54-6335-A16E-7BA1-778A6EB04485}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A3005345-99DA-F36D-5C7B-449014A0C639}"/>
                 </a:ext>
               </a:extLst>
             </xdr14:cNvPr>
@@ -1589,228 +2186,33 @@
           </xdr14:nvContentPartPr>
           <xdr14:nvPr macro=""/>
           <xdr14:xfrm>
-            <a:off x="8348482" y="3377782"/>
-            <a:ext cx="164520" cy="230678"/>
+            <a:off x="15295864" y="5496382"/>
+            <a:ext cx="287640" cy="327600"/>
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:pic>
           <xdr:nvPicPr>
-            <xdr:cNvPr id="82" name="Ink 81">
+            <xdr:cNvPr id="106" name="Ink 105">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AE9E1C54-6335-A16E-7BA1-778A6EB04485}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A3005345-99DA-F36D-5C7B-449014A0C639}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvPicPr/>
           </xdr:nvPicPr>
           <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId29"/>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId46"/>
             <a:stretch>
               <a:fillRect/>
             </a:stretch>
           </xdr:blipFill>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="8342362" y="3371664"/>
-              <a:ext cx="176760" cy="242914"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-        </xdr:pic>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>236028</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>77410</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>373188</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>144481</xdr:rowOff>
-    </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
-      <mc:Choice Requires="xdr14">
-        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId30">
-          <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="87" name="Ink 86">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{526F19A3-B47B-8B5B-5F7E-2278904D2D22}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr14:cNvPr>
-            <xdr14:cNvContentPartPr/>
-          </xdr14:nvContentPartPr>
-          <xdr14:nvPr macro=""/>
-          <xdr14:xfrm>
-            <a:off x="8539200" y="3572100"/>
-            <a:ext cx="137160" cy="251002"/>
-          </xdr14:xfrm>
-        </xdr:contentPart>
-      </mc:Choice>
-      <mc:Fallback xmlns="">
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="87" name="Ink 86">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{526F19A3-B47B-8B5B-5F7E-2278904D2D22}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvPicPr/>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId31"/>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="8533096" y="3565862"/>
-              <a:ext cx="149368" cy="263479"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-        </xdr:pic>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>276690</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>39332</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>61788</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>17401</xdr:rowOff>
-    </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
-      <mc:Choice Requires="xdr14">
-        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId32">
-          <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="92" name="Ink 91">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7EBBDE61-FD4D-0145-DBA4-1EB301E1751A}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr14:cNvPr>
-            <xdr14:cNvContentPartPr/>
-          </xdr14:nvContentPartPr>
-          <xdr14:nvPr macro=""/>
-          <xdr14:xfrm>
-            <a:off x="7949242" y="3534022"/>
-            <a:ext cx="415718" cy="162000"/>
-          </xdr14:xfrm>
-        </xdr:contentPart>
-      </mc:Choice>
-      <mc:Fallback xmlns="">
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="92" name="Ink 91">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7EBBDE61-FD4D-0145-DBA4-1EB301E1751A}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvPicPr/>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId33"/>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="7943123" y="3527902"/>
-              <a:ext cx="427956" cy="174240"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-        </xdr:pic>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>449590</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>114212</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>595030</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>150241</xdr:rowOff>
-    </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
-      <mc:Choice Requires="xdr14">
-        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId34">
-          <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="93" name="Ink 92">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6D7C51EE-9D46-7945-9C66-2E0A66570ADE}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr14:cNvPr>
-            <xdr14:cNvContentPartPr/>
-          </xdr14:nvContentPartPr>
-          <xdr14:nvPr macro=""/>
-          <xdr14:xfrm>
-            <a:off x="8752762" y="3608902"/>
-            <a:ext cx="145440" cy="219960"/>
-          </xdr14:xfrm>
-        </xdr:contentPart>
-      </mc:Choice>
-      <mc:Fallback xmlns="">
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="93" name="Ink 92">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6D7C51EE-9D46-7945-9C66-2E0A66570ADE}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvPicPr/>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId35"/>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="8746642" y="3602638"/>
-              <a:ext cx="157680" cy="232487"/>
+              <a:off x="15289752" y="5490262"/>
+              <a:ext cx="299865" cy="339840"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -2152,7 +2554,7 @@
           <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
         </inkml:channelProperties>
       </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2025-01-04T15:29:40.095"/>
+      <inkml:timestamp xml:id="ts0" timeString="2025-02-22T15:34:54.405"/>
     </inkml:context>
     <inkml:brush xml:id="br0">
       <inkml:brushProperty name="width" value="0.035" units="cm"/>
@@ -2160,9 +2562,13 @@
       <inkml:brushProperty name="color" value="#004F8B"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">36 228 656,'0'0'17600,"-3"2"-17378,1 1-217,0 0 0,0 0 1,0 1-1,1-1 1,-1 0-1,1 0 0,0 1 1,0-1-1,0 1 0,1-1 1,-1 1-1,1-1 0,0 7 1,1 60 219,0-36-56,-1 166 333,0-200-387,0-3 74,-15-91-26,14 78-195,-1-22-245,1 1 0,7-59 0,-5 86 212,0 0 1,1 0-1,1 0 0,0 0 1,0 1-1,1-1 0,0 1 1,0 0-1,1 0 0,1 1 1,-1-1-1,1 1 0,1 0 1,12-11-1,-16 16 45,1 0 0,0 1 1,0 0-1,0 0 0,1 0 0,-1 0 1,0 0-1,1 1 0,-1 0 1,1 0-1,-1 0 0,1 1 0,-1-1 1,10 2-1,-13-1 15,0 1 1,-1 0 0,1-1-1,0 1 1,-1 0 0,1 0-1,0 0 1,-1 0-1,1-1 1,-1 1 0,1 0-1,-1 0 1,0 0-1,0 0 1,1 0 0,-1 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0-1,0 0 1,0 0 0,0 0-1,-1 2 1,-3 31 6,0-27-12,0-1 1,-1 1 0,0-1-1,0 1 1,0-1-1,-1-1 1,0 1 0,0-1-1,-8 6 1,1-2-367,0 0 1,-1-1 0,-27 12-1,41-20 386,-1 0 0,1 1 0,-1-1 0,1 0 0,-1 1 0,1-1-1,0 0 1,-1 1 0,1-1 0,0 1 0,0-1 0,-1 0 0,1 1 0,0-1-1,0 1 1,-1-1 0,1 1 0,0-1 0,0 1 0,0-1 0,0 1 0,0-1-1,0 1 1,0-1 0,0 1 0,0-1 0,0 1 0,0-1 0,0 1-1,0 0 1,0-1 0,1 0 0,-1 1 0,0-1 0,0 1 0,0-1 0,1 1-1,-1-1 1,0 1 0,1-1 0,-1 0 0,0 1 0,1-1 0,-1 1-1,1-1 1,-1 0 0,0 0 0,1 1 0,-1-1 0,1 0 0,0 1 0,24 18-11,-25-19 3,34 23 290,54 26 1,-21-23-1472,-55-23-177,1 0-1,-1-1 0,19 2 0,1-4-4078</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="710.83">399 381 1713,'0'0'15113,"-9"-10"-13968,-29-28-612,38 38-521,-1-1-1,0 1 1,0-1-1,1 1 0,-1 0 1,0-1-1,0 1 0,0 0 1,1 0-1,-1 0 0,0-1 1,0 1-1,0 0 0,0 0 1,0 0-1,0 0 0,1 0 1,-1 1-1,0-1 0,0 0 1,0 0-1,0 1 1,0-1-1,1 0 0,-1 1 1,0-1-1,0 1 0,1-1 1,-1 1-1,0-1 0,1 1 1,-1-1-1,0 1 0,1 0 1,-1-1-1,1 1 0,-1 0 1,1 0-1,0-1 1,-1 1-1,1 0 0,0 0 1,-1 0-1,1 0 0,0 1 1,-3 2 20,-1 1-64,1 0 0,-1 0-1,1 1 1,0 0-1,1-1 1,-1 1-1,1 0 1,0 0 0,0 1-1,1-1 1,0 0-1,-1 13 1,3-19-13,-1 1 1,1 0 0,-1-1-1,1 1 1,-1-1-1,1 1 1,0-1 0,-1 1-1,1-1 1,0 1-1,0-1 1,-1 1-1,1-1 1,0 0 0,0 0-1,-1 1 1,1-1-1,0 0 1,0 0 0,0 0-1,-1 0 1,1 0-1,0 0 1,0 0-1,0 0 1,0 0 0,-1 0-1,1-1 1,1 1-1,30-6-351,-24 2 344,0-1 0,0 0 0,0 0 0,-1 0 0,1-1 0,-1 0-1,-1 0 1,1-1 0,10-14 0,-6 8 661,-10 12 258,0 1-861,0 1 1,0-1-1,1 0 0,-1 0 0,0 1 0,0-1 0,0 1 1,0-1-1,0 1 0,0 0 0,1-1 0,-1 1 1,0 0-1,-1-1 0,1 1 0,0 0 0,0 0 1,0 0-1,0 0 0,-1 0 0,1 0 0,-1 0 0,2 2 1,2 3 18,0-1-22,1-1 1,-1 0 0,1 0 0,-1-1 0,1 1 0,0-1-1,0 0 1,1 0 0,-1-1 0,1 0 0,-1 0 0,1 0-1,0 0 1,-1-1 0,1 0 0,0 0 0,0-1 0,0 0-1,0 0 1,0 0 0,0 0 0,0-1 0,0 0 0,-1-1-1,9-2 1,-7 1-12,0 0-1,0 0 1,0-1-1,-1 0 0,0 0 1,0-1-1,0 1 1,0-1-1,-1-1 0,0 1 1,0-1-1,0 0 1,-1 0-1,0 0 0,0-1 1,0 1-1,-1-1 1,0 0-1,3-10 1,-2-5 167,0-1 1,-2 0-1,-1 0 1,0 0 0,-4-26-1,1-7 108,2 39-61,0 0-1,-6-32 0,6 49-198,0 0 0,0 1 0,0-1 0,-1 0 0,1 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0 0 0,-1 1 0,1-1 0,0 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 1 0,0-1 0,0 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,0-1 0,0 1 0,-1 0 0,1 0 0,0 0 0,0 0 0,0 0 0,0-1 0,-1 1 0,1 0 0,0 0 0,0 0 0,0 0 0,0-1 0,0 1-1,-1 0 1,1 0 0,0-1 0,0 1 0,0 0 0,0 0 0,0 0 0,0-1 0,0 1 0,0 0 0,0-1 0,-6 39-42,1-1-1,1 1 0,3 0 0,4 54 1,-2-84 14,0 0 0,0 0 1,1 0-1,1 0 1,-1 0-1,1-1 0,1 1 1,-1-1-1,1 0 1,1 0-1,-1 0 0,1 0 1,0-1-1,1 0 1,-1 0-1,1 0 0,0-1 1,1 0-1,-1 0 1,1 0-1,0-1 0,1 0 1,-1 0-1,0-1 1,1 0-1,0 0 1,0-1-1,0 0 0,0-1 1,0 1-1,16-1 1,-11 0-28,0-1 0,-1-1 0,1 0 0,0 0 0,0-1 0,-1-1 0,0 0 0,1-1 0,13-7 0,-21 9 67,0-1 0,-1 0 1,1 0-1,-1 0 0,0-1 0,0 1 0,0-1 0,0 0 0,-1 0 0,0-1 0,0 1 0,0-1 0,0 1 0,0-1 0,-1 0 0,0 0 0,0 0 0,-1 0 1,1-1-1,-1 1 0,0 0 0,-1-1 0,1 1 0,-1-11 0,0 13 1,0 0 0,0 1 1,0-1-1,0 0 0,-1 0 0,1 0 0,-1 0 1,1 1-1,-1-1 0,0 0 0,0 1 0,-1-1 1,1 1-1,0-1 0,-1 1 0,0-1 0,1 1 1,-1 0-1,0 0 0,0 0 0,0 0 0,0 0 1,-1 0-1,1 1 0,0-1 0,-1 1 0,1-1 1,-1 1-1,0 0 0,1 0 0,-1 0 0,0 0 1,0 1-1,0-1 0,1 1 0,-1 0 0,0 0 1,0 0-1,0 0 0,0 0 0,1 0 0,-1 1 1,0-1-1,0 1 0,0 0 0,1 0 0,-1 0 1,-2 2-1,1-1-25,0 0-1,0 0 1,0 1 0,1 0 0,-1 0 0,1 0-1,-1 0 1,1 0 0,0 1 0,0-1 0,1 1-1,-1 0 1,1 0 0,0 0 0,0 0 0,0 0 0,0 0-1,1 1 1,0-1 0,0 0 0,-1 10 0,-1 4-11,1 0 0,1 0 1,0 0-1,3 22 1,-1-37-29,0 0 1,0 0 0,0 0-1,0 0 1,0 0 0,0 0-1,1 0 1,0-1 0,-1 1 0,1 0-1,0-1 1,0 0 0,0 1-1,1-1 1,-1 0 0,1 0-1,-1 0 1,1-1 0,-1 1-1,1-1 1,0 1 0,0-1 0,0 0-1,0 0 1,0 0 0,0 0-1,0-1 1,0 1 0,6-1-1,7 2-1191,0-1-1,-1 0 0,1-2 0,27-3 1,-14-5-3949,-10-11-2345</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="913.33">657 153 2897,'0'0'13511,"118"-15"-13768,-26-6-2608,5-7-3362</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1759 202 3522,'0'0'6811,"0"-10"-1652,0 358-4441,-1-345-699,1-3-97,0 1-1,-1-1 1,1 0 0,0 0 0,0 0-1,-1 0 1,1 0 0,0 0 0,0 1-1,-1-1 1,1 0 0,0 0 0,0 0 0,0 1-1,0-1 1,-1 0 0,1 0 0,0 0-1,0 1 1,0-1 0,0 0 0,0 0-1,0 1 1,-1-1 0,1 0 0,0 1 0,0-1-1,0 0 1,0 0 0,0 1 0,0-1-1,0 0 1,0 0 0,0 1 0,0-1-1,0 0 1,1 1 0,-1-1 0,0 0-1,0 0 1,0 1 0,0-1 0,0 0 0,0 0-1,1 1 1,-1-1 0,0 0 0,0 0-1,0 0 1,1 1 0,-1-1 0,0 0-1,1 0 1,11 0-5391,-11 0 5430,15-2-6457</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="521.4">2031 172 4018,'0'0'7208,"0"-4"-6594,0 4-589,0-1 0,1 1-1,-1 0 1,0-1 0,0 1 0,0-1-1,0 1 1,0 0 0,0-1 0,0 1-1,0-1 1,0 1 0,0 0-1,0-1 1,0 1 0,0-1 0,0 1-1,0 0 1,0-1 0,-1 1 0,1-1-1,0 1 1,0 0 0,0-1 0,-1 1-1,1 0 1,0-1 0,0 1 0,-1 0-1,1 0 1,0-1 0,-1 1 0,1 0-1,0 0 1,-1-1 0,1 1 0,0 0-1,-1 0 1,1 0 0,0 0 0,-1 0-1,1-1 1,-1 1 0,1 0 0,0 0-1,-1 0 1,-19 17 591,-17 37 129,27-35-615,1-1-1,1 1 1,1 1 0,1-1-1,1 1 1,0 1 0,2-1-1,0 0 1,0 36 0,3-54-129,1 0 0,-1 0 0,0 0 0,1 0 0,-1 0 0,1-1 0,0 1 0,-1 0 0,1 0 0,0-1 0,0 1 0,0 0 0,0-1 0,1 1 0,-1-1 0,0 1 0,0-1 0,1 0 0,-1 0 0,1 1 0,0-1 0,-1 0 0,1 0 0,0-1 1,-1 1-1,1 0 0,0-1 0,0 1 0,0 0 0,-1-1 0,4 0 0,8 3-65,0-2 0,0 0 1,21-1-1,-19-1-93,-13 1 160,-1-1 0,1 0 0,-1 1 0,1-1 0,-1 0 0,0 0 1,0 0-1,1 0 0,-1 0 0,0-1 0,0 1 0,0 0 0,0-1 1,0 1-1,0 0 0,-1-1 0,1 1 0,0-1 0,-1 1 0,1-1 0,-1 1 1,0-1-1,1 1 0,-1-1 0,0 0 0,0 1 0,0-1 0,0 0 1,-1-2-1,2 1 9,-1-1 1,0 1 0,0 0-1,0 0 1,0 0-1,-1-1 1,0 1 0,1 0-1,-1 0 1,0 0 0,0 0-1,-1 0 1,1 0 0,0 0-1,-4-3 1,1 3-114,0 0 1,-1 1-1,1-1 1,-1 1-1,1 0 1,-1 1-1,0-1 1,0 1-1,0 0 1,0 0-1,0 1 1,0-1-1,0 1 1,0 0-1,0 0 1,0 1-1,-9 1 1,15 18-6567,8-16 2927</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="959.61">2248 321 2689,'0'0'9522,"-4"0"-9191,2 0-318,1 0 1,-1 0 0,0 0-1,1 0 1,-1 0 0,0 0-1,1 0 1,-1 1 0,0-1-1,1 1 1,-1-1 0,1 1-1,-1 0 1,1-1 0,-1 1-1,1 0 1,0 0-1,-1 0 1,1 0 0,0 0-1,0 0 1,0 1 0,0-1-1,0 0 1,0 1 0,0-1-1,0 1 1,0-1 0,0 1-1,1-1 1,-1 1 0,1-1-1,-1 1 1,1 1 0,-3 9 102,2-1 0,-1 0 0,2 1 0,0 12 0,0-19-67,1-4-43,-1 0-1,1 0 1,0 0-1,0-1 1,0 1 0,0 0-1,1-1 1,-1 1 0,0-1-1,0 0 1,0 1 0,0-1-1,0 0 1,1 0-1,-1 1 1,0-1 0,0 0-1,1 0 1,-1 0 0,0-1-1,2 1 1,31-2 22,-30 0-8,-1-1 0,1 1 0,0-1 0,-1 1 0,1-1 0,-1 0-1,0 0 1,0-1 0,0 1 0,0-1 0,-1 1 0,1-1 0,-1 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,-1 0 0,0 0 0,0-1-1,0 1 1,0-1 0,-1 1 0,0 0 0,0-1 0,0 1 0,0-1 0,-1 1 0,0 0 0,0-1 0,-1-3 0,1 6-12,0 1 1,0 0 0,0 0-1,0-1 1,0 1 0,0 0 0,-1 0-1,1 0 1,0 0 0,-1 0-1,1 1 1,0-1 0,-1 0-1,1 1 1,-1-1 0,1 1 0,-1-1-1,0 1 1,1 0 0,-1-1-1,1 1 1,-1 0 0,0 0-1,1 0 1,-1 1 0,1-1 0,-1 0-1,1 0 1,-1 1 0,-2 1-1,0-2-138,1 1-1,0 0 0,0 1 0,1-1 1,-1 0-1,0 1 0,0 0 0,1 0 1,-1-1-1,1 2 0,-1-1 0,1 0 1,0 0-1,-3 5 0,-1 9-2131,6-15 1970,-1-1 0,1 1 0,0 0 0,0 0 0,0-1 0,0 1-1,0 0 1,0 0 0,0 0 0,0-1 0,0 1 0,0 0 0,0 0 0,1-1 0,-1 1 0,0 0 0,1 0 0,-1-1-1,0 1 1,1 1 0,13 4-3211</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1313.16">2408 315 5394,'0'0'6956,"0"22"-6308,-1-10-476,5 19 184,-4-30-345,1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0-1-1,0 1 1,1-1 0,-1 1 0,0 0 0,0-1 0,1 0 0,-1 1 0,0-1-1,0 0 1,1 0 0,-1 1 0,0-1 0,1 0 0,-1 0 0,3-1 0,-2 1 34,-1 1-1,1-1 1,0 0 0,0 0 0,0 0 0,0 0 0,0-1 0,0 1-1,0 0 1,-1-1 0,1 1 0,0-1 0,0 0 0,-1 0 0,1 1 0,0-1-1,-1 0 1,1-1 0,-1 1 0,1 0 0,2-3 0,-3 0 85,1 0 0,-1 0 0,0 0 1,-1 0-1,1 0 0,0 0 0,-1 0 0,0-1 1,-1-5-1,1 9-129,0 0 0,0-1 0,0 1 0,0 0 1,0 0-1,0-1 0,-1 1 0,1 0 0,0 0 1,-1 0-1,1 0 0,-1-1 0,1 1 0,-1 0 1,0 0-1,0 0 0,1 0 0,-1 0 0,0 0 1,0 1-1,0-1 0,0 0 0,0 0 0,0 0 0,0 1 1,0-1-1,0 1 0,0-1 0,0 1 0,-1-1 1,1 1-1,0 0 0,0-1 0,0 1 0,-1 0 1,1 0-1,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 1,0 1-1,-3-1 0,1 1-129,-1 0 0,0 0 1,1 0-1,-1 0 0,0 1 0,1-1 0,0 1 1,-1 0-1,1 0 0,0 0 0,0 1 0,0-1 0,0 1 1,-2 3-1,-11 26-5664,15-21-707</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="17662.17">2805 343 2113,'0'0'7449,"0"-8"-6814,0 7-1250,1-33 3533,-3 26-228,-1 26-1977,-1 33-661,5 96-1,1-54-15,-2 173 479,-1-273-527,-1 1 1,0-1 0,-1 0-1,0 0 1,0 1-1,0 0 1,0 0-1,-1 0 1,0 0 0,-9-10-1,-4-7-11,-21-41 41,38 64-23,0 0 1,0 0-1,0 0 0,0 1 0,0-1 1,0 0-1,-1 0 0,1 0 0,0 0 1,0 0-1,0 0 0,0 0 0,0 0 1,0 0-1,-1 1 0,1-1 0,0 0 1,0 0-1,0 0 0,0 0 0,0 0 1,-1 0-1,1 0 0,0 0 0,0 0 0,0 0 1,0 0-1,-1 0 0,1 0 0,0 0 1,0 0-1,0 0 0,0 0 0,0 0 1,-1-1-1,1 1 0,0 0 0,0 0 1,0 0-1,0 0 0,0 0 0,0 0 1,0 0-1,-1 0 0,1-1 0,0 1 1,0 0-1,0 0 0,0 0 0,0 0 1,0 0-1,0 0 0,0-1 0,0 1 1,0 0-1,0 0 0,0 0 0,0 0 0,0 0 1,0-1-1,0 1 0,0 0 0,0 0 1,0 0-1,0 0 0,0-1 0,0 1 1,0 0-1,0 0 0,0 18-79,12 28 101,-5-30-17,0 0-1,2-1 1,0 0-1,1-1 1,0 0 0,17 18-1,-26-31 6,0 0-1,0-1 1,0 1-1,-1-1 0,1 1 1,0-1-1,0 1 1,0-1-1,0 0 1,0 1-1,0-1 0,0 0 1,0 0-1,0 0 1,0 1-1,0-1 1,0 0-1,0 0 0,0-1 1,0 1-1,0 0 1,0 0-1,0 0 1,0-1-1,1 0 0,24-20 260,14-43 219,-36 57-462,62-106-367,-57 105-801,-2 9-5406</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="28418.5">3550 859 3666,'0'0'9156,"-5"-9"-8417,-6-15-96,1-1 0,1 0 1,1-1-1,1 0 0,-5-34 0,5 2-716,1-91 1,8 70-60,0 37-1,-6-80 0,1 122 100,1 0-1,0 1 1,0-1 0,0 1-1,0 0 1,0-1 0,0 1-1,0 0 1,0 0 0,1 0-1,-4 3 1,-34 32-352,-39 50 1,61-66 243,14-17 63,-16 25-791,19-28 415,4-1-714,7-3 1170,0 0-1,0-1 1,0-1 0,-1 0 0,0 0-1,0-1 1,-1 0 0,1 0 0,11-15-1,-5 8 46,1-1 0,35-22-1,-51 37-53,0 0-1,-1 0 1,1 0 0,0-1-1,0 1 1,-1 0-1,1 0 1,0 0-1,0 0 1,-1 0-1,1 0 1,0 0-1,0 1 1,-1-1 0,1 0-1,0 0 1,0 1-1,-1-1 1,1 0-1,0 1 1,-1-1-1,1 0 1,-1 1 0,1-1-1,0 1 1,-1-1-1,1 1 1,-1 0-1,1-1 1,-1 1-1,1-1 1,-1 1-1,0 0 1,1-1 0,-1 1-1,0 0 1,0 0-1,1 0 1,12 35 56,-10-28-64,21 44-897,-3-8-5000,-19-31 1598</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="30093.83">773 23 3394,'0'0'3887,"-9"-1"-3124,-30-5-207,13 1-95,0 1 0,-27-1 0,23 4-455,0 1-1,0 1 1,0 2 0,1 1-1,-1 2 1,1 0-1,0 2 1,0 1 0,-47 23-1,43-12 0,0 1 0,2 2 0,0 1 0,2 1 0,-27 30 0,49-48 13,1 0 0,0 1 0,1 0 1,0 0-1,0 0 0,0 0 0,1 1 0,1 0 1,-1 0-1,2 0 0,-4 14 0,3-6 30,1 0-1,1 0 0,1-1 0,0 1 0,4 26 0,-3-39-14,0 1 0,1 0 0,0-1 0,0 1 0,1-1 0,-1 1 0,1-1 0,0 0 0,0 0 0,0 0 0,1-1 0,0 1 0,-1-1 0,1 0 0,0 0 0,0 0 0,1 0 1,-1-1-1,5 2 0,12 7 60,0-2 1,37 11 0,-4-6 13,-1-2-1,79 6 1,113-3 176,-163-12-223,0-3-1,1-3 1,-2-4 0,143-32 0,-89 15-58,-104 20 6,1-1 0,-1-1 0,0-2 0,50-19 0,-78 25 10,-1 0 0,1-1 0,-1 1-1,0-1 1,0 0 0,0 0-1,0 0 1,0 0 0,0 0 0,-1 0-1,1 0 1,-1-1 0,0 1-1,0 0 1,-1-1 0,1 1 0,-1-1-1,1 1 1,-1-1 0,0 1-1,0-1 1,-1-4 0,1-1-5,-1 0 0,0 0-1,0 0 1,-1 1 0,0-1 0,0 0 0,-1 1-1,-5-12 1,-5-2 8,0 1 1,-2 0-1,0 1 0,-1 0 0,-1 1 1,-1 1-1,-1 1 0,0 1 0,-1 0 0,-1 1 1,0 2-1,-1 0 0,0 1 0,-1 1 1,-1 2-1,0 0 0,0 1 0,0 1 0,-1 2 1,0 0-1,-49-2 0,7 7-12,0 2-1,1 4 1,-83 16 0,91-7 208,8-3-936,17-5-4038,23-6-488</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -2182,7 +2588,7 @@
           <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
         </inkml:channelProperties>
       </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2025-01-04T15:33:08.598"/>
+      <inkml:timestamp xml:id="ts0" timeString="2025-02-22T15:38:14.533"/>
     </inkml:context>
     <inkml:brush xml:id="br0">
       <inkml:brushProperty name="width" value="0.035" units="cm"/>
@@ -2190,11 +2596,7 @@
       <inkml:brushProperty name="color" value="#004F8B"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">110 0 944,'0'0'1999,"1"3"-3123,4-3 217</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="170.22">110 0 1409</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="480.64">123 0 1409,'72'13'1045,"-58"-10"8074,-41 16-8796,-17 37 84,-72 98 1072,99-127-1064,12-18-9116,10-19 3301</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1003.78">3 52 1297,'0'0'6507,"1"10"-3218,-1-5-3163,0 0 0,1 1-1,0-1 1,0 0 0,1 0 0,3 10-1,28 24 328,1-1 0,54 48-1,-82-81-2319</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2374.58">408 79 1905,'0'0'13257,"-4"32"-11894,-3 12-1169,1 0-1,3 0 1,1 0 0,6 53-1,-2 1-97,-2 77 390,0-175 18,-27-21-458,23 16-35,-1 0 0,1 0 0,0 0 0,1-1 0,-1 0 0,1 1 0,0-1 0,1-1 0,-1 1 0,1 0 0,1 0 0,-1-1 0,1 1 0,-1-8 0,2 13-30,12 30-437,13 11 500,23 47 104,-48-86-141,0-1 1,0 0-1,1 1 0,-1-1 1,0 1-1,0-1 0,0 1 1,0-1-1,0 0 0,1 1 1,-1-1-1,0 1 0,0-1 1,1 0-1,-1 1 0,0-1 1,1 0-1,-1 1 0,0-1 1,1 0-1,-1 0 0,0 1 0,1-1 1,-1 0-1,1 0 0,-1 0 1,0 1-1,1-1 0,-1 0 1,1 0-1,-1 0 0,1 0 1,-1 0-1,1 0 0,-1 0 1,0 0-1,1 0 0,-1 0 1,1 0-1,-1 0 0,1 0 1,-1-1-1,0 1 0,1 0 1,-1 0-1,1 0 0,-1-1 1,0 1-1,1 0 0,-1 0 0,0-1 1,1 1-1,0-1 0,9-14 217,42-91-93,-51 101 52</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 125 4978,'0'0'8730,"1"-48"-4822,1 43-3913,1 0-1,-1 0 1,1 0 0,1 0-1,-1 0 1,0 1 0,1 0-1,0-1 1,9-6 0,4-6 143,-17 16-137,1 1 0,-1-1 0,1 1-1,-1 0 1,0-1 0,1 1-1,-1 0 1,1 0 0,-1-1 0,1 1-1,-1 0 1,1 0 0,-1-1-1,1 1 1,-1 0 0,1 0 0,0 0-1,-1 0 1,1 0 0,-1 0-1,1 0 1,-1 0 0,1 0 0,-1 0-1,1 0 1,-1 0 0,1 1-1,-1-1 1,1 0 0,-1 0-1,1 0 1,-1 1 0,1-1 0,-1 0-1,1 1 1,-1-1 0,1 0-1,-1 1 1,0-1 0,1 1 0,-1-1-1,0 0 1,1 1 0,-1-1-1,0 1 1,0-1 0,1 1 0,-1-1-1,0 2 1,15 30-54,-13-27 121,5 17-27,0 0-1,-1 0 1,-2 0 0,0 1 0,1 29-1,-5 120 39,-2-81-7,2-71-97,-1-10 71,1-1 0,0 1 0,0 0 0,1 0 0,1 0 0,0-1 0,0 1 0,1-1 0,4 12 0,-6-19-43,0-1-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0 0,1 0 0,-1 0-1,0 0 1,0 0 0,1 0-1,-1-1 1,1 1 0,-1-1-1,0 1 1,1-1 0,-1 1 0,1-1-1,0 0 1,-1 0 0,1 0-1,-1 0 1,1 0 0,-1 0 0,1 0-1,1-1 1,-1 1 10,0 0 0,0 0 0,0-1 0,0 1-1,0-1 1,0 0 0,0 0 0,0 0 0,0 1 0,0-2 0,-1 1 0,1 0-1,0 0 1,-1 0 0,1-1 0,-1 1 0,1-1 0,-1 1 0,2-3 0,2-10 45,-1 0 0,0 0 0,-1-1 0,0 0 0,-2 0 0,1 1 0,-2-24 0,0 37 451,-1 34-797,-14 343 286,26 133-25,-12-508 28,1 0 0,0 0 0,0 0 1,-1 0-1,1 0 0,-1 0 0,1 0 0,-1 0 1,1 0-1,-1 0 0,1-1 0,-1 1 0,0 0 0,0 0 1,1-1-1,-1 1 0,0 0 0,0-1 0,0 1 0,0-1 1,0 1-1,1-1 0,-1 1 0,0-1 0,0 0 1,0 1-1,0-1 0,0 0 0,-1 0 0,1 0 0,0 0 1,-1 0-1,-44 0 79,32 0-135,9 0-126,0-1 1,0 1-1,1-1 1,-1 0-1,1 0 1,-1 0-1,1 0 1,-1-1-1,1 0 1,-5-2-1,-22-19-6005,20 10-777</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -2214,7 +2616,7 @@
           <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
         </inkml:channelProperties>
       </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2025-01-04T15:33:16.752"/>
+      <inkml:timestamp xml:id="ts0" timeString="2025-02-22T15:38:22.213"/>
     </inkml:context>
     <inkml:brush xml:id="br0">
       <inkml:brushProperty name="width" value="0.035" units="cm"/>
@@ -2222,9 +2624,13 @@
       <inkml:brushProperty name="color" value="#004F8B"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">162 12 304,'0'0'2892,"4"-3"-2148,10-5 291,-13 11 1632,-23 23 3128,-1 2-6237,-12 22 898,-43 54 1460,65-93-887,6-7-3257,4-19-11620</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="447.74">27 2 720,'0'0'5453,"2"10"85,8 37-4758,-2-30-623,0 1 0,2-2-1,0 1 1,1-1 0,0-1-1,1 0 1,24 23 0,-26-33-562,-4-3-4873</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1684.78">334 114 4690,'0'-2'11015,"0"5"-10326,-6 340 1285,22-144-1251,-12-177-645,-2-8 933,-14-28-542,-11-18-425,14 22-28,2-1 1,-1 0-1,-8-17 1,11 11-41,4 14-299,1 17 212,0-13 115,3 12-10,0-1 0,1 1 0,0 0-1,1-1 1,1 0 0,0-1 0,0 1 0,10 12-1,4-4 53,-19-20-40,-1 1-1,1-1 0,-1 0 1,1 0-1,-1 0 0,1 0 1,-1 0-1,1 0 1,0 0-1,-1 0 0,1 0 1,-1 0-1,1 0 0,-1 0 1,1 0-1,0-1 0,-1 1 1,1 0-1,-1 0 0,1-1 1,-1 1-1,1 0 0,-1 0 1,0-1-1,1 1 0,-1-1 1,1 1-1,2-5 24,0 0 0,0 0 0,0 0-1,-1 0 1,0-1 0,3-9 0,-1 4-61,44-135-248,-48 146 369,1-8-471,-1 8 235,0 0 1,0 0-1,0 0 0,0-1 0,-1 1 0,1 0 1,0 0-1,0 0 0,0 0 0,0-1 0,0 1 1,0 0-1,-1 0 0,1 0 0,0 0 0,0 0 1,0-1-1,0 1 0,-1 0 0,1 0 0,0 0 1,0 0-1,0 0 0,0 0 0,-1 0 0,1 0 1,0 0-1,0 0 0,0 0 0,-1 0 0,1 0 1,0 0-1,0 0 0,0 0 0,-1 0 0,1 0 1,0 0-1,0 0 0,0 0 0,-1 0 0,1 0 1,0 0-1,0 1 0,0-1 0,0 0 0,-1 0 0,1 0 1,0 0-1,0 0 0,0 0 0,0 1 0,0-1 1,-1 0-1,-17 10-4669</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">0 148 6115,'0'0'11853,"0"39"-10303,0 166-88,0-118-10666</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="164.63">88 38 7203,'0'0'9253,"43"4"-16009,-32 20 273</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1221.8">253 201 7459,'0'0'8879,"0"20"-7580,0 168 902,0-163-1882,2-33-36,8-39-212,-5 36-68,-2 2-48,1-1 0,0 1 0,0 0 1,1 0-1,0 0 0,1 1 0,0 0 0,0 0 0,1 1 0,12-12 0,-18 19 41,0 0 0,0-1 1,0 1-1,0 0 0,-1 0 1,1 0-1,0 0 0,0 0 1,0 0-1,0 0 0,0 1 0,0-1 1,0 0-1,0 0 0,0 1 1,0-1-1,0 1 0,-1-1 1,1 1-1,0-1 0,0 1 1,-1-1-1,1 1 0,0 0 0,0-1 1,-1 1-1,1 0 0,-1-1 1,1 1-1,-1 0 0,1 0 1,-1 0-1,1 0 0,-1 0 0,1 1 1,16 40 290,-14-33-206,7 17-45,-5-9 118,2 0 0,14 29-1,-19-43-235,0 0-1,-1 0 0,1-1 0,0 1 0,1 0 0,-1-1 0,0 1 0,1-1 0,-1 0 0,1 1 0,0-1 1,0-1-1,0 1 0,0 0 0,0-1 0,0 1 0,0-1 0,0 0 0,1 0 0,4 1 0,-2-2-379,0 1 0,0-1-1,0 0 1,-1-1 0,1 0 0,0 1-1,0-2 1,-1 1 0,1-1-1,0 0 1,-1 0 0,0 0-1,1-1 1,-1 0 0,7-5-1,-8 5 284,-1-1-1,0 0 0,1 0 0,-2 0 1,1 0-1,0 0 0,-1-1 0,0 1 0,0-1 1,0 1-1,0-1 0,-1 0 0,0 0 0,0 0 1,0 0-1,0 0 0,-1 0 0,0-8 0,0 6 37,0-1 938,0 0-1,0 1 1,-1-1 0,0 0-1,-3-14 1,3 21-704,1 0 0,-1 0 0,1 0 0,-1 0 0,0-1 0,1 1 0,-1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 1 0,0-1 1,0 0-1,0 0 0,0 1 0,0-1 0,0 0 0,-1 1 0,1 0 0,0-1 0,0 1 0,-1-1 0,1 1 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,-1 1 1,1-1-1,0 0 0,0 1 0,0-1 0,-1 1 0,1-1 0,0 1 0,0 0 0,0-1 0,-2 3 0,-2 0-56,1 0 0,-1 0 0,1 1-1,0 0 1,0 0 0,0 0 0,0 1 0,1-1 0,-1 1-1,1 0 1,0 0 0,1 0 0,-1 0 0,1 0 0,0 1-1,-2 8 1,0 3 58,0 0 0,2 0 0,0 0 0,0 23 0,2-39-97,1 1 0,-1-1 0,1 0 1,0 1-1,-1-1 0,1 0 1,0 0-1,0 0 0,0 0 1,0 0-1,0 0 0,0 0 1,0 0-1,0 0 0,0 0 1,0 0-1,1-1 0,-1 1 0,0 0 1,0-1-1,1 1 0,-1-1 1,1 0-1,-1 1 0,0-1 1,1 0-1,-1 0 0,1 0 1,-1 0-1,0 0 0,1 0 1,-1 0-1,2-1 0,5 1-73,-1 0 0,1-1 0,-1 0 0,1 0 1,12-5-1,-9 1-144,-1-1 1,-1 0 0,1-1-1,-1 1 1,0-2-1,-1 1 1,1-1 0,-2-1-1,1 1 1,-1-2 0,0 1-1,-1 0 1,0-1 0,-1 0-1,7-16 1,3-12-27,-2 0 0,-1 0 0,6-44 0,-14 58 483,-2 0 0,0-47 1,-2 46 1577,0 24-125,-1 2-1688,0 0 0,0 0 1,1 0-1,-1 0 0,0 0 0,1 0 0,-1 0 1,1 0-1,0 0 0,-1 0 0,1 0 0,0 0 1,0 0-1,-1 1 0,1-1 0,0 0 0,0 0 1,0 0-1,0 0 0,1 2 0,-2 6-61,-10 74 522,-3 135 0,15-212-455,-1 1 1,1 0 0,0-1 0,1 1-1,-1-1 1,1 0 0,1 0 0,-1 1 0,1-1-1,0-1 1,0 1 0,1 0 0,0-1 0,0 0-1,0 1 1,0-2 0,1 1 0,0 0 0,0-1-1,6 4 1,-7-5-4,0-1-1,0 1 1,1-1-1,-1 0 1,1 0-1,0-1 1,-1 1-1,1-1 1,0 0-1,0 0 1,0-1-1,0 1 1,0-1-1,0 0 1,-1-1-1,1 1 1,0-1-1,0 0 1,0 0-1,0 0 1,-1-1-1,1 0 1,0 0-1,-1 0 1,0 0-1,1-1 0,6-4 1,-3 0-6,0 1-1,0-1 1,0-1 0,-1 1-1,0-1 1,-1-1 0,0 1-1,0-1 1,-1 0 0,7-15-1,-7 10 20,-1 0 0,-1 0-1,0 0 1,0 0-1,-1-1 1,-1-29 0,-1 42-16,0 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,-1 0 0,1 0 0,-1 0 0,0 0 1,1 0-1,-1 0 0,0 0 0,0 0 0,0 1 0,-1-1 0,1 0 0,0 1 0,-1-1 0,1 1 0,0-1 0,-1 1 0,0 0 0,1 0 0,-1 0 1,0 0-1,0 0 0,0 0 0,0 0 0,1 0 0,-1 1 0,0-1 0,0 1 0,-1-1 0,1 1 0,0 0 0,-3 0 0,4 0 9,-1 1-1,0 0 1,0 0-1,1-1 1,-1 1-1,1 0 1,-1 0-1,0 1 1,1-1-1,0 0 0,-1 0 1,1 1-1,0-1 1,0 1-1,0-1 1,0 1-1,0 0 1,-1 2-1,-17 33 300,19-37-301,-8 20 11,1 1 0,2 0 0,0 0 0,1 0 1,1 0-1,0 1 0,2-1 0,1 1 0,3 25 1,-3-45-154,0-1 1,1 1 0,-1-1-1,1 1 1,-1-1-1,1 0 1,-1 1 0,1-1-1,0 0 1,0 0-1,0 1 1,0-1 0,0 0-1,0 0 1,0 0-1,0 0 1,0 0 0,0 0-1,1 0 1,-1-1-1,0 1 1,0 0 0,1-1-1,-1 1 1,1-1 0,2 1-1,41 3-5915,-39-4 4775,27 0-6626</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1570.69">1296 198 8740,'0'0'10738,"-6"4"-10575,-18 18-64,2 0 0,0 1 0,2 2 1,1 0-1,-24 40 0,43-64-145,-2 2-103,1-1 0,-1 1 0,1-1 0,-1 1 0,0-1 0,0 0 0,0 0 0,0 1-1,0-1 1,-1-1 0,1 1 0,0 0 0,-1 0 0,0-1 0,1 0 0,-1 1 0,-3 0 0,5-23-1954,1 7 2044,1-1-1,1 0 0,0 1 0,1 0 1,0-1-1,1 1 0,1 0 0,0 0 1,11-19-1,-16 32 116,1 1 0,-1-1 0,0 1 1,0 0-1,0-1 0,0 1 0,0 0 1,1-1-1,-1 1 0,0 0 0,0 0 1,1-1-1,-1 1 0,0 0 0,1 0 1,-1-1-1,0 1 0,0 0 0,1 0 1,-1 0-1,0-1 0,1 1 0,-1 0 1,1 0-1,-1 0 0,0 0 0,1 0 0,-1 0 1,0 0-1,1 0 0,-1 0 0,1 0 1,-1 0-1,0 0 0,1 0 0,-1 0 1,0 0-1,1 0 0,-1 1 0,1-1 1,11 16 363,2 26-345,-9-18-208,-1-6 387,0 0 0,13 31 0,-15-45-583,0 1 0,0-1 1,1 1-1,0-1 0,0 0 0,0 0 1,0 0-1,1 0 0,-1-1 0,1 0 0,0 1 1,0-1-1,0 0 0,0-1 0,6 3 1,16 5-4997</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1762.67">1414 343 6355,'0'0'11269,"27"-16"-11317,0 16-224,-5 0-1969,5 0-1217,-6 0-2112</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2811.2">1656 241 9652,'0'0'7948,"0"9"-7686,0 141 1253,0-150-1184,1-11 72,2 0-397,0 0 1,0-1 0,1 2 0,1-1-1,0 0 1,0 1 0,1 0 0,0 0-1,1 1 1,0-1 0,0 2 0,10-10 0,-16 17-18,-1 1 0,1-1 1,-1 1-1,1-1 1,-1 1-1,1 0 0,-1-1 1,1 1-1,-1 0 1,1-1-1,-1 1 0,1 0 1,0 0-1,-1-1 1,1 1-1,0 0 0,-1 0 1,1 0-1,0 0 1,-1 0-1,1 0 1,0 0-1,-1 0 0,1 0 1,-1 0-1,1 0 1,0 0-1,-1 1 0,1-1 1,0 0-1,-1 0 1,1 1-1,-1-1 0,1 1 1,12 24-139,-3 39 122,-10-60 19,1 94 74,-1-97 33,22-48 296,-16 31-433,1 0-1,1 0 1,0 1-1,1 0 1,0 0 0,1 1-1,1 1 1,0-1-1,16-13 1,-26 27 32,-1 0 0,0-1 1,1 1-1,-1 0 1,1-1-1,-1 1 0,1 0 1,-1 0-1,1-1 0,-1 1 1,0 0-1,1 0 0,0 0 1,-1 0-1,1 0 0,-1 0 1,1 0-1,-1 0 1,1 0-1,-1 0 0,1 0 1,-1 0-1,1 0 0,-1 0 1,1 0-1,-1 0 0,1 1 1,-1-1-1,1 0 1,-1 0-1,0 1 0,1-1 1,-1 0-1,1 0 0,-1 1 1,0-1-1,1 1 0,-1-1 1,0 0-1,1 1 0,-1-1 1,0 1-1,1-1 1,-1 1-1,0-1 0,0 1 1,0-1-1,0 1 0,1-1 1,-1 1-1,0-1 0,0 1 1,0-1-1,0 1 1,0-1-1,0 1 0,0 0 1,2 38 202,-2-34-123,0 158-333,0-162 71,1 0 0,0 0 0,0-1 0,-1 1 0,1 0 0,0 0 1,0-1-1,0 1 0,0 0 0,0-1 0,0 1 0,0-1 0,0 1 0,0-1 0,0 0 0,0 0 0,1 1 1,-1-1-1,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,1 0 0,-1-1 0,0 1 0,1-1 0,38-5-3657,-35 3 3462,1 0 0,-1 0 0,0-1 1,0 1-1,0-1 0,-1 0 0,1-1 0,-1 1 0,0-1 1,0 0-1,0 0 0,-1 0 0,1 0 0,-1-1 0,3-9 0,9-38 2959,-11-2 6985,-6 55-9399,0 0 0,0 0 1,0 0-1,0 0 0,0 1 1,0-1-1,0 1 0,1 0 1,-1-1-1,0 1 0,0 0 1,-2 2-1,-1 1-165,0 1-1,0-1 0,0 1 1,1 1-1,0-1 1,0 1-1,0-1 1,0 1-1,1 0 0,0 0 1,1 1-1,-1-1 1,1 1-1,0-1 1,1 1-1,0 0 1,-1 8-1,2-14-852,4-2 369,1-1 1,-1 0-1,1 0 1,-1 0-1,0 0 1,0 0 0,0-1-1,0 0 1,-1 0-1,1 0 1,-1 0-1,0-1 1,1 1-1,-1-1 1,-1 0 0,1 1-1,3-8 1,-4 14 3305,0 0-2593,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,1 0 0,0 0 0,0-1 0,0 1 0,0-1 1,0 1-1,0-1 0,6 3 0,-6-6-140,1 0 1,-1 0 0,1 0 0,-1 0-1,0-1 1,1 1 0,-1-1 0,0 0-1,0 0 1,0 0 0,0 0 0,-1-1 0,1 1-1,0-1 1,-1 1 0,0-1 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0-1,-1-1 1,2-3 0,6-14 76,-2 0 0,9-31 1,-7 10 408,-2 0 0,-2 0 0,1-49 1,-9 134-459,-8 55 1,-3 21-32,10-16-960,3-36-5655,1-46 36</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3481.86">2210 287 10629,'0'0'7299,"11"-6"-7488,0 0-363,-1 0 1,1 1-1,1 0 0,-1 1 1,1 0-1,-1 1 1,24-4-1,-26 6-129,-2 1 407,-1 0 1,0-1 0,0 0-1,1 0 1,-1 0 0,0-1-1,0 0 1,0 0 0,7-10 7531,-13 12-7095,-9 5 3108,4-1-4395,0 3 1165,0 0-1,0-1 1,1 2 0,0-1-1,1 0 1,-1 1 0,2-1 0,-1 1-1,1 0 1,0 0 0,0 0-1,1 0 1,1 0 0,-1 1-1,1 11 1,4-19-106,0 0-1,-1-1 1,1 1 0,-1-1-1,1 0 1,0 1-1,-1-2 1,1 1 0,0 0-1,-1-1 1,7-1 0,-3-1-115,1-1-1,-1 0 1,0 0 0,0-1 0,0 1 0,0-2 0,-1 1 0,0-1 0,0 0-1,-1 0 1,0 0 0,0-1 0,6-9 0,0-2-39,-1 0 1,-1-1-1,0-1 0,7-23 1,7-40 64,-19 62 3632,-20 227-3121,16-200-350,0 1 0,0-1-1,1 1 1,0-1-1,0 0 1,0 1 0,3 6-1,-3-11-2,0-1 0,0 0-1,-1 1 1,1-1 0,0 0-1,0 0 1,0 0 0,0 1-1,1-1 1,-1 0 0,0-1 0,0 1-1,1 0 1,-1 0 0,0 0-1,1-1 1,-1 1 0,1-1-1,-1 1 1,1-1 0,-1 1-1,1-1 1,-1 0 0,1 0-1,-1 0 1,1 0 0,-1 0 0,1 0-1,-1 0 1,1 0 0,0-1-1,-1 1 1,1-1 0,-1 1-1,0-1 1,2 0 0,2-1 16,-1-1 0,0 1 0,0 0 0,0-1 0,0 0 0,0 0 0,-1 0 0,1 0 1,-1-1-1,0 1 0,5-8 0,29-50 118,-26 41-45,-11 19-64,0 1-1,0 0 1,1-1 0,-1 1-1,0 0 1,0-1 0,0 1 0,0 0-1,1 0 1,-1-1 0,0 1-1,0 0 1,1 0 0,-1-1-1,0 1 1,0 0 0,1 0 0,-1-1-1,0 1 1,0 0 0,1 0-1,-1 0 1,0 0 0,1 0-1,-1 0 1,0 0 0,1-1-1,-1 1 1,0 0 0,1 0 0,-1 0-1,1 0 1,-1 0 0,1 1-1,6 10 260,3 25-349,-9-30 260,0 0-134,1 0 0,0 0 1,1 0-1,-1-1 0,1 1 0,0-1 1,0 1-1,1-1 0,7 8 0,-9-11-84,-1 0-1,1-1 1,0 1 0,0-1-1,0 0 1,1 0 0,-1 0-1,0 0 1,0 0 0,1 0-1,-1 0 1,0-1-1,1 1 1,-1-1 0,0 0-1,1 0 1,-1 0 0,1 0-1,-1 0 1,1 0 0,-1-1-1,0 1 1,1-1-1,-1 1 1,0-1 0,0 0-1,1 0 1,1-2 0,29-23-2569,4-7-4191</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -2244,7 +2650,7 @@
           <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
         </inkml:channelProperties>
       </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2025-01-04T15:33:26.966"/>
+      <inkml:timestamp xml:id="ts0" timeString="2025-02-22T15:38:18.606"/>
     </inkml:context>
     <inkml:brush xml:id="br0">
       <inkml:brushProperty name="width" value="0.035" units="cm"/>
@@ -2252,7 +2658,14 @@
       <inkml:brushProperty name="color" value="#004F8B"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1164 0 2353,'0'0'10696,"-5"2"-7096,-23 8-3441,-16-5 211,-77-2 0,-20 2-185,45 7-128,0-4 0,-131-7 0,153-14 30,57 8-45,-1 2 0,1 0 1,-25 0-1,16 2-13,1 2-1,-1 1 1,0 1 0,1 1-1,0 1 1,-35 12-1,58-17 4,1 0 0,0 0 0,0 1-1,0-1 1,0 1 0,-1-1-1,1 1 1,0-1 0,0 1 0,0 0-1,0 0 1,0-1 0,0 1-1,0 0 1,1 0 0,-1 0-1,0 0 1,0 0 0,1 0 0,-1 0-1,0 0 1,1 0 0,-1 0-1,1 1 1,0-1 0,-1 0 0,1 0-1,0 0 1,0 1 0,0-1-1,0 0 1,0 0 0,0 1 0,0-1-1,0 0 1,0 0 0,1 3-1,-1 9-184,3 22 198,1 0 0,1 0 0,14 44 0,5 30 17,-14-75 5,-10-33-38,28 0 185,53 11 0,-1-1-207,478 2 123,-397-14-105,-137 3-21,-1 1 0,1 1-1,41 12 1,4 0 18,-30-3-27,-32-10 25,0-1 0,0 0 0,1 0 0,-1 0 0,14 1 0,-20-3 97,10-34 526,-6-15-647,-2-1 0,-4-57-1,-1 24 42,1 76-31,0 0 0,0-1 0,0 1 0,-1 0 0,-1-1-1,1 1 1,-1 1 0,0-1 0,0 0 0,-1 1-1,0-1 1,-5-5 0,-8-15 14,15 20-26,1 5 13,1 1 0,0 0 0,-1-1 0,1 1 0,-1-1-1,1 1 1,-1 0 0,0-1 0,0 1 0,0 0 0,1 0-1,-1 0 1,0 0 0,0 0 0,-1 0 0,1 0-1,0 0 1,0 0 0,0 0 0,-1 0 0,0 0 0,-10-2-47,1 0 1,0 1-1,-1 0 1,0 1-1,1 0 1,-1 1 0,0 0-1,-18 4 1,-13-3-68,41-1 49,-1 0 0,1 0 0,0 1 0,-1-1 0,1 0 0,0 1 0,0-1 0,-1 1 0,1 0 0,0 0-1,-3 1 1,5-2-157,-1 1-1,0-1 0,1 1 1,-1 0-1,1-1 0,-1 1 0,1 0 1,-1-1-1,1 1 0,-1 0 0,1-1 1,0 1-1,-1 0 0,1 0 1,0 0-1,0-1 0,-1 1 0,1 0 1,0 0-1,0 0 0,0 1 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">156 121 3874,'0'0'6896,"0"-16"489,-1 37-7265,-1 0-1,0-1 1,-2 1 0,-1-1-1,-11 31 1,-1-8 168,-32 61 0,17-52-227,15-37-3348,14-13 1683,-5-15-10214</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="250.18">0 155 4178,'0'0'9479,"1"0"-9469,-1-1-1,0 1 1,1 0-1,-1 0 1,0 0 0,1 0-1,-1 0 1,0 0 0,0-1-1,1 1 1,-1 0 0,0 0-1,1 0 1,-1 0 0,0 0-1,1 0 1,-1 0-1,0 0 1,1 1 0,-1-1-1,0 0 1,1 0 0,-1 0-1,0 0 1,0 0 0,1 0-1,-1 1 1,0-1-1,1 0 1,-1 0 0,0 0-1,0 1 1,0-1 0,1 0-1,-1 0 1,0 1 0,0-1-1,0 0 1,1 1 0,-1-1-1,0 0 1,0 0-1,0 1 1,8 12 384,-1-1-1,0 1 1,-1 0-1,0 0 1,-1 1-1,5 21 1,-1-8-156,51 154 736,-60-179-1068,0-1 0,1 1 0,0-1 0,-1 1 0,1-1 0,0 0 0,0 1 0,0-1 0,0 1 0,0-1 0,0 0 0,0 0 0,0 0 0,0 0 0,2 1 0,25 4-6888,-12-6 237</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="578.31">299 74 464,'0'0'15447,"0"5"-14910,0 444 3029,0-448-3509,17-4-4094,0-14-472,3-6-1814</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="916.86">511 296 5715,'0'0'10666,"-1"7"-10349,-5 20 132,2 1 0,-1 51 1,6-77-444,-1 0 1,1 1 0,-1-1 0,1 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0-1,1-1 1,-1 1 0,1 0 0,0-1-1,-1 1 1,1-1 0,0 1 0,0-1-1,0 0 1,0 0 0,3 2-1,-3-3-1,-1 1 0,0 0 0,1-1-1,-1 1 1,0-1 0,1 1 0,-1-1-1,0 0 1,1 1 0,-1-1 0,1 0-1,-1 0 1,1 0 0,-1 0 0,0 0-1,1-1 1,-1 1 0,1 0-1,-1-1 1,0 1 0,1-1 0,-1 1-1,0-1 1,1 0 0,-1 1 0,0-1-1,0 0 1,0 0 0,0 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0-1,1-2 1,2-10-2,-1 1 0,0-1 0,-1 1 1,0-1-1,-1 0 0,-1 0 0,0 1 0,-2-19 0,1-7-58,1 37 43,-1-1-1,1 1 0,0 0 1,0 0-1,-1-1 0,1 1 1,-1 0-1,1 0 0,-1-1 1,0 1-1,1 0 0,-1 0 1,0 0-1,0 0 0,0 0 1,0 0-1,0 0 0,0 0 1,0 0-1,0 1 0,0-1 1,0 0-1,0 0 0,0 1 1,-1-1-1,1 1 0,0 0 1,0-1-1,-1 1 0,1 0 1,0-1-1,-1 1 0,1 0 1,0 0-1,-1 0 0,1 0 1,-2 1-1,0-1-207,0 0 0,0 0 0,1 1 1,-1-1-1,0 1 0,1-1 0,-1 1 0,0 0 0,1 0 1,-1 0-1,1 1 0,-1-1 0,1 0 0,0 1 1,0 0-1,0-1 0,0 1 0,-2 2 0,-5 14-2925,7-2-1793</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1260.39">751 222 5523,'0'0'10975,"-10"21"-10583,-29 71-176,37-88-204,0 1-1,0-1 1,0 1-1,1-1 0,0 1 1,0 0-1,0 0 1,0-1-1,1 1 0,0 0 1,0 0-1,0 0 1,1 0-1,0 0 0,-1-1 1,4 10-1,-2-12 1,0 0 0,0 0 0,0 0 0,0 0 0,0 0-1,0 0 1,1-1 0,-1 1 0,0-1 0,1 0 0,0 1 0,-1-1 0,1 0-1,0-1 1,-1 1 0,1 0 0,0-1 0,0 0 0,-1 1 0,1-1 0,0 0 0,5-1-1,-6 1 10,1-1 0,0 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1-1 0,0 1 0,0-1 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,-1-1 0,0 1 0,0-1 0,0 1 0,0-1 0,0 1 0,0-1 0,0-4 0,3-6 46,-2 0 0,1 0 0,-2 0 0,1-19 0,-2 27-64,0 1 0,-1 0 0,1-1 0,-1 1 0,0 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,-1 0 0,1 1 0,-1-1 0,0 1 0,0 0 0,0 0 0,0 0 0,0 0 0,-1 1 0,1-1 0,-1 1 0,1 0 0,-6-3 0,5 4-347,0 0 0,0 0 0,1 0 0,-1 0 0,0 1 0,0-1 0,0 1 0,-1 0 0,1 0 0,0 1 1,-4 0-1,3 3-3015,4 7-1054</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1508.46">934 25 10485,'0'0'9188,"0"9"-9268,0 34 80,0 9 880,0 4-608,0 2-127,0-6-81,0 4-48,0-7-32,0-9-609,11-16-1392,5-11-2257,0-13-3633</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2585.58">1124 228 8580,'0'0'7860,"-18"22"-7540,-9 10-255,-61 69 96,60-78 210,33-35-194,-5 12-178,1-1 1,-1 0 0,0 0-1,0 0 1,1 0-1,-1 0 1,0 1 0,1-1-1,-1 0 1,1 0 0,-1 1-1,1-1 1,-1 0-1,1 0 1,-1 1 0,1-1-1,0 1 1,-1-1 0,1 1-1,0-1 1,1 0-1,4-2-15,-1 0 0,1 1 0,0 0 0,0 0 0,0 1 0,0 0 0,0-1 0,0 2 0,0-1 0,0 1 0,12 1 0,4 2 14,0 1 0,23 7 0,34 5-2,-76-15 10,-1-1 0,1 0 0,-1 1 0,1-1 0,-1 0 1,1 0-1,-1-1 0,1 1 0,-1 0 0,0-1 0,1 0 1,-1 0-1,1 1 0,-1-1 0,0 0 0,0-1 0,1 1 1,-1 0-1,0-1 0,3-2 0,-3 0 25,1 0 1,-1 0-1,0-1 0,0 1 0,-1-1 0,1 1 0,-1-1 1,1-8-1,4-13 44,0-20 2497,-6 59-2831,-1-5 244,2 0 0,-1 0 0,1-1 1,0 1-1,0-1 0,1 1 0,0-1 0,4 10 0,-5-15 0,0 0 0,0 0 0,1-1 0,-1 1 0,1 0 0,-1-1 0,1 1 0,-1 0 0,1-1 0,0 0 0,0 1 0,-1-1 0,1 0 0,0 0 1,0 0-1,0 0 0,1-1 0,-1 1 0,0 0 0,0-1 0,0 1 0,0-1 0,1 0 0,-1 0 0,0 0 0,0 0 0,1 0 0,-1-1 0,0 1 0,0 0 0,0-1 0,0 0 0,3-1 0,0 1-16,-1-1 0,0-1 0,0 1 0,0 0 0,0-1 0,0 0 0,-1 0 1,1 0-1,-1 0 0,0-1 0,0 1 0,5-8 0,23-43-29,-23 43 1064,-8 20-1011,0 0 0,1-1-1,0 1 1,1 0 0,0-1 0,0 1 0,7 13 0,-8-19-1,0 0 1,1 0-1,0 0 1,-1 0 0,1-1-1,0 1 1,0 0-1,1-1 1,-1 0 0,0 1-1,1-1 1,0 0-1,-1 0 1,1 0 0,0-1-1,0 1 1,0-1-1,0 0 1,0 1 0,0-1-1,0-1 1,1 1-1,3 0 1,-3 0-11,0-1-1,0 1 1,0-1-1,0 0 0,0 0 1,0-1-1,0 1 1,0-1-1,0 0 1,0 0-1,0 0 1,0-1-1,-1 1 1,1-1-1,-1 0 1,1 0-1,-1 0 1,0-1-1,1 1 1,-1-1-1,0 1 1,-1-1-1,1 0 1,0 0-1,-1 0 1,0-1-1,0 1 1,0-1-1,0 1 0,0-1 1,-1 0-1,1 1 1,0-7-1,6-16 21,-1-1 0,-2 0-1,0-1 1,0-29 0,-2-87 762,-3 126-248,-42 551-723,40-516 190,1-7 16,0 11 2,-2-1 0,0 1 0,-1-1 1,-1 1-1,-1-1 0,0-1 0,-11 21 0,10-36 67,2-14 85,0-13 101,0-10-300,2-1 1,1 1-1,2-1 0,6-44 1,-4 59-160,1-1 0,1 1 0,1 0 0,1 0 0,0 0 0,2 1 0,0 0 0,17-28 0,-23 44 143,-1 0 0,0 0 0,1 0 0,-1 0 0,1 0 0,0 1 0,-1-1 0,1 0 1,0 1-1,0 0 0,0-1 0,4 0 0,-6 2 46,1-1 0,0 1 0,-1 0 1,1 1-1,0-1 0,0 0 0,-1 0 0,1 0 0,0 0 1,-1 1-1,1-1 0,0 0 0,-1 0 0,1 1 1,0-1-1,-1 1 0,1-1 0,-1 0 0,1 1 0,-1-1 1,1 1-1,-1 0 0,1-1 0,-1 1 0,1-1 1,-1 1-1,0 0 0,1-1 0,-1 1 0,0 0 0,1-1 1,-1 1-1,0 0 0,0-1 0,0 1 0,0 0 0,0 0 1,0 0-1,3 9-1,-1 0 1,0 0-1,0 0 0,-2 1 1,1-1-1,-1 0 1,0 0-1,-3 14 0,2-18-80,-1-1 0,0 1 0,0-1-1,0 1 1,-1-1 0,0 0-1,0 0 1,0 0 0,0-1-1,-1 1 1,0-1 0,0 0 0,0 0-1,0 0 1,-1-1 0,-7 5-1,-2 1-4117,7-5-2060</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2836.99">2122 376 12550,'0'0'8628,"0"18"-8580,0 13 0,-10 6 80,-12 3-112,-5-6-16,-5 0-400,0-4-833,5-8-1856,5-10-4883</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -2272,7 +2685,7 @@
           <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
         </inkml:channelProperties>
       </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2025-01-04T15:33:23.434"/>
+      <inkml:timestamp xml:id="ts0" timeString="2025-02-22T15:38:30.015"/>
     </inkml:context>
     <inkml:brush xml:id="br0">
       <inkml:brushProperty name="width" value="0.035" units="cm"/>
@@ -2280,8 +2693,7 @@
       <inkml:brushProperty name="color" value="#004F8B"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">0 442 2225,'0'0'7273,"2"-7"-5126,8-20 8586,-9 28-10749,1-1 0,0 1 0,-1 0 0,0-1 1,1 1-1,-1 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,1 1 0,-1-1 0,-1 0 0,1 1 0,1 2 0,19 33 56,-14-23-22,-1-1 1,0 1-1,0 0 1,-2 0 0,5 22-1,-5-21 70,-4-14-85,0-1 0,0 1-1,0-1 1,0 1 0,0 0-1,1-1 1,-1 1 0,0-1-1,0 1 1,1-1 0,-1 1-1,0 0 1,1-1-1,-1 1 1,0-1 0,1 0-1,-1 1 1,1-1 0,-1 1-1,1-1 1,-1 0 0,1 1-1,-1-1 1,1 0 0,-1 1-1,1-1 1,-1 0 0,1 0-1,-1 1 1,1-1 0,0 0-1,0 0 1,19-11 61,19-37-5,-32 39-59,85-96 61,-88 99-1787,1 0-2896,-3 21-5805</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1231.07">431 635 1777,'0'0'16599,"4"-35"-14934,34-240-352,-35 226-1196,-4-54 0,0 33-31,0 66-83,0 0 0,0 0 0,0 0 1,0 1-1,0-1 0,-1 0 0,1 1 0,-5-8 0,3 8-8,1-1-1,0-1 0,0 1 0,0 0 0,0 0 1,1-1-1,0 1 0,0-1 0,-1-6 1,2 11 1,0-1 1,1 1 0,-1-1 0,0 1 0,0 0 0,0-1 0,0 1 0,0-1-1,0 1 1,-1-1 0,1 1 0,0-1 0,0 1 0,0 0 0,0-1-1,0 1 1,-1-1 0,1 1 0,0 0 0,0-1 0,-1 1 0,1 0 0,0-1-1,-1 1 1,1 0 0,0-1 0,-1 1 0,1 0 0,0 0 0,-1-1-1,1 1 1,-1 0 0,1 0 0,-1-1 0,-16 8-292,-13 19 99,19-10 198,1 1-1,0 0 0,-11 28 1,62-97 130,-36 46-121,0 0 0,0 0 1,1 1-1,-1 0 0,1 0 0,0 0 1,1 1-1,-1 0 0,1 0 0,10-4 1,-11 7-23,-1 1 1,1-1-1,0 1 1,-1 1-1,1-1 1,-1 1-1,1 0 1,-1 0-1,1 1 1,-1-1-1,0 1 1,1 1-1,-1-1 1,0 1-1,0-1 1,-1 1-1,1 1 1,-1-1-1,1 1 1,-1 0-1,0-1 1,-1 2-1,1-1 1,-1 0-1,1 1 1,-1 0-1,-1 0 0,1 0 1,-1 0-1,1 0 1,-2 0-1,3 10 1,-2 13-531,-2-27 202,0-1 0,0 1 0,0 0 0,-1 0 0,1-1-1,0 1 1,0 0 0,-1 0 0,1-1 0,0 1 0,-1 0 0,1-1 0,-1 1 0,1-1 0,-1 1-1,1 0 1,-1-1 0,1 1 0,-1-1 0,0 1 0,-1 0 0,-21 5-9129</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">0 185 7587,'0'0'8922,"6"-28"-7676,5 14-1232,0 0 1,0 1 0,1 0-1,1 0 1,0 1 0,1 1 0,0 0-1,1 1 1,0 1 0,0 0-1,33-13 1,-45 20-17,15-2 9,-16 4-63,3 320-139,-5-317 176,1 0-1,-1 0 0,1 0 1,-1 0-1,1 1 0,0-1 0,0 0 1,1-1-1,-1 1 0,1 0 0,-1 0 1,1 0-1,0-1 0,0 1 0,0-1 1,0 0-1,1 1 0,-1-1 1,0 0-1,1 0 0,0-1 0,-1 1 1,1-1-1,0 1 0,0-1 0,0 0 1,0 0-1,0 0 0,0 0 1,0 0-1,0-1 0,1 1 0,-1-1 1,0 0-1,0 0 0,0 0 0,1-1 1,-1 1-1,0-1 0,0 0 1,0 0-1,4-1 0,-6 2 15,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 0 1,1 0-1,-1 0 0,0 0 0,1 1 0,-1-1 0,1 0 0,-1 0 0,1 1 0,-1-1 0,0 0 0,1 0 1,-1 1-1,1-1 0,-1 0 0,0 1 0,1-1 0,-1 1 0,0-1 0,0 0 0,1 1 0,-1-1 0,0 1 1,0-1-1,0 1 0,0-1 0,1 1 0,-1-1 0,0 1 0,0-1 0,0 1 0,0-1 0,0 1 0,0-1 1,0 1-1,-1 0 0,1 28-110,0-22 132,-1 11-19,0-1 1,-1 0-1,0 0 0,-2 0 0,0 0 1,-11 28-1,12-38 8,-1 1-1,1-1 1,-1 1 0,0-1 0,-1 0-1,1-1 1,-1 1 0,-1-1 0,1 0-1,-1 0 1,0-1 0,-1 0 0,1 0-1,-1 0 1,0-1 0,-11 6 0,17-10 4,0 1 0,0-1 1,0 1-1,-1-1 0,1 1 1,0-1-1,0 0 0,0 1 1,-1-1-1,1 0 0,0 0 1,0 0-1,0 0 0,-1 0 1,1 0-1,0 0 0,0-1 1,-1 1-1,1 0 0,0-1 1,0 1-1,0-1 0,0 1 1,-2-1-1,3 0-141,-1-1-1,0 1 1,1 0 0,-1 0-1,1 0 1,0 0 0,-1 0 0,1-1-1,0 1 1,0 0 0,-1 0-1,1-1 1,0 1 0,0 0-1,0 0 1,1 0 0,-1-1-1,1-1 1,0-3-769,1 0-1,-1 0 1,1 1-1,1-1 1,-1 1-1,1-1 1,0 1-1,4-5 1,19-17-4070</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -2301,7 +2713,7 @@
           <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
         </inkml:channelProperties>
       </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2025-01-04T15:33:36.167"/>
+      <inkml:timestamp xml:id="ts0" timeString="2025-02-22T15:38:30.444"/>
     </inkml:context>
     <inkml:brush xml:id="br0">
       <inkml:brushProperty name="width" value="0.035" units="cm"/>
@@ -2309,10 +2721,14 @@
       <inkml:brushProperty name="color" value="#004F8B"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">175 35 2113,'0'0'11621,"-2"1"-13389,-10 5-7696,5-3 8971,1-1-668</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1502.11">198 5 992,'-5'-4'13940,"0"6"-14762,-3 8 887,-1 1 0,1 0 0,1 0 0,0 1 0,1 0 0,0 0 0,1 1 0,-5 15 0,5-12 99,-2 0-1,0-1 1,0 1 0,-14 18 0,-54 65 641,76-107-8368,8-12 2713</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2019.92">32 87 1121,'0'0'6680,"-1"0"-6481,1 0-1,0-1 1,0 1 0,0 0-1,-1-1 1,1 1 0,0 0 0,0-1-1,0 1 1,0 0 0,0-1-1,0 1 1,0-1 0,0 1 0,0 0-1,0-1 1,0 1 0,0 0-1,0-1 1,0 1 0,0-1 0,1 1-1,-1 0 1,0-1 0,0 1-1,0 0 1,0-1 0,1 1 0,-1 0-1,0-1 1,7 5-168,-1 0 0,0 1 0,0-1-1,-1 1 1,1 1 0,-1-1 0,0 1 0,-1 0 0,1 0 0,3 7-1,15 17 50,47 56 195,-66-83-259,-3-3 162</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3688.59">290 26 1585,'0'0'4319,"3"11"3777,10 40-7239,-8 396 2342,6-394-3073,-10-43 365,-14-30-267,0 6-250,9 11 38,0-1 0,0 1 1,1-1-1,-1 0 1,1 0-1,0 0 0,0 0 1,1 0-1,-1-1 1,1 1-1,-3-8 0,5 11 4,-5-7-97,3 9-85,6 13 208,1-5-42,0 0 0,0 0 0,1-1-1,0 0 1,15 15 0,10 14 14,-30-35 6,0 0-1,0 0 0,1-1 0,-1 1 0,0 0 1,1-1-1,-1 1 0,1-1 0,0 0 1,0 0-1,-1 0 0,1 1 0,4 0 1,-5-2-8,0 0 0,0 0 0,0 1 0,0-1 1,0 0-1,0-1 0,-1 1 0,1 0 0,0 0 0,0 0 1,0-1-1,0 1 0,0 0 0,0-1 0,0 1 0,0-1 1,-1 1-1,1-1 0,0 1 0,0-1 0,1-1 0,3-4 34,-1 0 0,1-1-1,-1 0 1,0 0-1,-1 0 1,4-8-1,5-12-90,-12 27 45,5-8-3,0-1 0,0 0-1,-1 0 1,-1 0 0,0-1-1,0 1 1,2-16 0,-5 24 11,-22 15-7036,18-9 5196,-13 7-4558</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">149 234 4322,'0'0'11797,"0"-9"-10935,-1-30-294,1 37-525,-1 0 0,1 0-1,-1 0 1,0 0-1,1 0 1,-1 0 0,0 0-1,-1 1 1,1-1 0,0 0-1,0 0 1,-1 1-1,1-1 1,-1 1 0,1 0-1,-1-1 1,0 1-1,1 0 1,-1 0 0,0 0-1,0 0 1,0 0-1,0 0 1,-3 0 0,-1-1-29,0 0 0,0 0 0,-1 1 0,1 0 0,-12 0 0,16 1-23,-1 0 0,1 1 0,-1-1 0,1 1 0,-1 0 0,1 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 1 0,0-1 0,0 1 0,0 0 0,0-1 0,1 1 0,-1 0-1,0 0 1,1 0 0,-1 0 0,1 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 1 0,0-1 0,1 1 0,-1-1 0,1 1 0,-1 2 0,-1 13 2,-1 1 1,2-1-1,1 23 1,0-27 12,0 61-306,0 55-662,0-87-3258,0 0-3598,0-39 3496</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="375.08">1 526 6419,'0'0'11997,"3"-13"-11503,-3 10-476,1-2-14,-1 1 0,1 0 0,0-1 0,0 1 0,0 0 0,1 0 0,0 0 1,-1 0-1,1 0 0,1 0 0,-1 0 0,0 1 0,1-1 0,0 1 0,0 0 0,0-1 0,0 1 0,1 1 0,-1-1 0,1 0 1,-1 1-1,1 0 0,0 0 0,0 0 0,0 0 0,5-1 0,24-4-849,1 1 1,49-3-1,-7 6-4407,1 3-3736,-75 0 8696,2-4 1744,-2-12 11784,-8 30-13070,-1 9-179,0 1 0,2-1 0,1 1 0,-2 31 0,3 8-7405,3-57 588</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="525.37">506 203 8836,'0'0'8500,"0"-21"-13350,0 45 1952,6 4-4817</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="916.46">641 510 6067,'0'0'10300,"10"-14"-9734,-4 5-516,20-27 59,-2-1 1,-2-2 0,28-64-1,-41 61-176,-1 0 0,-2-1 0,-2 0 0,-2-57-1,-2 98 60,-11 183 408,0 6 531,11-162-889,2 50 101,-2-70-154,1 0 0,0 1 0,1-1 0,-1 0-1,1 0 1,0 0 0,0 0 0,0-1 0,1 1-1,-1 0 1,6 5 0,-6-8-210,1 0-1,-1-1 1,1 1-1,0 0 1,0-1-1,0 0 1,0 0-1,0 0 1,0 0 0,0 0-1,0-1 1,0 1-1,0-1 1,5 0-1,-1 1-681,-1-1-1,0-1 0,0 1 1,1-1-1,-1 0 1,9-3-1,17-16-5363</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1164.67">1087 15 6339,'0'0'9364,"0"104"-8467,-5-48-289,-1-1-112,1 0-304,0-2-64,5-1-64,0-6-64,0-6-32,0-9-1088,0-10-1521,0-9-1617</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1305.01">996 384 5603,'0'0'11717,"0"-10"-11973,21 10-352,12 0-1281,-1 0-1377,0 0-2945</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1613.97">1179 288 6067,'0'0'10514,"27"0"-8796,-22 0-1793,82-5 756,-45-7-4533,-39 10 2718,0 1 1,0-1-1,0 0 0,-1 0 1,1 0-1,0 0 0,-1 0 1,0-1-1,4-4 0,-4 0-2502</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2155.03">1378 209 2769,'0'0'11480,"-5"-6"-10149,2 1-1107,-1 1-1,1 0 0,-1 1 0,0-1 0,0 1 1,-1 0-1,-8-6 0,12 9-197,0-1 0,-1 0-1,1 0 1,0 1 0,-1-1 0,1 1-1,0-1 1,-1 1 0,1 0 0,-1 0-1,1-1 1,-1 1 0,1 0 0,-1 0-1,1 0 1,-1 1 0,1-1 0,-1 0-1,1 0 1,0 1 0,-1-1 0,1 1-1,-1-1 1,1 1 0,0 0 0,0 0-1,-1-1 1,1 1 0,0 0 0,0 0-1,0 0 1,0 0 0,0 0-1,0 1 1,0-1 0,0 0 0,0 0-1,1 1 1,-1-1 0,0 2 0,-5 13 13,1 0 0,1 0 0,0 0 0,1 0 0,1 1 0,0-1 0,1 1 0,1-1 0,1 1 0,3 21 0,-3-36-61,-1 1 0,1-1 0,0 0 0,0 1 0,0-1 0,0 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,0 0 0,-1 0 0,1-1 0,0 1 0,0-1 0,0 1 0,0-1 0,0 0 1,1 0-1,-1 0 0,0 0 0,1 0 0,-1 0 0,5 0 0,-4 0-92,0 0-1,0-1 1,0 1 0,0-1 0,0 0 0,0 0 0,0 0 0,0 0 0,0-1 0,0 1 0,0-1 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,-1-1 0,1 0 0,3-2 0,3-7-55,-1 1 0,-1-1 1,0 0-1,6-13 0,13-20 1034,-25 43-832,-1 1 0,1-1 1,-1 0-1,1 1 0,0-1 0,-1 0 0,1 1 1,0-1-1,-1 1 0,1-1 0,0 1 0,0 0 1,-1-1-1,1 1 0,0 0 0,0-1 0,0 1 1,0 0-1,0 0 0,-1 0 0,1 0 0,0 0 1,0 0-1,0 0 0,0 0 0,0 0 0,0 0 1,-1 0-1,1 0 0,0 1 0,0-1 0,0 0 1,-1 1-1,1-1 0,0 1 0,0-1 1,-1 1-1,1-1 0,0 1 0,-1-1 0,1 1 1,0 0-1,-1-1 0,1 1 0,0 1 0,23 33-93,-17-22 175,-1 0 0,-1 1-1,0 0 1,-1 0 0,0 0 0,-1 0-1,-1 1 1,0-1 0,-1 1-1,-2 29 1,-1-89 2735,1 29-2809,0 1 0,1-1 0,0 0 0,1 1 0,1-1 0,1 1 0,0-1 0,1 1 0,6-16 0,2 3-218,2 1-1,0 1 0,2 0 0,1 1 1,31-35-1,-38 50-381,0 0 0,0 1 0,1 0 0,1 1 0,22-13-1,-24 16-472,-1 1 0,1 1 0,-1-1 0,1 2 0,0-1 0,0 1-1,0 1 1,20-1 0,-10 2-6065</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -2332,7 +2748,7 @@
           <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
         </inkml:channelProperties>
       </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2025-01-04T15:33:43.727"/>
+      <inkml:timestamp xml:id="ts0" timeString="2025-02-22T15:40:15.656"/>
     </inkml:context>
     <inkml:brush xml:id="br0">
       <inkml:brushProperty name="width" value="0.035" units="cm"/>
@@ -2340,10 +2756,7 @@
       <inkml:brushProperty name="color" value="#004F8B"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">166 3 1617,'-2'0'13696,"-17"13"-13647,-57 79 207,17-19-136,53-67 780,2-3-3379</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="118.39">166 3 2593</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="258.31">166 3 2593,'-134'30'1958,"104"-27"2301,40-3-143,17 44-4021,10 16 956,-35-58-1354,0 1 1,0-1-1,0 0 1,0 0-1,0 0 1,1 0-1,-1 0 1,1-1-1,0 1 1,-1-1-1,1 1 1,0-1-1,0 0 0,0 0 1,0 0-1,0-1 1,0 1-1,4 0 1,9-1-4324</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1327.43">268 5 5090,'0'0'7777,"0"-4"-4154,-2 100-2431,5 117-55,-2-201-1089,13 194 387,-13-181-289,2 0 0,9 48 0,-13-66-132,1-6-11,0 1 1,0-1-1,-1 0 0,1 0 0,0 0 0,0 0 0,0 1 0,0-1 0,1 0 0,-1 0 0,0 0 0,0 0 1,1 0-1,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,0 0 0,0 1 0,1-3 671,-7-11-551,-7-13-173,-7-4 65,-30-34 0,42 51-75,6 10-191,2 10 148,4 3 108,0 0 0,1-1-1,0 1 1,0-1 0,1-1-1,0 1 1,9 8 0,12 17-21,-28-35 20,0 1 1,0 0 0,1-1 0,-1 1 0,0-1 0,1 1-1,-1 0 1,0-1 0,1 1 0,-1-1 0,1 1-1,-1-1 1,1 1 0,0-1 0,-1 1 0,1-1 0,-1 0-1,1 1 1,0-1 0,-1 0 0,1 1 0,0-1 0,-1 0-1,1 0 1,0 0 0,-1 0 0,1 1 0,0-1-1,0 0 1,-1 0 0,1 0 0,0-1 0,-1 1 0,1 0-1,0 0 1,0 0 0,-1 0 0,1-1 0,0 1 0,-1 0-1,1-1 1,-1 1 0,1 0 0,0-1 0,-1 1-1,1-1 1,-1 1 0,1-1 0,-1 1 0,1-1 0,-1 0-1,0 1 1,1-1 0,-1 1 0,0-1 0,1 0 0,-1 0-1,16-43 42,-14 39-43,1-5-88,4-8-292,-2 0 0,0 0 0,-1 0 1,3-34-1</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">60 1 288,'0'0'16031,"-1"13"-16033,-22 76 69,15-61-15,-9 56 0,12-18 746,4 68 1,2-64-454,-1-69 631,-1-26-760,-3-87-5899,4 92 3312,0-29-5435</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -2363,7 +2776,7 @@
           <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
         </inkml:channelProperties>
       </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2025-01-04T15:33:50.382"/>
+      <inkml:timestamp xml:id="ts0" timeString="2025-02-22T15:40:16.720"/>
     </inkml:context>
     <inkml:brush xml:id="br0">
       <inkml:brushProperty name="width" value="0.035" units="cm"/>
@@ -2371,8 +2784,7 @@
       <inkml:brushProperty name="color" value="#004F8B"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">0 4 1617,'0'0'8524,"0"-4"-7636,0 7-294,1 68 1399,14 108 1,-3-126-1455,-6-31-373,-1 1 0,-1 0 0,2 34 0,-5-46 1081,3-4-3877,-3-7 2378,-1-1-1,1 1 1,0-1-1,-1 1 1,1-1-1,-1 1 0,1-1 1,-1 1-1,1-1 1,-1 1-1,0-1 1,1 1-1,-1-1 0,1 0 1,-1 1-1,0-1 1,0 0-1,1 1 1,-1-1-1,0 0 0,0 1 1,0-1-1,0 0 1,0 0-1,2-23-3693</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1053.6">74 50 2193,'0'0'5165,"17"1"-3281,18 6-1017,0-2 0,0-2 0,0-1 0,70-6 0,-50 2-392,141-6 228,113-2-398,-51 10 1395,-258 301-292,-43-301-36,-213-1-1317,-272 3-1989,491 1 1775,-58 12-1,63-8 201,0-2-1,-45 1 1,75-6 79,-3 27-10946,5-20 6421</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">19 104 7652,'0'0'9804,"0"-1"-9705,-1 1 1,1-1-1,0 1 0,0-1 1,0 1-1,0-1 0,-1 1 0,1-1 1,0 1-1,0-1 0,0 1 1,0-1-1,0 1 0,0-1 1,0 1-1,0-1 0,1 1 0,-1-1 1,0 1-1,0-1 0,0 1 1,0 0-1,1-1 0,-1 1 1,0-1-1,1 0 0,9-7-89,0 0-1,1 0 1,1 1-1,-1 0 1,1 1-1,0 0 1,0 1-1,16-4 1,9-6 0,-33 14-15,-1-1-1,1 0 0,0 1 0,0 0 1,1 0-1,-1 0 0,0 0 0,0 0 1,0 1-1,0 0 0,1 0 0,-1 0 1,0 1-1,0-1 0,1 1 0,-1 0 1,5 2-1,-7-1 1,1-1 1,0 1-1,0 0 0,-1 1 1,1-1-1,-1 0 0,0 1 1,0 0-1,0-1 0,0 1 1,0 0-1,-1 0 0,1 0 1,-1 0-1,1 0 0,-1 0 1,0 0-1,-1 1 0,1-1 1,0 0-1,-1 1 0,0 3 0,2 3 1,-1 1 0,0-1 0,0 0-1,-1 1 1,-1-1 0,1 1-1,-2-1 1,0 0 0,0 0-1,0 0 1,-2 0 0,1 0-1,-1 0 1,0-1 0,-1 1-1,0-1 1,-1-1 0,0 1-1,0-1 1,-10 11 0,0-3 7,0 0-1,-2-1 1,-31 23 0,40-32-19,1-1 1,-1 0 0,0-1-1,0 0 1,0 0 0,-1-1-1,0 0 1,1-1-1,-1 0 1,0-1 0,-10 1-1,19-3-9,0-1 0,0 1 0,1-1 0,-1 1 0,0-1 0,1 1 0,-1-1 0,1 0 0,0 1 0,-1-1 0,1 0 0,0 1 0,0-1 0,0 0 0,0 1 0,0-1-1,1-2 1,-1 0-26,0 1 0,0 0-1,0-1 1,1 1-1,-1 0 1,1 0 0,0-1-1,0 1 1,0 0-1,2-3 1,1 3 23,1 0 1,-1 0-1,1 1 0,0-1 1,0 1-1,0 0 0,0 1 1,0-1-1,0 1 0,1 0 1,-1 0-1,0 1 0,9-1 1,74 5-104,-76-2 121,1 1 0,-1 0 0,1 1 0,-1 1-1,16 7 1,-18-6 18,0-2 0,1 1 0,0-2 0,0 1 0,0-1 0,0-1 0,22 2 0,-26-4 70,-1 0 1,1-1-1,0 0 1,0 0-1,-1-1 1,1 0-1,-1 0 1,1 0-1,6-5 1,-10 6-172,-1-1 1,0 1 0,1-1-1,-1 0 1,0 0 0,0 1-1,0-2 1,-1 1 0,1 0 0,0 0-1,1-4 1,-2 4-347,0 0 1,-1 0-1,1 0 1,0 0-1,-1-1 1,0 1-1,1 0 1,-1 0-1,0-1 1,0 1-1,0 0 1,-1-1-1,1 1 1,0 0-1,-2-4 1,-2-3-7345</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -2392,7 +2804,7 @@
           <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
         </inkml:channelProperties>
       </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2025-01-04T15:33:48.279"/>
+      <inkml:timestamp xml:id="ts0" timeString="2025-02-22T15:40:36.342"/>
     </inkml:context>
     <inkml:brush xml:id="br0">
       <inkml:brushProperty name="width" value="0.035" units="cm"/>
@@ -2400,8 +2812,63 @@
       <inkml:brushProperty name="color" value="#004F8B"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">0 441 6995,'0'0'8738,"0"0"-8712,0 0 1,0 0-1,0 0 1,0 1 0,0-1-1,1 0 1,-1 0 0,0 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0-1,0 0 1,0 1 0,0-1-1,0 0 1,1 0 0,-1 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0-1,0 0 1,0 0 0,1 0-1,-1 0 1,0 0 0,0 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0-1,1 0 1,-1 0 0,0 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0 0,0 0-1,1 0 1,-1-1 0,0 1-1,0 0 1,0 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0-1 0,0 1-1,1 0 1,-1 0-1,0 0 1,0 0 0,0 0-1,0-1 1,47 118 181,-39-100-292,4 5 426,-11-21-330,0-1-1,0 0 0,0 0 1,0 0-1,0 0 1,0-1-1,0 1 0,0 0 1,0 0-1,0 0 1,0-1-1,0 1 0,0-1 1,0 1-1,-1-1 1,1 1-1,0-1 0,0 1 1,0-1-1,-1 1 1,1-1-1,0 0 0,-1 0 1,1 1-1,-1-1 1,1 0-1,-1 0 1,1 0-1,0-1 0,122-163 414,-118 152-9117</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1055.18">404 500 1425,'0'0'14673,"-12"-31"-12376,8 24-2226,0 0 0,1 0 0,0 0-1,0 0 1,1-1 0,0 1 0,-2-12 0,-7-23 109,-5-35-79,10 54-92,2 0-1,-3-44 0,-5-22 29,9 75-28,1 6 14,0-1 0,1 0 1,0 1-1,0-18 0,1 26-28,0 0 0,0-1-1,-1 1 1,1 0 0,0-1-1,-1 1 1,1 0 0,0-1-1,-1 1 1,1 0 0,0 0 0,-1-1-1,1 1 1,-1 0 0,1 0-1,0 0 1,-1 0 0,1 0-1,-1 0 1,1-1 0,0 1-1,-1 0 1,1 0 0,-1 0-1,1 0 1,-1 0 0,1 1 0,-1-1-1,1 0 1,0 0 0,-1 0-1,1 0 1,-1 0 0,1 1-1,0-1 1,-1 0 0,0 1-1,-15 5-139,-48 98 159,148-206-110,-84 102 84,1 0 1,-1-1 0,0 1-1,1-1 1,-1 1-1,1 0 1,-1-1 0,1 1-1,-1 0 1,1-1-1,-1 1 1,1 0 0,0 0-1,-1-1 1,1 1-1,-1 0 1,1 0 0,0 0-1,-1 0 1,1 0-1,-1 0 1,1 0 0,0 0-1,-1 0 1,1 0 0,-1 0-1,1 1 1,0-1-1,0 0 1,17 16-75,7 25 111,-16-25 361,0-1-1548,-6-6-8141</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">28 31 3265,'0'0'6243,"0"-28"2487,0 25-7746,3 105-988,26 161 0,-3-62 95,-14-118 5,-10-78 161,-5-17 9,-33-46-277,-8-18 14,43 73 1,0 1-1,1 0 0,-1 1 0,0-1 0,0 0 0,1 1 0,-1-1 0,0 1 0,0-1 0,0 1 0,-1 0 0,1-1 0,-2-1-1,2 3-20,3 18-526,-1-10 546,1-1 0,1 0 0,-1-1 0,1 1 0,0 0 1,1-1-1,0 1 0,0-1 0,0 0 0,1-1 0,-1 1 1,2-1-1,-1 0 0,0 0 0,1 0 0,0-1 0,0 0 1,0 0-1,1 0 0,-1-1 0,1 0 0,0-1 1,0 1-1,0-1 0,0 0 0,14 1 0,-17-3 9,1-1-1,-1 1 1,0-1-1,0 0 1,-1 0-1,1 0 1,0-1-1,0 1 1,0-1-1,-1 0 1,1 0-1,-1-1 1,0 1-1,0-1 1,1 1 0,-2-1-1,1 0 1,0 0-1,0 0 1,-1 0-1,0-1 1,0 1-1,3-6 1,4-4 11,-1 0 30,-1 0 0,0 0 1,9-27-1,-12 29-331,0-1 0,1 1 0,1 0 0,0 0 0,13-18 0,-10 28-5366</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink18.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2025-02-22T15:40:40.931"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.035" units="cm"/>
+      <inkml:brushProperty name="height" value="0.035" units="cm"/>
+      <inkml:brushProperty name="color" value="#004F8B"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">183 35 4130,'0'0'10410,"-3"-5"-9330,0 2-761,2 2-195,0 0 0,-1-1 0,1 1 1,0 0-1,0-1 0,0 1 0,0-1 0,0 1 0,0-1 0,0 0 0,0 1 0,1-1 0,-1 0 0,0-3 1446,0 5-1394,-3 0-101,3 2-95,0 0 1,0-1-1,0 1 1,0 0-1,0 0 1,0 0-1,0 0 1,1 1-1,-1-1 1,1 0-1,-1 0 1,1 0-1,0 0 1,0 5-1,-1 3-23,-8 59 56,4 0 0,6 118 0,1-69-4,-3-36 106,2 82 274,-34-188-160,20 13-216,1-1-1,1-1 1,0 1-1,1-2 1,0 1-1,1-1 1,0-1-1,-6-16 1,14 25-16,1 5-29,0 9-272,1 4 294,1 0 1,0-1 0,1 1-1,0 0 1,1-1 0,1 0-1,0 0 1,0 0 0,1 0-1,0-1 1,1 0 0,0 0-1,0-1 1,1 0 0,1 0-1,-1-1 1,1 0 0,1 0-1,12 7 1,-20-14 11,0 0 1,0 0-1,0 0 1,0 0 0,0-1-1,0 1 1,0-1-1,0 1 1,0-1-1,0 0 1,1 0-1,-1 0 1,0 0-1,0 0 1,0-1-1,0 1 1,1-1-1,-1 1 1,0-1-1,0 0 1,0 1-1,0-1 1,2-2-1,-1 0 9,0 1 0,1-1 0,-1-1-1,-1 1 1,1 0 0,0-1 0,-1 1-1,0-1 1,0 0 0,0 0 0,1-4 0,4-12 27,-1 0 1,-1-1 0,4-34-1,-9 54-38,0-4-160,14-113-666,-11 78-2101,-2 1-3677,-1 33 433</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink19.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2025-02-22T15:40:44.380"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.035" units="cm"/>
+      <inkml:brushProperty name="height" value="0.035" units="cm"/>
+      <inkml:brushProperty name="color" value="#004F8B"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">169 47 3298,'0'0'8894,"-4"-8"-7621,-10-23-225,10 24-31,-12 61 669,6-13-1620,2 1 1,1 1-1,0 43 0,6 133 250,2-115-219,9 27-109,1 6 610,-13-143-588,0 1 0,-1-1-1,0 1 1,0 0-1,0 0 1,0 0 0,-1 1-1,0-1 1,-7-5-1,-4-8-3,1-2 1,0-1 0,-21-44 0,32 59-434,10 23 346,19 28 120,-17-37-41,0 0 1,0 0 0,0-1 0,15 8 0,-20-13 9,0 0 0,0 0 0,0-1 0,0 1 0,0-1 0,0 0 0,1 0 0,-1-1 0,0 1 0,0-1 0,1 0 0,-1 0 0,0 0 0,0-1 0,9-2 0,-11 2-2,1 0 0,-1-1 0,0 1 0,1-1 0,-1 1 0,0-1 0,0 0 0,0 0 0,0 0 0,0 0 0,-1-1 0,1 1 0,-1 0 0,1-1 0,-1 1 0,0-1 0,0 0 0,0 1 0,1-5 0,13-60 113,-13 51-110,1-7-2322,-1 0-1,-1-25 0,-1 42 1785</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -2421,7 +2888,7 @@
           <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
         </inkml:channelProperties>
       </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2025-01-04T15:29:51.452"/>
+      <inkml:timestamp xml:id="ts0" timeString="2025-02-22T15:36:33.136"/>
     </inkml:context>
     <inkml:brush xml:id="br0">
       <inkml:brushProperty name="width" value="0.035" units="cm"/>
@@ -2429,8 +2896,95 @@
       <inkml:brushProperty name="color" value="#004F8B"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">38 8 2001,'0'0'11330,"0"-7"-10583,0 19-216,1 21 173,-2 0 1,-1 0-1,-1 0 0,-13 52 1,3-34-1181,9-17-3786,7-25 228,10-5-2156</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="658.24">293 138 8308,'0'0'5234,"0"5"-4484,0 115 1208,3-119-1917,0 0 0,1 0 0,-1-1 0,0 1 0,1-1 0,-1 0 0,0 1 0,1-1 0,-1-1 0,7 0 0,-8 1-31,-1 0 1,1 0-1,0-1 0,0 1 0,-1 0 1,1-1-1,0 1 0,-1-1 0,1 0 1,0 0-1,-1 0 0,1 1 1,-1-1-1,1-1 0,-1 1 0,0 0 1,1 0-1,-1 0 0,0-1 0,0 1 1,0 0-1,0-1 0,0 1 0,0-1 1,-1 0-1,2-1 0,0-3 10,-1 0 0,0-1 0,0 1 0,-1 0 0,0-12 0,0 10-9,0 6-17,-1 1-1,1-1 0,-1 0 1,0 0-1,1 1 1,-1-1-1,0 0 1,0 1-1,0-1 1,0 1-1,0-1 0,-1 1 1,1 0-1,0-1 1,0 1-1,-1 0 1,1 0-1,-1 0 0,0 0 1,1 0-1,-1 0 1,1 0-1,-1 1 1,0-1-1,-3 0 0,-39-9-947,41 9 619,8 1-8,29 1-234,137-11-1533,-171 54 4786,-4-14-2020,3-25-614,0 0 1,0 0 0,0 0 0,1 0-1,0 0 1,0 0 0,0 0 0,1 0-1,-1 0 1,3 9 0,0-12-40,-1-1 0,0 1 0,1-1 1,-1 0-1,1 0 0,-1 0 0,1 0 0,0 0 0,-1-1 1,1 1-1,0-1 0,0 1 0,-1-1 0,1 0 0,0 0 1,0 0-1,-1-1 0,1 1 0,3-1 0,8 0-5,-4 1-23,0-1 0,-1 1-1,1-2 1,0 1-1,-1-1 1,0-1 0,1 0-1,-1 0 1,0-1 0,-1 0-1,1 0 1,-1-1 0,1 0-1,-1-1 1,-1 0 0,1 0-1,-1-1 1,0 1 0,6-9-1,-12 13 60,1-1 0,-1 1 0,0-1 0,1 1 0,-1-1 0,0 1 0,-1-1 0,1 0 0,0 1 0,-1-1 0,0 0 0,1 0 0,-1 0 0,0 1 0,0-1 0,-1 0 0,1 0 0,0 1 0,-1-1 0,0 0 0,0 1 0,0-1 0,0 0 0,0 1 0,0-1 0,-4-4 0,3 4-10,-1 0-1,0 0 0,-1 0 1,1 0-1,0 0 1,-1 1-1,0-1 0,1 1 1,-1 0-1,0 0 0,0 1 1,0-1-1,-1 1 0,1 0 1,0 0-1,-6-1 1,0 1-214,1 1 0,-1 0 0,0 0 1,1 1-1,-11 2 0,-23 12-4626,21-3-629</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">210 72 2465,'0'0'9420,"-3"-10"-8472,1-2-593,1 7-160,0 1 0,0-1-1,0 0 1,-1 1 0,1-1-1,-1 1 1,-5-9-1,7 13-147,0 0 0,0 0 0,0-1 0,0 1 0,0 0 0,0 0 0,0-1 0,0 1 0,-1 0 0,1 0 0,0 0 0,0 0 0,0-1 0,0 1 0,0 0-1,-1 0 1,1 0 0,0 0 0,0 0 0,0-1 0,-1 1 0,1 0 0,0 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 0-1,0 0 1,-1 0 0,1 0 0,0 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,-1 1 0,-5 10 295,-2 20-708,8-29 469,-15 89 90,-5 132-1,17 96 570,3-216-324,0-103 122,-3-2-550,0 0-1,0 0 0,1 0 1,-1-1-1,1 1 0,-1-1 1,1 0-1,0 0 0,0 1 0,0-2 1,-3-3-1,-1-3-1,-84-119 0,89 128 0,2 13-413,4 6 385,1 0 1,1 0-1,0-1 1,1 0-1,1 0 1,1-1-1,0 0 0,24 28 1,-33-43 21,1 1-1,-1 0 1,1-1 0,-1 1-1,1-1 1,0 0 0,-1 1-1,1-1 1,0 0 0,0 0 0,0 0-1,0 0 1,4 1 0,-6-2 1,1 0 1,0 0 0,0 0 0,0 0-1,0 0 1,0-1 0,0 1-1,0 0 1,0 0 0,0-1 0,0 1-1,0 0 1,0-1 0,-1 1 0,1-1-1,0 1 1,0-1 0,-1 1-1,1-1 1,0 0 0,1-1 0,2-4 27,-1 0 0,1 0 0,-1 0 0,0-1 0,-1 0 0,4-10 0,3-8 43,-8 22-89,6-11-58,0 0 0,-1-1-1,-1 0 1,0 0 0,-1 0-1,3-23 1</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink20.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2025-02-22T15:40:45.618"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.035" units="cm"/>
+      <inkml:brushProperty name="height" value="0.035" units="cm"/>
+      <inkml:brushProperty name="color" value="#004F8B"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">270 711 7331,'0'0'8135,"-8"-14"-7247,-3-4-622,4 6-8,0 0 1,1 0-1,-8-21 0,7 9-129,1 0 0,1 0 0,1-1-1,2 1 1,0-1 0,2-31 0,0 18-136,-7-53 1,5 67-1,-2-19 11,4 41-6,0 0 0,0 1-1,-1-1 1,1 0 0,-1 0-1,0 1 1,1-1-1,-1 0 1,0 1 0,0-1-1,0 1 1,0-1 0,0 1-1,0-1 1,0 1-1,-2-2 1,2 3-46,-1 1 24,0 0 1,0 0-1,0 0 1,1 0-1,-1 0 0,0 1 1,1-1-1,-1 1 1,1-1-1,0 1 0,-1 0 1,1-1-1,0 1 0,0 0 1,0 0-1,0 0 1,0 0-1,1 0 0,-1 0 1,1 0-1,-1 2 0,-4 9-21,5-13 45,-11 22-88,-26 40 0,34-57 71,0-1 0,-1 1 0,1-1 0,-1 0 0,0 0-1,0 0 1,-1 0 0,1-1 0,-1 0 0,1 0 0,-1 0 0,0 0 0,-1-1-1,-9 4 1,14-6 4,1-1-1,0 1 0,-1 0 1,1 0-1,-1 0 0,1-1 1,0 1-1,-1 0 1,1 0-1,0-1 0,-1 1 1,1 0-1,0-1 0,-1 1 1,1-1-1,0 1 0,0 0 1,-1-1-1,1 1 1,0-1-1,0 1 0,0 0 1,0-1-1,0 1 0,0-1 1,-1 1-1,1-1 0,0 1 1,0-1-1,0 1 0,0-1 1,1 1-1,-1 0 1,0-1-1,0 1 0,0-1 1,0 1-1,0-1 0,1 1 1,-1 0-1,0-1 0,0 1 1,1-1-1,-1 1 1,1-1-1,8-25-330,-3 14 195,22-40 43,-27 50 91,0 0 0,0 0 1,1 0-1,-1 0 0,1 1 1,0-1-1,0 0 0,-1 1 0,1-1 1,0 1-1,0 0 0,0-1 1,1 1-1,-1 0 0,0 0 0,0 1 1,1-1-1,-1 0 0,4 0 1,-5 1 10,0 1 0,0-1 0,0 0 0,0 0 0,0 1 0,-1-1 0,1 1 0,0-1 0,0 1 0,-1-1 0,1 1-1,0 0 1,-1-1 0,1 1 0,-1 0 0,1-1 0,-1 1 0,1 0 0,-1 0 0,1-1 0,-1 1 0,0 0 0,1 0 0,-1 1 0,10 31-47,-3-8 16,-6-22-113,0 0-1,1 0 1,0 0 0,0-1-1,0 1 1,0 0 0,0-1-1,4 5 1,-4-6-312,0 0-1,-1 0 1,1 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0-1,0-1 1,0 1-1,0-1 1,0 0 0,0 1-1,3-1 1,12 0-6277</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="268.11">349 41 3618,'0'0'9303,"0"-5"-8364,0-4-667,0 14-65,0 32 93,0 58 436,-3 65 598,1-81-2423,1 1-6354</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="789.59">308 87 2609,'0'0'8695,"7"-13"-8324,-3 6-342,-3 3-19,1 1 0,0-1 0,0 0 0,0 1 0,0-1 0,0 1 0,1 0 0,0 0 0,-1 0-1,1 0 1,0 0 0,1 0 0,-1 1 0,0 0 0,1-1 0,-1 1 0,1 1 0,0-1 0,-1 0 0,1 1 0,0 0-1,0 0 1,0 0 0,6-1 0,315-2 130,-194 5 1308,-130 0-1430,1-1 0,0 1 0,-1 0 0,1 0 0,-1-1 0,1 1 0,-1 0 0,1 0 0,-1 0-1,0 0 1,1 1 0,-1-1 0,0 0 0,0 1 0,0-1 0,0 0 0,0 1 0,0-1 0,0 1 0,-1 0 0,1-1 0,0 3 0,14 40-26,-1 16 21,-3 0-1,-2 1 1,1 88 0,-11-148-9,1 1 1,-1-1-1,0 1 1,0-1 0,1 1-1,-1-1 1,0 0-1,0 0 1,0 1-1,0-1 1,-1 0-1,1 0 1,0 0 0,0 0-1,-1 0 1,1-1-1,-1 1 1,1 0-1,0 0 1,-1-1-1,1 1 1,-1-1 0,1 0-1,-1 1 1,0-1-1,-2 0 1,-50 7 298,50-6-289,-294 2 1864,225-5-4519,-1 2-3919,68 0 471</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink21.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2025-02-22T15:43:34.228"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.035" units="cm"/>
+      <inkml:brushProperty name="height" value="0.035" units="cm"/>
+      <inkml:brushProperty name="color" value="#004F8B"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">19 129 6499,'0'0'10074,"-3"-7"-8943,0 1-724,2 5-221,-1-1 0,1 0 0,0 0 0,0 0 0,0 0 0,1-1 0,-1 1 0,0 0 0,1 0 0,0 0 0,-1 0 0,1-4 1100,0 9-1524,-1 45 127,0-18 105,1 0 0,1 0-1,11 58 1,-2-32-10,3-149 336,-10 64-407,1 1 0,2 0-1,1 0 1,0 0 0,3 1 0,15-33-1,-25 59 72,0 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1 1-1,-1-1 1,1 0 0,0 0 0,-1 1 0,1-1 0,0 0 0,0 1 0,0-1 0,0 1 0,-1-1 0,1 1-1,0-1 1,0 1 0,0-1 0,0 1 0,0 0 0,0 0 0,0 0 0,0-1 0,0 1 0,0 0 0,2 0-1,-1 1 3,0 0 0,0 0-1,-1 0 1,1 1-1,0-1 1,0 0 0,0 1-1,-1-1 1,1 1-1,-1 0 1,1-1 0,-1 1-1,2 2 1,5 11 2,1 0 0,10 27 0,-17-37 1,12 34 11,-10-26-13,1 0 0,0 0-1,1 0 1,7 12 0,-13-25-9,1 1 0,-1-1 0,0 1 0,1-1 0,-1 1 1,1-1-1,-1 0 0,1 1 0,-1-1 0,0 0 0,1 1 1,-1-1-1,1 0 0,-1 0 0,1 1 0,-1-1 1,1 0-1,0 0 0,-1 0 0,1 0 0,-1 0 0,1 0 1,-1 0-1,1 0 0,-1 0 0,1 0 0,0 0 0,-1 0 1,1 0-1,-1 0 0,1-1 0,-1 1 0,1 0 0,-1 0 1,1-1-1,-1 1 0,1 0 0,-1 0 0,1-1 1,-1 1-1,0-1 0,1 1 0,-1 0 0,1-2 0,14-19 33,-14 21-21,68-134 362,-68 135-357,0 0 1,0 0-1,1-1 0,-1 1 1,0 0-1,0 0 0,0 0 1,0 0-1,0 1 0,-1-1 1,1 0-1,0 0 1,-1 0-1,1 1 0,0-1 1,-1 0-1,1 3 0,15 32 49,-12-24-33,0-1 0,0 0 0,1 0 0,0 0 1,11 15-1,-13-23-273,-1 0 0,1 0 0,0 0 0,0 0 0,0-1 0,0 1 0,0-1 0,0 0 0,1 0 0,-1 0 0,1 0 0,0 0 0,-1-1 0,1 0 0,0 0 0,0 0 0,0 0 0,0-1 0,0 1 0,5-1 0,-2 0-151,1 0-1,-1 0 1,0-1 0,1 0-1,-1 0 1,0-1-1,0 0 1,0 0-1,0 0 1,11-7-1,-13 6 193,-1-1 0,1 1-1,-1-1 1,0-1 0,0 1 0,0-1-1,-1 1 1,1-1 0,-1 0-1,0 0 1,-1 0 0,1-1-1,-1 1 1,2-7 0,0-3 1077,-1 0 1,0 0 0,-2-1-1,1 1 1,-2 0 0,-1-22-1,0-1 452,1 38-1253,0 0-1,0-1 0,0 1 0,0 0 0,0 0 1,0-1-1,0 1 0,0 0 0,0-1 0,0 1 0,0 0 1,0 0-1,0-1 0,0 1 0,0 0 0,-1 0 1,1-1-1,0 1 0,0 0 0,0 0 0,0-1 0,0 1 1,-1 0-1,1 0 0,0 0 0,0-1 0,-1 1 1,1 0-1,0 0 0,0 0 0,0 0 0,-1-1 0,1 1 1,0 0-1,-1 0 0,1 0 0,0 0 0,0 0 0,-1 0 1,1 0-1,0 0 0,0 0 0,-1 0 0,1 0 1,0 0-1,-1 0 0,1 0 0,0 0 0,0 0 0,-1 0 1,1 0-1,0 1 0,0-1 0,-1 0 0,1 0 1,0 0-1,0 0 0,-1 0 0,1 1 0,0-1 0,0 0 1,0 0-1,-1 1 0,-16 15 200,6 0-264,1 0-1,1 0 1,0 0-1,1 1 1,1 1-1,0-1 1,2 1-1,0 0 1,1 0 0,0 1-1,2-1 1,-1 37-1,3-55-133,5-3 181,0-1-1,0 1 1,0-1 0,0 0-1,0-1 1,-1 1 0,0-1-1,0 0 1,0 0-1,-1 0 1,0-1 0,0 1-1,2-7 1,5-11 104,12-45 0,-18 56-133,-3 7-8,-1 5-67,0 10-155,1 1 207,0-1 0,1 0 1,0 0-1,0 0 0,1 0 1,1 0-1,-1 0 0,2-1 1,-1 0-1,12 17 0,-15-25 9,1 1 1,0-1-1,0 0 0,0 1 1,0-1-1,0 0 0,0 0 0,0-1 1,0 1-1,0 0 0,1 0 0,-1-1 1,0 0-1,0 1 0,1-1 0,-1 0 1,0 0-1,0 0 0,1 0 0,-1-1 1,0 1-1,0-1 0,1 1 0,-1-1 1,0 0-1,3-1 0,-2 1-196,-1-1 1,0 1-1,0 0 0,0-1 1,0 1-1,-1-1 0,1 1 0,0-1 1,0 0-1,-1 0 0,0 1 0,1-1 1,-1-1-1,0 1 0,1-2 0,1-18-4344</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink22.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2025-02-22T15:43:49.099"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.035" units="cm"/>
+      <inkml:brushProperty name="height" value="0.035" units="cm"/>
+      <inkml:brushProperty name="color" value="#004F8B"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">237 910 416,'0'0'5443,"-4"-6"-4571,-7-8 48,-16-10 6302,25 23-6966,1-1 0,0 1-1,-1 0 1,1-1 0,0 1-1,0-1 1,0 0 0,0 1-1,0-1 1,0 0 0,1 0-1,-2-1 1,-12-53-440,10 38 457,-3-23-248,2 0 1,2 0-1,1 0 1,6-51-1,-2-1 48,-2 90-73,1-8-1,-1 0-1,-1-1 1,0 1 0,0-1-1,-1 1 1,0 0-1,-7-20 1,8 31-4,1-1 1,0 1-1,-1-1 0,1 1 0,0 0 0,-1-1 0,1 1 1,-1 0-1,1-1 0,-1 1 0,1 0 0,-1-1 1,1 1-1,-1 0 0,1 0 0,-1-1 0,1 1 1,-1 0-1,1 0 0,-1 0 0,1 0 0,-1 0 1,0 0-1,1 0 0,-1 0 0,1 0 0,-1 0 1,1 0-1,-1 0 0,1 1 0,-1-1 0,0 0 1,0 1-1,-16 8-208,0 8 190,1 0-1,-15 20 1,27-31 12,0 0 1,0-1 0,0 2-1,1-1 1,0 0-1,0 1 1,0-1 0,1 1-1,0 0 1,0 0 0,-1 11-1,3-17-29,17-23-320,79-83 208,-94 102 120,-1 1-1,1 0 1,0 0 0,-1 0-1,1 0 1,0 0 0,0 1-1,0-1 1,0 1 0,1-1-1,-1 1 1,0 0 0,1-1-1,3 0 1,-5 2 38,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 1 0,0-1 1,0 0-1,0 0 0,0 1 0,0-1 0,0 1 0,0-1 0,0 1 0,0-1 0,-1 1 0,1 0 0,0-1 0,0 1 0,-1 0 0,1 0 0,0-1 1,-1 1-1,1 0 0,0 2 0,4 7-462,-1 1-1,0 0 1,-1 0 0,0 1 0,1 14 0,4 11-5522,1-24 341</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="324.76">411 138 4530,'0'0'6704,"0"-4"-6418,0 67-49,-10 69 1,0-36-62,9-56-5464</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="917.82">393 83 6163,'0'0'5037,"6"-1"-4813,102-11-197,32-5-7,-122 13 21,0 0-1,0-1 1,0-1-1,-1-1 1,26-13 0,-35 14 930,-8 6-959,0 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0-1,0 0 1,0 1-1,0-1 1,0 0 0,0 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0 1 1,0-1 0,1 0-1,-1 0 1,0 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0 1-1,0-1 1,0 0-1,0 0 1,1 0 0,-1 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0 0 1,0 0 0,1 0-1,-1 0 1,0 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0 0 1,0 0 0,0 0-1,1 0 1,0 9-220,4 38 232,-3 0-1,-3 58 1,-1-25-2,2-75-21,0 0 0,0 1 0,-1-1 0,0 0 0,0 1 0,-1-1 0,1 0 0,-1 0 1,0 0-1,0-1 0,-1 1 0,1 0 0,-1-1 0,0 1 0,-6 5 0,3-4 21,-1 0 1,1-1-1,-1 1 1,0-2-1,-1 1 1,1-1 0,-1 0-1,-15 5 1,-1-1 98,0-2 0,-1-1 1,0-1-1,0-1 0,-42 0 0,-29-3-115,95 0-545,7-6-7075</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -2450,7 +3004,7 @@
           <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
         </inkml:channelProperties>
       </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2025-01-04T15:29:35.541"/>
+      <inkml:timestamp xml:id="ts0" timeString="2025-02-22T15:36:38.142"/>
     </inkml:context>
     <inkml:brush xml:id="br0">
       <inkml:brushProperty name="width" value="0.035" units="cm"/>
@@ -2458,38 +3012,7 @@
       <inkml:brushProperty name="color" value="#004F8B"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">421 238 1121,'0'0'8633,"0"-10"-3960</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="696.39">324 148 1777,'0'0'6168,"54"-3"-9996,-53 3 3933,-1 0 1,0 0 0,1 0 0,-1 1 0,0-1 0,1 0 0,-1 0 0,0 0 0,1 0 0,-1 0 0,1 0-1,-1 0 1,0 0 0,1-1 0,-1 1 0,0 0 0,1 0 0,-1 0 0,0 0 0,1 0 0,-1 0 0,0-1 0,1 1-1,-1 0 1,0 0 0,1-1 0,-1 1 0,0 0 0,0 0 0,1-1 0,-1 1 0,0 0 0,0-1 0,0 1-1,1 0 1,-1-1 0,0 1 0,0 0 0,0-1 0,0 1 0,0 0 0,0-1 0,0 1 0,0 0 0,0-1-1,0 1 1,0-1 0,0 1 0,0 0 0,0-1 0,0 1 0,0 0 0,0-1 0,0 1 0,0 0 0,-1-1 0,-8-10 4296,2 6-4869,2 3 492,1 1 0,-1-1 0,0 1-1,0 0 1,0 0 0,0 1 0,0 0 0,0-1 0,0 1-1,1 1 1,-1-1 0,0 1 0,0 0 0,0 0 0,0 1-1,1-1 1,-1 1 0,0 0 0,1 0 0,0 0-1,-1 1 1,1 0 0,0 0 0,0 0 0,1 0 0,-1 0-1,0 1 1,1 0 0,0-1 0,0 1 0,0 1 0,1-1-1,-1 0 1,1 1 0,0-1 0,0 1 0,1-1 0,-1 1-1,1 0 1,0 0 0,0 0 0,1 0 0,-1 0 0,1 0-1,0-1 1,1 1 0,-1 0 0,3 9 0,-3-12-48,1 1 1,0 0 0,0-1 0,0 0 0,0 1-1,1-1 1,-1 0 0,1 1 0,-1-1 0,1 0 0,0 0-1,0 0 1,-1-1 0,2 1 0,-1 0 0,0-1-1,0 1 1,0-1 0,3 2 0,3 0-134,1-1 1,-1 1-1,0-1 1,14 1-1,-14-2-4,-1 0-1,0 0 1,0 1-1,1 0 1,-1 0-1,8 5 1,-15-7 147,1 1 1,0-1 0,-1 1 0,1-1-1,-1 1 1,1-1 0,0 1 0,-1 0-1,1 0 1,-1-1 0,0 1 0,1 0 0,-1 0-1,0-1 1,1 1 0,-1 0 0,0 0-1,0 0 1,0-1 0,0 1 0,1 0-1,-1 0 1,0 0 0,-1 0 0,1 0 0,0-1-1,0 1 1,0 0 0,0 0 0,-1 0-1,1-1 1,0 1 0,-1 0 0,1 0-1,-1-1 1,1 1 0,-1 0 0,-20 25 10,-1-12 52,1 0 1,-2-2-1,0-1 0,0-1 1,-1 0-1,0-2 0,0-1 1,-32 5-1,38-11-866,8-4-3295,10-10 2238</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="943.13">470 136 2817,'0'0'12662,"5"40"-12342,-5 3 385,0 6-401,-5-3-192,-1-3-32,6-3-80,0-3 0,0-7-480,0-2-769,0-9-1664,0-7-1537,0-6-1569</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1315.04">445 431 5731,'0'0'6005,"9"-15"-5962,-2 2-38,-5 8-4,0 0 0,0 0-1,1 0 1,0 0 0,0 0-1,0 1 1,1 0 0,-1-1 0,1 1-1,0 1 1,0-1 0,1 0 0,-1 1-1,1 0 1,-1 0 0,1 1 0,10-5-1,7 0-4,-7 1-41,1 1-1,0 0 1,0 2-1,0 0 1,28-2-1,-45 28 289,-2-15-34,-1 1-1,1-1 1,-1 0 0,-1 0 0,0-1-1,0 1 1,-9 9 0,9-12-182,0 1 1,1 0-1,0-1 0,0 1 0,0 0 0,1 1 1,-1-1-1,2 1 0,-1-1 0,1 1 1,0 0-1,0 0 0,-1 12 0,4-18-54,-1 0-1,0 0 0,1 0 1,-1 0-1,1 0 0,-1 0 1,1 0-1,0 0 1,0 0-1,-1 0 0,1 0 1,0-1-1,0 1 0,0 0 1,0 0-1,0-1 0,0 1 1,0-1-1,0 1 1,0-1-1,0 1 0,0-1 1,0 1-1,0-1 0,0 0 1,0 0-1,1 0 0,-1 0 1,0 1-1,0-2 1,0 1-1,0 0 0,0 0 1,1 0-1,-1 0 0,0-1 1,1 0-1,48-11-674,-41 8 603,-1-1 1,1 0 0,-1-1 0,-1 1 0,1-1-1,8-9 1,-13 11 127,0 1 0,0 0 0,0-1-1,0 0 1,-1 0 0,0 0 0,0 0 0,0 0-1,0 0 1,0-1 0,-1 1 0,0 0-1,0-1 1,0 0 0,0-5 0,-1 8 12,0 1-1,-1 0 1,1 0 0,0 0 0,-1-1-1,1 1 1,-1 0 0,1 0 0,-1 0 0,0 0-1,1 0 1,-1 0 0,0 0 0,0 0-1,0 0 1,0 0 0,0 1 0,0-1 0,0 0-1,0 1 1,0-1 0,0 0 0,0 1 0,0-1-1,0 1 1,-1 0 0,1-1 0,0 1-1,0 0 1,-1 0 0,1 0 0,0 0 0,0 0-1,-2 0 1,-18-6-225,20 5-883</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1966.98">905 295 2065,'0'0'11419,"-14"15"-11091,-43 44-214,45-38-110,18-10-49,22-6-158,-25-5 149,8 0-216,1 0 0,0-1 0,0 0 1,0-1-1,-1 0 0,1-1 1,-1 0-1,0-1 0,0 0 1,11-6-1,-15 7 127,0-1 0,-1 0 0,0-1 0,0 1 0,0-1 0,0 0 0,-1-1 0,0 1 0,0-1 0,-1 0 0,1-1 0,-1 1-1,0-1 1,-1 1 0,0-1 0,0 0 0,2-9 0,1-9 183,-2 1-1,0-1 0,-1-35 1,-8-28 3220,5 87-3094,0 0-1,0 0 1,0 0 0,0 1 0,0-1-1,-1 0 1,1 0 0,0 0-1,0 0 1,-1 0 0,1 0 0,0 1-1,-1-1 1,1 0 0,-1 0-1,1 1 1,-1-1 0,0 0 0,1 1-1,-1-1 1,0 0 0,-11 9 1870,-5 30-1491,7-3-363,-20 82 329,28-103-653,0 0 0,1 0 0,0 0 0,1 0 0,0 1-1,4 18 1,-3-32 19,-1 0-1,1 0 1,-1 0-1,1 0 1,0 0-1,0-1 1,-1 1-1,1 0 1,0 0-1,0-1 0,0 1 1,0-1-1,0 1 1,0 0-1,0-1 1,0 0-1,0 1 1,0-1-1,0 0 1,0 1-1,0-1 1,0 0-1,0 0 1,0 0-1,1 0 1,-1 0-1,0 0 0,0 0 1,0-1-1,0 1 1,0 0-1,0 0 1,2-2-1,1 2-314,1-2 0,-1 1 0,1 0 0,-1-1 0,1 0 0,-1 0 0,5-3-1,1-5 134,-2 0 0,1 0-1,-1 0 1,-1-1-1,0 0 1,0-1 0,-1 1-1,5-17 1,-3 10 1984,1 0 0,19-29 1,-20 41 374,-5 11-571,-7 14-944,-2-9-493,-1 0-1,-1 0 1,1-1-1,-1-1 0,-1 1 1,0-1-1,0-1 1,0 1-1,-1-2 1,-18 10-1,13-7-400,1 1 0,0 0 0,0 1 0,-18 18 0,31-28-515,6 0 772,-1 0-1,0 0 1,1-1-1,-1 1 1,1-1-1,-1 0 1,1-1-1,6 0 1,8-1-27,237 2-5891,-212 0-22</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2895.1">1911 69 1457,'0'0'3836,"0"-14"8167,10 260-10226,-9-236-1762,-1-1 0,0 1 1,0 0-1,-1-1 0,0 1 1,-1-1-1,0 0 0,-1 1 0,-3 9 1,4-14-5,-1 0 1,0 0-1,0-1 0,0 1 1,-1-1-1,1 0 1,-1 0-1,0 0 0,0 0 1,0-1-1,-1 1 1,1-1-1,-1 0 0,0-1 1,0 1-1,-9 2 1,13-4-1,0 0 1,0 0-1,-1-1 1,1 1 0,0-1-1,0 1 1,-1-1-1,1 0 1,0 1 0,0-1-1,-1 0 1,1 0-1,0 0 1,-1 0 0,1 0-1,0 0 1,-1 0-1,1 0 1,0-1 0,-1 1-1,1-1 1,0 1-1,0 0 1,-1-1 0,1 0-1,0 1 1,0-1-1,0 0 1,0 0 0,0 0-1,0 1 1,0-1-1,0 0 1,-1-2 0,0-1-7,1 0 0,0-1 0,0 1 0,0 0 0,0-1-1,1 1 1,0 0 0,0-8 0,0 11-16,1 1 0,-1-1 1,1 1-1,-1-1 0,1 0 0,0 1 0,-1-1 0,1 1 0,0 0 0,-1-1 0,1 1 0,0-1 0,0 1 0,-1 0 0,1 0 0,0-1 0,0 1 0,-1 0 0,1 0 0,0 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,1 0 0,28 1-103,-25-1 84,8 2 21,0 1 0,0 0 0,0 1 0,-1 0 0,1 1 0,19 10 0,-20-8-4,1-2 1,0 1-1,0-1 0,0-1 0,0-1 1,25 4-1,-33-6 11,1-1-1,0 0 1,0 0 0,-1 0-1,1-1 1,0 0-1,0 0 1,6-2 0,-10 2 8,0-1 0,0 1 0,0 0 0,0 0 0,-1-1 0,1 1 0,-1-1 0,1 0-1,-1 1 1,0-1 0,1 0 0,-1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,0 0 0,1-1 0,-1-1 0,1-15 17,0-1-1,-2 1 1,0 0-1,-1 0 1,0-1 0,-2 1-1,-1 1 1,0-1-1,-1 1 1,-1 0-1,0 0 1,-2 0-1,0 1 1,-1 1 0,0 0-1,-2 0 1,0 1-1,0 0 1,-2 1-1,1 1 1,-19-14-1,29 25-36,0-1-1,0 1 0,-1 0 1,1 0-1,-1 0 1,0 0-1,0 1 0,1 0 1,-1 0-1,0 0 0,0 0 1,0 0-1,0 1 0,-6-1 1,7 2-11,0-1 0,0 1 0,1 0 0,-1-1 0,0 1 0,1 0 0,-1 1 0,1-1 1,-1 0-1,1 1 0,-1 0 0,1-1 0,0 1 0,0 0 0,0 0 0,-2 3 0,-1 1-284,1 1 0,0 0 0,0 0 0,1 0 0,0 0 0,0 1 0,1-1 0,0 1 0,0 0 0,1 0 0,0 0 0,0 15 0,1 22-3421,0-1-1523</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3718.1">2293 237 4770,'0'0'13222,"-1"-8"-12565,-8-21-289,-3 24-200,-9 18-88,14-6-110,0 0 1,1 1-1,0-1 1,0 1-1,1 1 1,0-1-1,0 1 1,1 0-1,0 0 1,1 0-1,0 0 1,0 1-1,1-1 1,0 1-1,0 19 1,2-28-12,0-1 0,0 1 0,0 0 1,0-1-1,0 1 0,0-1 0,0 1 1,1 0-1,-1-1 0,0 1 0,0-1 1,1 1-1,-1-1 0,0 1 0,1-1 1,-1 1-1,0-1 0,1 1 0,-1-1 1,1 0-1,-1 1 0,1-1 0,-1 1 1,1-1-1,-1 0 0,1 0 0,-1 1 1,1-1-1,-1 0 0,1 0 0,0 0 1,0 1-1,27-3-1124,-22 0 861,0 1 0,0-1 0,0-1 0,0 1 0,0-1 1,7-5-1,-11 6 278,0 1 0,0-1 0,0 0-1,0 0 1,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,0-1 0,0 1 0,0 0 0,0-1 0,0 1 0,-1-1-1,1 1 1,0-4 0,-1 5 1024,0 29-777,0-26-225,0 1-1,0-1 0,0 1 0,0 0 0,1-1 0,-1 1 0,1-1 0,0 1 0,0-1 0,0 1 0,0-1 0,0 1 0,0-1 0,1 0 0,-1 0 1,1 0-1,0 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,0-1 0,0 1 0,1-1 0,-1 1 0,0-1 0,1 0 0,-1 0 0,0 0 0,1 0 1,0-1-1,2 1 0,-1 0-5,0-1 1,0 0-1,-1 0 1,1 0-1,0 0 1,0 0-1,0-1 1,0 0 0,0 0-1,-1 0 1,1 0-1,0-1 1,-1 0-1,1 1 1,-1-1-1,0 0 1,1-1-1,-1 1 1,0 0 0,0-1-1,4-5 1,0-2 9,0 0 1,0-1 0,-2 1 0,1-1 0,-1 0 0,-1-1 0,0 1-1,0-1 1,-2 0 0,4-23 0,-3-9 367,-2-75 1,-3 55 752,2 62-707,0 30-681,0 24 228,-2-19 41,2 1 1,2 0-1,10 60 0,-10-85 0,1 1 1,0 0-1,1-1 1,0 0 0,0 0-1,0 0 1,1-1-1,1 1 1,0-1-1,0 0 1,0-1-1,1 1 1,0-1 0,0-1-1,1 1 1,0-1-1,13 7 1,-10-8-10,0 0 0,0-1-1,1 0 1,0-1 0,-1 0 0,1-1 0,0 0-1,0-1 1,0 0 0,0-1 0,0 0 0,14-3 0,-21 2 19,0 1 1,-1-2-1,1 1 1,0-1 0,-1 1-1,1-1 1,-1-1 0,0 1-1,1-1 1,-1 1 0,0-1-1,-1 0 1,1 0 0,0-1-1,-1 1 1,0-1 0,0 0-1,0 0 1,0 0-1,-1 0 1,1-1 0,-1 1-1,0 0 1,0-1 0,1-5-1,0 0 19,0 0 0,-1-1 0,0 1 0,0-1 0,-1 1 0,0-1 0,-1 1 0,-1-1 0,1 1 0,-5-19 0,5 28-27,0 0 0,0-1 0,-1 1 0,1 0 1,-1 0-1,1 0 0,-1 0 0,1-1 0,-1 1 0,1 0 0,-1 0 0,0 0 0,0 0 0,1 0 0,-1 1 0,0-1 0,0 0 1,0 0-1,0 0 0,0 1 0,0-1 0,0 0 0,0 1 0,-1-1 0,1 1 0,0 0 0,0-1 0,0 1 0,-1 0 0,1 0 0,0-1 1,0 1-1,0 0 0,-1 0 0,1 0 0,0 1 0,0-1 0,-1 0 0,0 1 0,-1 0-1,0 0 0,0 0 0,0 0-1,0 1 1,1-1 0,-1 1 0,1 0 0,-1 0 0,1 0-1,0 0 1,-1 0 0,1 0 0,0 1 0,1-1-1,-3 3 1,-3 12 3,0 0 1,1 1-1,1 0 0,1 0 0,0 0 0,1 0 0,1 1 0,1-1 1,2 24-1,-1-40-66,0 0 0,0 1 0,1-1-1,-1 0 1,1 1 0,-1-1 0,1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,1 0 0,-1 0 0,1-1 0,0 1 0,0 0 0,-1-1 0,1 0 0,0 1 0,0-1 0,0 0 0,1 0-1,-1 0 1,0 0 0,0-1 0,0 1 0,1 0 0,1-1 0,6 2-909,1 0-1,-1-1 0,0-1 0,0 0 1,21-2-1,6-6-4107</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3872.99">2438 237 5475,'0'0'7619,"188"-31"-9716,-75 4-2545</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7893.19">206 824 5539,'0'0'12557,"-3"-3"-12157,-1 0-321,-1 1 0,0-1 0,-1 1 0,1 0 0,0 0 0,-1 0 0,1 1 0,-1 0 0,0 0 0,1 0 0,-1 1 0,0 0 0,1 0 0,-1 0 0,0 1 0,1 0 0,-11 3 0,11-4-79,0 1 0,0 0 0,1 0 1,-1 1-1,0 0 0,1 0 0,-1 0 0,1 0 0,0 0 0,-1 1 1,1 0-1,0 0 0,1 0 0,-1 0 0,0 1 0,1 0 0,0-1 1,0 1-1,0 0 0,0 1 0,-3 8 0,5-10-36,0 0 0,0 0 0,1 0 0,-1 1 0,1-1 0,0 0 0,0 0 0,0 1 0,1-1 0,-1 0 0,1 0 0,0 1 0,-1-1 0,1 0 0,1 0 1,-1 0-1,0 0 0,1 0 0,0-1 0,-1 1 0,1 0 0,0-1 0,0 1 0,1-1 0,-1 0 0,1 1 0,-1-1 0,1 0 0,-1-1 0,1 1 0,0 0 0,0-1 0,0 0 0,4 2 0,13 4-253,1 0 1,0-2-1,-1-1 0,30 3 1,-5 0-299,-42-6 573,-1-1 0,0 0 1,0 1-1,1-1 1,-1 1-1,0 0 0,0 0 1,0 0-1,0 0 0,0 0 1,3 2-1,-5-2 18,0-1 0,0 0 0,0 1 0,0-1 0,0 0-1,0 1 1,0-1 0,0 0 0,0 1 0,0-1 0,0 1 0,0-1 0,0 0-1,0 1 1,0-1 0,0 0 0,0 1 0,0-1 0,-1 0 0,1 1 0,0-1-1,0 0 1,0 1 0,-1-1 0,1 0 0,0 0 0,0 1 0,0-1 0,-1 0-1,1 0 1,0 1 0,-1-1 0,1 0 0,0 0 0,-1 0 0,1 0 0,0 0-1,-1 1 1,1-1 0,-52 18 701,46-16-612,-51 10 412,42-9-609,0 0-1,1 0 0,-1 1 1,1 1-1,-15 7 1,27-11-1908</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8187.88">268 1061 3490,'0'0'8942,"17"-13"-8237,-1 2-588,5-3-5,-1 0 0,0-2 0,-1 0 0,24-27 0,-38 35 32,0-1 0,-1 0 0,0 0 0,0 0 0,-1-1 0,0 1 0,-1-1 0,0 0 0,0 0-1,-1 0 1,0 0 0,-1 0 0,0 0 0,0 0 0,-1 1 0,-3-12 0,-1 9 965,-2 15-448,-1 19-556,5 17-203,1 0 0,2 0 0,6 44 0,-4-77-258,-1 0 0,1 0 0,0 0 0,1 0 0,0 0 0,0 0-1,4 5 1,15 19-6631</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8331.59">380 999 6115,'0'0'9140,"-10"-40"-9700,58 34-929,17-3-1456,-6 0-1489,-5-1-1393</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8547.37">735 873 6947,'0'0'11445,"0"23"-10687,-1-6-455,-1 0-1,0 0 1,-2-1-1,-8 26 1,7-25-480,0 1-1,1-1 1,1 1 0,-2 29 0,5-46-551,0 5 785</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="11296.89">1857 849 304,'0'-2'17667,"-1"21"-17561,1 37 28,0-54-131,0-1 0,0 0 0,0 1 0,0-1-1,1 0 1,-1 1 0,0-1 0,1 0 0,-1 0-1,1 0 1,0 1 0,-1-1 0,1 0 0,0 0 0,0 0-1,-1 0 1,1 0 0,0 0 0,0 0 0,0 0-1,0-1 1,0 1 0,1 0 0,-1 0 0,0-1 0,0 1-1,0-1 1,1 1 0,-1-1 0,0 0 0,0 1-1,1-1 1,1 0 0,3 0-53,0 0 0,0 0-1,0 0 1,1-1 0,-1 0 0,0 0 0,-1-1-1,1 0 1,8-3 0,-11 3 40,0 0-1,0 0 1,-1-1 0,1 1-1,-1-1 1,1 1-1,-1-1 1,0 0 0,0 0-1,0 0 1,0 0 0,-1 0-1,1 0 1,-1 0 0,0-1-1,0 1 1,0 0-1,1-6 1,4-12 20,-4 27-93,-3 43-86,0-27 240,0 8-5,0-16-119,1 0-1,0-1 0,3 17 0,6-15-1867,9-9-3308,-3-5 774</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="11541.88">2177 760 4866,'0'0'7849,"4"-12"-7003,-3 55 675,-3 31 144,0-39-1616,1 1 1,7 52 0,-6-87-222,0 0 1,0 0-1,0 0 0,0 0 1,1 0-1,-1 0 0,0-1 1,0 1-1,1 0 1,-1 0-1,1 0 0,-1 0 1,1 0-1,-1-1 1,1 1-1,-1 0 0,1 0 1,0-1-1,-1 1 0,1-1 1,0 1-1,0 0 1,-1-1-1,1 1 0,0-1 1,0 0-1,0 1 1,0-1-1,0 0 0,-1 1 1,1-1-1,0 0 1,0 0-1,0 0 0,0 0 1,0 0-1,0 0 0,0 0 1,1 0-1,14 0-4513</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="11758.71">2309 855 5731,'0'0'7747,"0"7"-7555,0 14 593,0 4-17,0-1-384,0 4-112,0-10-272,0 1 0,0-4-320,0-3-1377,0-8-1040,5-4-1953</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="12234.7">2575 739 6835,'0'0'7905,"-2"6"-7742,-9 33-124,-38 165 2473,43-169-4314,2 0 0,0 35 0,15-69-10246</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="12681.44">2680 839 4130,'0'0'8625,"8"-5"-7953,-4 2-573,0 0 54,1-1-1,-1 1 1,1 1 0,0-1-1,0 1 1,0-1 0,0 2 0,0-1-1,0 0 1,0 1 0,1 0-1,8 0 1,-13 38 34,-1-33-181,0 0-1,-1-1 1,1 1 0,-1-1 0,0 1 0,0 0-1,0-1 1,-1 0 0,1 1 0,-1-1 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0 0,-4 3-1,-4 3 19,-1 0 1,0 0-1,-13 7 0,14-10 67,0 1 0,0 0 1,-17 17-1,27-23-73,1-1 1,-1 1-1,0-1 0,1 1 0,-1 0 0,0-1 1,1 1-1,-1-1 0,1 1 0,-1-1 0,1 1 1,-1-1-1,1 1 0,0-1 0,-1 0 0,1 1 1,0-1-1,-1 0 0,1 1 0,0-1 0,-1 0 1,1 0-1,0 0 0,-1 0 0,1 0 0,0 1 1,-1-1-1,1 0 0,0-1 0,1 1 0,27 5-627,31-5-3286,-34 0-30,0 0-2163</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="12990.43">2962 809 7443,'0'0'8631,"-11"-12"-8420,11 17-191,0 0 0,0 1 1,1-1-1,-1 1 0,1-1 1,1 0-1,-1 1 0,1-1 1,-1 0-1,5 8 0,-1-6 5,0-1 1,1 1-1,0-1 0,0 0 0,0 0 1,10 6-1,-13-10-20,-1 0 0,1 1 1,0-1-1,-1 1 0,1-1 0,-1 1 1,0 0-1,0-1 0,0 1 0,0 0 1,2 6-1,-4-8 0,0 1 0,0-1 0,0 0 0,0 1 0,0-1 0,0 0 0,-1 1 0,1-1 0,-1 0-1,1 1 1,-1-1 0,1 0 0,-1 0 0,0 1 0,1-1 0,-1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0-1 0,0 1 0,0 0 0,-1 0 0,1-1 0,0 1 0,0-1-1,-1 1 1,-1-1 0,-34 16-588,11-12-5645,20-4 839</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="13361.99">2973 753 6963,'0'0'5747,"69"-40"-5651,-47 31 64,-11 6 352,-6 0 241,1 3 95,-1 0-704</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="18643.43">284 1371 4770,'0'0'9498,"0"-4"-8863,0 3-566,0 0 1,0 0-1,0 0 0,0 0 1,-1 0-1,1 0 1,0 0-1,0 0 0,-1 1 1,1-1-1,0 0 1,-1 0-1,1 0 1,-1 0-1,1 1 0,-1-1 1,1 0-1,-1 0 1,0 1-1,1-1 0,-1 0 1,0 1-1,-1-2 1,-1 1 41,1 0 1,-1 0 0,0 0-1,0 1 1,0-1 0,0 1-1,0-1 1,0 1 0,-4 0-1,-14 0-74,16-1-31,0 0 1,0 1-1,-1 0 1,1 0-1,0 0 1,0 1-1,0 0 1,-1 0-1,1 0 1,0 0-1,0 1 1,0 0-1,1 0 1,-1 0-1,0 1 1,-6 4-1,9-6-29,1 1 0,0-1 0,-1 0 1,1 0-1,0 1 0,0-1 0,0 1 0,0-1 0,0 1 0,0 0 0,0-1 0,0 1 0,1 0 0,-1-1 1,1 1-1,-1 0 0,1 0 0,0 0 0,-1-1 0,1 1 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 0 1,0-1-1,1 1 0,1 3 0,0-2-47,0 1 1,0-1-1,1 0 1,0 0-1,-1 0 0,1 0 1,0 0-1,1 0 1,-1-1-1,0 0 1,1 0-1,5 3 0,36 13-872,-35-15 655,0 1 0,-1 0 0,1 0 0,-1 1-1,0 0 1,0 0 0,0 1 0,9 7-1,-18-12 299,1-1-1,-1 1 0,1-1 0,-1 1 0,0-1 0,1 1 0,-1 0 0,1-1 0,-1 1 0,0-1 0,0 1 0,1 0 0,-1-1 0,0 1 0,0 0 0,0-1 0,1 1 0,-1 0 0,0-1 0,0 1 0,0 0 0,0-1 0,-1 1 0,1 0 0,0-1 0,0 1 0,0 0 0,0-1 0,-1 1 0,1 0 0,-20 12 993,-35-3 828,51-9-1790,-102 2-652</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="18998.6">421 1556 6035,'0'0'5477,"16"-8"-5069,52-25-106,-65 31-256,1 0 0,-1 0 0,0-1 1,0 1-1,0-1 0,0 0 1,0 0-1,-1 0 0,1 0 0,-1 0 1,1 0-1,-1-1 0,-1 1 1,1-1-1,0 0 0,-1 1 0,2-7 1,-1-1 160,0 1 0,-1-1 0,0 0 0,-2-16 0,1 11 67,-6-12 440,6 28-666,0-1 0,0 1 0,0 0 0,-1-1 1,1 1-1,0 0 0,-1-1 0,1 1 0,0 0 1,-1-1-1,1 1 0,0 0 0,-1 0 0,1-1 0,-1 1 1,1 0-1,0 0 0,-1 0 0,1 0 0,-1 0 1,1-1-1,-1 1 0,1 0 0,0 0 0,-1 0 1,1 0-1,-1 0 0,1 0 0,-1 0 0,1 1 0,-1-1 1,-1 1 5,0 0 0,0 1 1,0-1-1,0 1 0,1-1 1,-1 1-1,1 0 0,-1 0 1,1 0-1,-1 0 0,1 0 0,0 0 1,0 0-1,0 0 0,0 0 1,0 0-1,0 5 0,-4 8-245,2 0-1,-1 1 0,2-1 0,0 1 1,1 0-1,1 0 0,2 27 0,-1-41-56,-1-1-1,0 0 1,0 1 0,1-1-1,-1 0 1,1 0-1,-1 1 1,1-1-1,-1 0 1,1 0 0,0 0-1,-1 0 1,1 0-1,0 0 1,0 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0-1-1,0 1 1,0 0-1,0-1 1,2 1 0,9 1-5987</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="19124.25">421 1556 4338</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="19229.77">421 1556 4338,'38'-92'7876,"-38"89"-6308,0 0-1568,27 0-784,0 0-96,10 0-1730,6-1-2192</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="19677.55">739 1423 768,'0'0'13812,"37"0"-12105,-33 0-1640,-1 0 0,1 0-1,-1-1 1,1 0 0,-1 0-1,1 0 1,-1 0-1,0 0 1,0 0 0,1-1-1,-1 0 1,0 1 0,0-1-1,0-1 1,-1 1-1,1 0 1,-1-1 0,1 1-1,-1-1 1,0 1 0,1-1-1,-1 0 1,-1 0-1,1 0 1,0-1 0,-1 1-1,0 0 1,0 0 0,0-1-1,0 1 1,0-1-1,-1 1 1,1-1 0,-1 1-1,0-8 1,0 10 264,1 5-401,-1 1 1,1-1-1,-1 0 1,1 0 0,-2 1-1,1-1 1,-1 8-1,0-2 47,-1 24-371,-8 52 1,10-84 334,-1 1 0,0-1-1,0 1 1,0-1 0,0 0 0,0 1 0,0-1 0,-1 0 0,1 0 0,-1 0-1,0 0 1,1 0 0,-1 0 0,0 0 0,0-1 0,0 1 0,0-1 0,0 1-1,-1-1 1,1 0 0,-5 2 0,0-1 348,1 1 0,-1-1 0,0-1 0,0 0 1,0 0-1,-14 1 0,92 12-68,112-12 126,-99-3-2919</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="20668.72">2085 1337 4290,'0'0'11376,"-33"-6"-7718,24 6-3529,1 0-56,1-1 0,-1 2 0,0-1 0,0 1 0,1 0 0,-1 1 0,-10 3 0,16-4-79,0 0 0,0 1 0,0-1 1,0 1-1,0 0 0,0-1 0,0 1 1,0 0-1,1 0 0,-1 0 0,1 1 1,-1-1-1,1 0 0,0 0 0,0 1 1,0-1-1,0 1 0,0-1 0,1 1 0,-1-1 1,1 1-1,0-1 0,-1 1 0,1 0 1,0-1-1,1 5 0,-1-4 4,0 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1 1 0,0-1 0,0-1 0,1 1 0,-1 0 0,1 0 0,-1 0 0,1-1 1,0 1-1,0-1 0,0 1 0,0-1 0,0 0 0,5 4 0,4 1-60,0 0 0,1-1 0,21 9 0,-25-12-8,1 1 0,-1 0 0,0 0 1,0 1-1,0-1 0,-1 2 0,10 8 0,-16-14 48,-1 1-1,0-1 0,1 0 0,-1 0 1,0 1-1,1-1 0,-1 0 0,0 1 1,0-1-1,1 1 0,-1-1 0,0 0 1,0 1-1,0-1 0,1 1 0,-1-1 0,0 1 1,0-1-1,0 0 0,0 1 0,0-1 1,0 1-1,0-1 0,0 1 0,0-1 1,0 1-1,0-1 0,0 0 0,-1 1 1,1-1-1,0 1 0,0-1 0,0 0 1,-1 1-1,1 0 0,-18 6-470,-26-4-3773,41-3 2961,-8 0-3131</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="20854.82">2015 1406 6195,'0'0'7907,"97"-47"-7554,-81 44-193,-5 3-160,-6 0-240,12 0-1025,-7 0-1248,1 0-2225</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="21200.39">2306 1329 464,'0'0'13438,"2"-4"-12280,4-6-91,-1 12-281,1 31 174,-4 60 105,-2-85-826,-1 46 57,-1-34-312,1 0 0,2 0 0,0 0 0,1 0 0,5 22 0,-7-41-186,1 0 0,0 0 0,0 0 0,0-1 0,0 1 1,0 0-1,0-1 0,0 1 0,0-1 0,1 1 0,-1-1 0,0 0 0,0 1 0,0-1 0,1 0 1,-1 0-1,0 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,2-1 1,5 0-1747,13 1-2574</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="21446.39">2575 1393 1793,'0'0'15343,"0"64"-13225,0 15-4047,0-78 1710,0-1-1,0 0 1,1 1 0,-1-1-1,0 0 1,1 1-1,-1-1 1,0 0 0,1 1-1,-1-1 1,0 0-1,1 0 1,-1 1 0,1-1-1,-1 0 1,0 0-1,1 0 1,-1 0-1,1 0 1,-1 1 0,1-1-1,-1 0 1,0 0-1,1 0 1,-1 0 0,1 0-1,-1 0 1,1 0-1,-1-1 1,1 1 0,-1 0-1,1 0 1,1 0-1219,10 0-7209</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="21681.75">2774 1280 7331,'0'0'10117,"-11"89"-9365,5-46-303,-4-6-17,4 2-256,6-5-96,-5 0-32,5-3-48,0-4-432,0-2-865,0-7-2000,0-5-3282</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="22038.15">2935 1445 9748,'0'0'7441,"6"0"-7398,-4 0-38,0 0 1,0 0-1,0 0 0,0 0 0,-1 0 1,1 1-1,0-1 0,0 1 1,0-1-1,0 1 0,-1 0 1,1-1-1,0 1 0,-1 0 1,1 0-1,-1 1 0,1-1 0,1 2 1,-2-1 2,0 0-1,0 0 1,0 0 0,0 0 0,0 0-1,-1 0 1,1 0 0,0 0 0,-1 1-1,0-1 1,0 0 0,0 0 0,0 1-1,0-1 1,0 0 0,0 0 0,-1 1-1,0 3 1,-1-2 7,1 1 0,-1-1 0,1 0 0,-1 0-1,-1-1 1,1 1 0,0 0 0,-1-1 0,0 1 0,1-1 0,-2 0 0,1 0-1,-6 5 1,-57 33 185,6-3 142,54-36-319,3 0 529,10 0-290,19 0-419,1-1-1,28-3 1,16-11-4280,-28-2-1573</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="22327.98">3145 1393 6339,'0'0'10994,"-11"4"-10668,-32 16-153,41-18-167,1 0-1,-1 0 1,1 1 0,0-1-1,-1 1 1,1-1 0,0 1-1,1-1 1,-1 1 0,0-1-1,1 1 1,-1 0-1,1 0 1,0-1 0,0 1-1,0 0 1,0-1 0,1 1-1,-1 0 1,1-1 0,0 4-1,0 0 7,1-1 12,0 1 0,0-1 0,0 1 0,1-1-1,0 0 1,0 0 0,0 0 0,0 0 0,1-1 0,0 1 0,0-1-1,0 0 1,1 0 0,-1 0 0,1-1 0,0 0 0,0 0 0,9 4-1,15 13 119,-29-20-187,0 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 1 0,0-1 0,1 0 0,-1 0 0,0 0 0,0 0 0,0 0 0,1 1 0,-1-1 0,0 0 0,0 0 0,0 0 0,0 1 0,0-1 0,1 0 0,-1 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,-1 0 0,1 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0 0 0,-1 1 0,1-1 0,0 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 1 0,-17 0-5230,16-1 5106,-16 0-6260</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="22483.79">3105 1359 8756,'0'0'8676,"140"-67"-8612,-114 64-64,-9 0-416,-7 3-1825</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">54 72 224,'0'0'5723,"2"-8"-4766,3-25 693,-1 2 5334,-5 116-6973,0-5 498,13 128 1,-4-142 114,1 89 0,-9-155-560,1 0-43,0-1 1,-1 0-1,1 0 0,0-1 0,-1 1 1,1 0-1,-1 0 0,1 0 0,-1 0 0,0 0 1,1-1-1,-1 1 0,0 0 0,0 0 1,0-1-1,0 1 0,0 0 0,0 0 1,0 0-1,0-1 0,0 1 0,-1-2 0,-5-33 452,2 27-487,-1-1 1,0 1-1,0 1 0,-1-1 1,0 1-1,-1 0 1,0 0-1,0 1 1,0 0-1,-1 0 0,-16-10 1,24 16 0,0 17-269,0-1 265,1 0-1,1 0 1,1 0 0,0 0-1,1-1 1,1 1 0,0-1-1,1 0 1,0 0 0,1 0-1,1-1 1,16 22 0,-24-35 29,0 0 0,1 1 1,-1-1-1,0 0 0,1 0 0,-1 0 1,0 1-1,1-1 0,-1 0 1,1 0-1,-1 0 0,0 0 0,1 1 1,-1-1-1,1 0 0,-1 0 1,0 0-1,1 0 0,-1 0 1,1 0-1,-1 0 0,1 0 0,-1 0 1,0 0-1,1-1 0,-1 1 1,0 0-1,1 0 0,-1 0 0,1 0 1,-1-1-1,0 1 0,1 0 1,-1 0-1,0-1 0,1 1 1,-1 0-1,0 0 0,0-1 0,1 1 1,-1 0-1,0-1 0,0 1 1,1-1-1,-1 1 0,0 0 0,0-1 1,0 1-1,0 0 0,0-1 1,0 1-1,0-1 0,0 0 1,10-29 247,-7 22-221,50-127-55,-40 117-1202,-4 7-2340,-5-1-4000,-4 6 2132</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -2509,7 +3032,7 @@
           <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
         </inkml:channelProperties>
       </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2025-01-04T15:30:15.599"/>
+      <inkml:timestamp xml:id="ts0" timeString="2025-02-22T15:36:43.974"/>
     </inkml:context>
     <inkml:brush xml:id="br0">
       <inkml:brushProperty name="width" value="0.035" units="cm"/>
@@ -2517,7 +3040,7 @@
       <inkml:brushProperty name="color" value="#004F8B"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">264 6 6787,'0'0'6144,"-17"-2"-6069,-53-1 58,67 3-104,0 0-1,0 1 0,1-1 1,-1 1-1,0 0 0,1 0 1,-1 0-1,1 0 0,-1 0 1,1 0-1,-1 1 0,1-1 1,0 1-1,0 0 0,0 0 1,0 0-1,0 0 0,0 0 1,0 0-1,1 0 0,-1 1 1,-1 1-1,-7 10 331,-8 5 334,1 1-1,-26 37 1,38-49-637,1 0 1,0 1-1,0-1 1,0 1 0,1 0-1,0 0 1,1 0 0,0 1-1,1-1 1,-1 19-1,2-27-49,1 1 0,0 0 0,-1-1 0,1 1 0,0 0 0,0-1 0,0 1 0,0-1 0,0 0 0,0 1 0,0-1 0,1 0 0,-1 1 0,0-1 0,1 0 0,-1 0 0,1 0 0,-1 0-1,1-1 1,0 1 0,-1 0 0,1-1 0,0 1 0,-1-1 0,1 1 0,0-1 0,0 0 0,-1 0 0,4 0 0,63 4 153,-60-4-136,-3 0-4,1 1 1,-1-1 0,0 0 0,0-1-1,1 1 1,-1-1 0,0 0 0,0 0-1,0-1 1,0 1 0,0-1 0,0 0-1,-1-1 1,1 1 0,-1-1 0,1 0-1,-1 0 1,0 0 0,0-1 0,0 1-1,0-1 1,-1 0 0,0 0 0,0 0-1,0 0 1,4-8 0,-1 1 51,-1 0 1,0-1-1,-1 0 1,-1 1-1,1-1 0,-2-1 1,0 1-1,0 0 1,-1-1-1,0 1 1,-2 0-1,-2-24 1,3 34-43,-1 0 1,0 1-1,1-1 1,-1 1-1,0-1 1,0 1-1,0-1 1,0 1-1,0 0 1,-1-1 0,1 1-1,0 0 1,-1 0-1,1 0 1,0 0-1,-1 0 1,0 0-1,1 1 1,-1-1-1,1 0 1,-1 1 0,0-1-1,1 1 1,-1-1-1,0 1 1,0 0-1,1 0 1,-1 0-1,-3 0 1,-1 0-36,1 0 0,-1 0-1,0 1 1,0-1 0,1 1 0,-1 1 0,1-1-1,-8 3 1,4 2-275,-1 0 0,2 0 1,-1 1-1,1 0 0,0 0 0,0 1 0,-12 15 0,-22 34-7136,24-28-1599</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">6 81 4034,'0'0'7347,"0"-5"-6488,0-61 4503,0 56-3667,0 49-2351,14 184 857,-11-192-200,8 64 36,4 83 126,-4-125 160,-11-53-8,-1-34-24,-3 11-290,0 0 0,-2 1-1,-1 0 1,0 0 0,-19-37 0,22 56-4,4 2-21,-1 24-187,2 0 74,5 26 0,-6-44 140,1 1 1,1-1-1,-1 1 1,1-1-1,0 0 0,0 0 1,0 0-1,1 0 0,-1 0 1,1 0-1,1-1 1,-1 1-1,1-1 0,6 6 1,-9-9-6,0 0 1,1 0 0,-1 0 0,0 0-1,0 0 1,1-1 0,-1 1-1,1 0 1,-1-1 0,0 1 0,1-1-1,-1 0 1,1 1 0,-1-1 0,1 0-1,0 0 1,-1 0 0,1 0-1,-1 0 1,1-1 0,-1 1 0,1 0-1,-1-1 1,0 1 0,3-2 0,-1 1 9,0-1 0,-1 0 0,1-1 0,-1 1 0,1 0 0,-1-1 0,0 1 0,0-1 0,0 0 0,0 0 0,2-3 0,1-6 15,0 1 1,-1 0-1,0-1 0,-1 0 0,4-20 0,-6-35-1912,-18 67-7856,-4 2 2461</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -2537,7 +3060,7 @@
           <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
         </inkml:channelProperties>
       </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2025-01-04T15:30:22.954"/>
+      <inkml:timestamp xml:id="ts0" timeString="2025-02-22T15:36:48.832"/>
     </inkml:context>
     <inkml:brush xml:id="br0">
       <inkml:brushProperty name="width" value="0.035" units="cm"/>
@@ -2545,9 +3068,9 @@
       <inkml:brushProperty name="color" value="#004F8B"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">6 7 4210,'0'0'10557,"0"-6"-4255,1 7-6047,5 17-192,-1-1-1,-1 1 0,-1-1 1,2 25-1,-4-35-33,-1-1-1,0 1 1,0-1-1,-1 1 1,1-1-1,-1 1 1,-1-1-1,1 0 1,-1 1 0,-1-1-1,1 0 1,-1 0-1,0 0 1,0-1-1,-5 8 1,7-7-2086</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="592.65">291 4 1409,'0'0'12261,"-31"-3"-9737,26 4-2343,1 0 1,0 0-1,-1 1 0,1 0 1,0-1-1,0 1 0,0 1 0,0-1 1,1 1-1,-1-1 0,-3 5 1,-38 34 1246,41-36-1380,0 0 0,1 0-1,0 0 1,0 0-1,0 0 1,0 1 0,1 0-1,0-1 1,0 1 0,0 0-1,1 0 1,0 0-1,0 0 1,1 0 0,-1 0-1,1 0 1,2 12-1,-2-9-39,0-8-7,0 0 0,1 1 0,-1-1 0,1 0 0,-1 0 0,1 0 0,0 0 1,-1 0-1,1 0 0,0 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,0-1 1,1 1-1,-1 0 0,0-1 0,0 1 0,0-1 0,0 0 0,1 1 0,-1-1 0,0 0 0,0 1 1,1-1-1,-1 0 0,2 0 0,46 2 84,-42-2-63,-3 0-15,0 0 0,0 0-1,0-1 1,0 1 0,0-1-1,0 0 1,0 0 0,0 0 0,0-1-1,-1 1 1,1-1 0,-1 0-1,1 0 1,-1 0 0,1-1-1,-1 1 1,0-1 0,0 0 0,0 0-1,-1 0 1,1 0 0,3-7-1,-2 3-75,0-1 0,-1 0 0,0 0 0,-1 0 0,0 0 0,0 0 0,0 0 0,-1-1 0,-1 1 0,0-10 0,0 16 62,-1 1 1,1 0 0,-1 0 0,0 0 0,1 1 0,-1-1 0,0 0-1,0 0 1,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 1-1,0-1 1,0 1 0,0-1 0,0 1 0,0 0 0,-1-1 0,1 1 0,0 0-1,0 0 1,0 0 0,-3 0 0,-31-3-3137</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1128.67">488 31 4514,'0'0'11130,"-6"16"-9822,-31 36 831,29-44-1858,1 1 0,1 0-1,0 0 1,0 0-1,-9 20 1,15-28-275,0 0 0,-1 0 0,1 0-1,0 0 1,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,1 0 0,-1 1 0,0-1-1,0 0 1,0 0 0,1 0 0,-1 0 0,0 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1 0-1,-1 0 1,1-1 0,0 1 0,0 0 0,-1 0 0,1-1 0,0 1 0,0 0 0,0-1-1,0 1 1,0 0 0,0-1 0,0 0 0,0 1 0,0-1 0,0 1 0,0-1 0,0 0 0,0 0-1,0 0 1,0 0 0,0 0 0,2 0 0,60 1 122,-46-2-47,-13 1-70,1 0 1,-1 0-1,0 0 0,1-1 0,-1 0 1,0 0-1,0 0 0,1 0 0,-1 0 0,0-1 1,0 0-1,-1 0 0,1 0 0,0 0 1,-1-1-1,1 0 0,-1 1 0,0-1 1,0 0-1,0-1 0,0 1 0,0 0 1,-1-1-1,1 0 0,-1 1 0,0-1 1,0 0-1,-1 0 0,1 0 0,-1 0 1,0-1-1,0 1 0,0 0 0,-1 0 1,1-1-1,-1 1 0,0 0 0,0-1 1,-1 1-1,1 0 0,-3-8 0,2 10-12,-1 0-1,1 0 0,-1 0 1,1 0-1,-1 0 0,0 0 0,0 1 1,0-1-1,0 1 0,0-1 1,-1 1-1,1 0 0,0 0 1,0 0-1,-1 0 0,1 0 1,-4 0-1,-45-9-101,43 10-87,-20 3-234,27-3 182,0 0 0,1 1 0,-1-1 0,0 1 0,0-1 1,1 1-1,-1-1 0,0 1 0,1-1 0,-1 1 0,1 0 1,-1-1-1,1 1 0,-1 0 0,1-1 0,-1 1 0,1 0 1,0 0-1,-1 0 0,1-1 0,0 1 0,0 0 0,-1 0 1,1 0-1,0 0 0,0 0 0,0-1 0,0 3 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">102 651 4690,'0'0'8433,"0"-20"-7979,0-158 573,-2 143-762,-12-69 1,8 69-219,-4-68-1,10 17 624,0 85-441,-6 4-181,0 5-87,0 0 0,1 1-1,0 0 1,1 0 0,0 0-1,0 0 1,-3 15 0,-4 10 41,5-14-1,0-1 7,7-28-220,1 1 63,0 0-1,0 0 1,1 0-1,0 1 1,0-1-1,1 1 0,0-1 1,1 1-1,-1 0 1,1 1-1,1-1 0,-1 1 1,10-7-1,-14 12 156,1 0 0,-1 1-1,1-1 1,-1 1 0,1-1 0,0 1-1,-1 0 1,1-1 0,0 1 0,-1 0 0,1 0-1,0 0 1,-1 1 0,1-1 0,0 0-1,-1 1 1,1-1 0,-1 1 0,1-1-1,0 1 1,-1 0 0,1-1 0,-1 1-1,0 0 1,1 0 0,-1 0 0,0 0-1,1 1 1,-1-1 0,0 0 0,0 0-1,0 1 1,1 2 0,6 7 44,0 1 0,-1 1 1,7 17-1,2 1-84,-15-29-288,8 11-103,-3-7-4772</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="402.52">446 38 6403,'0'0'7777,"0"-8"-6703,0 5-1059,-1 5 318,-6 41 245,-4 80 0,10-103-384,0 141 47,1-145-3713,0-42-834,0-1-3316</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1008.43">395 50 6819,'0'0'3946,"23"-5"-3356,-4 0-478,23-4 181,84-9 1,506 6 1012,-545 12 133,-86 1-1405,1-1 0,-1 1 0,0 0 0,0 1 1,0-1-1,0 0 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0 1,-1 1-1,1-1 0,0 1 0,-1-1 0,1 1 0,-1-1 1,0 1-1,0-1 0,1 1 0,-1-1 0,0 3 0,0-1 26,15 76 567,-4 1 0,1 101 0,-13-179-601,1 0-1,-1 0 1,1 0-1,-1 0 0,0 0 1,0 0-1,0 0 1,0 0-1,0 0 1,0-1-1,0 1 0,-1 0 1,1-1-1,-1 1 1,1-1-1,-1 1 1,0-1-1,1 0 0,-1 1 1,0-1-1,0 0 1,0 0-1,0-1 1,0 1-1,0 0 0,-4 0 1,-65 15 578,57-15-491,-71 8 115,-167-5 1,147-5-187,-72-13 109,2 1-1228,187 0-5070,3 1 1892</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -2567,7 +3090,7 @@
           <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
         </inkml:channelProperties>
       </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2025-01-04T15:30:21.623"/>
+      <inkml:timestamp xml:id="ts0" timeString="2025-02-22T15:37:36.165"/>
     </inkml:context>
     <inkml:brush xml:id="br0">
       <inkml:brushProperty name="width" value="0.035" units="cm"/>
@@ -2575,8 +3098,15 @@
       <inkml:brushProperty name="color" value="#004F8B"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">15 96 2721,'0'0'9757,"-15"0"-2229,394-9-6847,-318 6-799,-49 10-4948,-5 0-1750</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="355.39">426 16 4370,'0'0'14852,"-4"-3"-14417,-10-7-328,10 8-211,28 6-198,-6 2 295,0 0 0,-1 1-1,1 1 1,-1 1 0,-1 0-1,0 2 1,28 21 0,-43-31 4,0 1 1,1 0-1,-1-1 1,0 1-1,0 0 1,0 0 0,0-1-1,-1 1 1,1 0-1,0 0 1,-1 0-1,1 0 1,-1 0 0,0 0-1,1 0 1,-1 0-1,0 0 1,0 0 0,0 0-1,-1 0 1,1 0-1,0 0 1,-1 0-1,0 0 1,1 0 0,-1 0-1,0 0 1,0 0-1,0 0 1,0-1-1,0 1 1,0 0 0,-1-1-1,1 1 1,0-1-1,-1 1 1,0-1 0,1 0-1,-1 0 1,0 1-1,1-1 1,-5 1-1,-73 28 457,56-22-1407,0 0 0,-32 17-1,53-23-943</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">11 194 6467,'0'0'3799,"-11"5"4664,12 37-8274,1 0 0,16 80 1,-18-122-224,3 15-11,0-29-14291</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="246.69">35 219 10389,'0'0'7579,"-2"-15"-7085,-5-44-291,7 56-202,0 1 1,0 0 0,0-1 0,0 1-1,1 0 1,-1-1 0,1 1-1,-1 0 1,1 0 0,0-1 0,0 1-1,0 0 1,0 0 0,0 0 0,1 0-1,-1 0 1,1 1 0,-1-1 0,1 0-1,0 0 1,-1 1 0,1-1 0,0 1-1,4-2 1,0-1-43,1 0 1,0 1-1,0 0 1,1 1-1,8-3 0,-10 3-292,1 1-1,-1 0 0,1 0 0,-1 0 0,12 1 0,-17 0 132,1 0-1,-1 1 1,0-1-1,0 0 1,1 0 0,-1 0-1,0 1 1,0-1-1,0 1 1,0-1 0,0 1-1,1-1 1,-1 1 0,0 0-1,0-1 1,0 1-1,-1 0 1,1 0 0,0 0-1,0 0 1,0 0-1,0 0 1,-1 0 0,1 0-1,-1 0 1,1 0-1,-1 0 1,1 0 0,-1 1-1,1-1 1,-1 0-1,0 0 1,0 0 0,0 1-1,0 1 1,0 21-4283</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="446.96">35 219 2353,'-27'79'12134,"32"-79"-12471,17 0 113,10 0 96,6 0 48,-1 0-2081,1 0-848,-6 0-2818</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="659.48">355 278 10645,'0'0'6643,"-5"15"-6643,5 7 224,0-1-160,0 1-48,0 2-16,0-5-64,0-4-736,0-3-1345,0-3-1217</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="817.27">371 216 6627,'0'0'10581,"11"-68"-10741,0 68-1425,5 0-2177,6 0-1408</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1625.98">371 216 7027,'48'8'1708,"-32"-5"-610,1 0-1,0-1 1,25 0 0,-42 5 1692,6 21-2157,-3-11-374,0 0-1,0 0 1,-2 1 0,-1 27 0,0-35-110,-1-30 1284,0 17-1466,1 1 0,-1-1 0,1 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,1 0 0,-1 1 1,1-1-1,0 0 0,-1 1 0,1-1 0,1 0 0,-1 1 0,0-1 0,1 1 0,-1 0 0,1-1 0,0 1 0,-1 0 0,1 0 0,0 0 0,4-2 1,20-14-1569,2 2 1,0 0 0,58-21 0,-45 20 24,-41 17 1612,1 0 1,-1 0-1,1 0 1,-1-1 0,0 1-1,1 0 1,-1 0 0,1 0-1,-1 0 1,1 0 0,-1-1-1,1 1 1,-1 0 0,0 0-1,1-1 1,-1 1 0,0 0-1,1-1 1,-1 1 0,0 0-1,1-1 1,-1 1 0,0-1-1,0 1 1,1 0 0,-1-1-1,0 1 1,0-1 0,0 1-1,0-1 1,1 0-1,-16-4 2436,-27 4 353,40 1-3089,0 0 287,0 0 0,0 1 0,-1-1 0,1 1 0,0-1 0,0 1 0,0 0 0,0 0 0,0 0 1,0 0-1,0 0 0,1 0 0,-1 0 0,0 1 0,0-1 0,1 1 0,-1-1 0,1 1 0,0 0 0,-1 0 0,1-1 0,0 1 0,0 0 0,0 0 0,0 0 0,0 0 0,1 0 0,-1 0 1,1 1-1,-1-1 0,1 0 0,0 0 0,-1 0 0,1 0 0,0 1 0,1-1 0,-1 2 0,0 2-51,0 0 0,1 1 1,0-1-1,0-1 0,0 1 0,0 0 1,1 0-1,0 0 0,0-1 0,1 1 0,0-1 1,4 7-1,-1-7 7,-1 1 0,0 0 1,0 0-1,0 0 0,-1 0 1,1 1-1,-2-1 0,1 1 0,-1 0 1,0 0-1,0 1 0,-1-1 1,0 1-1,0-1 0,-1 1 0,1 8 1,-2-16 639,3-37-1078,9 14-219,1 2 0,1-1 0,0 2 0,22-24 0,6-10-422,-30 39 1033,-1-1 0,-1 0 0,-1-1 0,0 0 0,-1 0 0,10-37 0,-15 40 1363,0 1 0,-1 0-1,-1-23 959,-6 44-1425,-2 22-660,1 1 0,1 1-1,2-1 1,1 1 0,3 46-1,-1-35-222,1-32-230,-1 0 0,1 0 0,1 0 0,0-1 0,6 19 1,14 19-5521,-15-34 1388,-7-7 1244</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1798.32">901 354 7347,'0'0'10341,"10"-46"-11093,28 43-433,10 0-1120,1 3-1585,-1 0-2993</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2077.3">1270 302 288,'0'0'16848,"-9"3"-16165,7-2-674,0 0 1,0-1 0,-1 1-1,1 0 1,0 1-1,0-1 1,0 0 0,0 1-1,0-1 1,0 1-1,1-1 1,-1 1-1,0 0 1,1 0 0,-1 0-1,1 0 1,0 0-1,0 0 1,0 0 0,0 0-1,0 1 1,0-1-1,0 0 1,1 1 0,-1-1-1,1 0 1,0 1-1,-1-1 1,1 1-1,0-1 1,1 5 0,-1-7-33,0 1 1,1 0 0,-1 0-1,0-1 1,0 1 0,1 0-1,-1-1 1,1 1 0,-1 0 0,0-1-1,1 1 1,-1-1 0,1 1-1,-1-1 1,1 1 0,0-1-1,-1 1 1,1-1 0,-1 1-1,1-1 1,0 0 0,-1 1-1,1-1 1,0 0 0,0 0 0,-1 1-1,1-1 1,0 0 0,0 0-1,-1 0 1,1 0 0,1 0-1,30 0-182,-25-1 226,-4 2 0,0-1 0,1 0 0,-1 0 1,0-1-1,0 1 0,0-1 0,0 1 0,0-1 0,-1 0 0,1 0 0,0 0 0,0-1 0,0 1 0,-1-1 1,1 1-1,-1-1 0,1 0 0,-1 0 0,0 0 0,0 0 0,0 0 0,0-1 0,4-4 0,-4 0 97,1 1 0,-1 0 0,0-1-1,0 0 1,-1 1 0,0-1-1,0 0 1,-1 0 0,0-9 0,0 14-117,-1 1 0,1 0 0,-1-1 1,1 1-1,-1 0 0,0-1 1,1 1-1,-1 0 0,0 0 0,0-1 1,0 1-1,0 0 0,0 0 1,0 0-1,0 0 0,0 0 0,0 1 1,-1-1-1,1 0 0,0 0 1,-1 1-1,1-1 0,0 1 0,-1-1 1,1 1-1,-1 0 0,1-1 1,-1 1-1,1 0 0,-3 0 0,2 0-91,0-1 0,0 1 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0 0,0 1-1,0-1 1,0 0 0,0 1 0,0 0-1,0-1 1,1 1 0,-1 0 0,0 0-1,0 0 1,1 0 0,-1 0 0,0 0 0,1 1-1,-3 2 1,3-1-601,0 0 1,0 0-1,0 0 0,0 1 1,1-1-1,-1 1 0,1-1 1,0 5-1,0 6-5736</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2363.94">1654 219 10181,'0'0'6952,"-21"11"-6546,-64 38 125,80-46-473,1 1 0,0 0 0,0 1 0,0-1 0,0 1 1,1-1-1,-1 1 0,1 0 0,1 0 0,-1 1 1,1-1-1,0 1 0,0-1 0,0 1 0,1-1 0,0 1 1,0 0-1,0 0 0,1 0 0,0 0 0,0-1 0,1 12 1,0-3-79,-1-13 18,0 0 0,1 0 0,-1 0 1,0 1-1,1-1 0,-1 0 0,1 0 1,0 0-1,-1 0 0,1 0 1,0 0-1,0 0 0,0 0 0,0 0 1,0 0-1,0 0 0,0-1 0,0 1 1,0 0-1,0-1 0,0 1 1,0-1-1,0 1 0,1-1 0,-1 1 1,0-1-1,0 0 0,0 0 0,1 0 1,-1 1-1,2-2 0,51 3 77,-42-2-62,6-1-55,0 1 0,-1-2 0,28-6 0,-38 6-335,0 0 1,0 0 0,0-1 0,0 0 0,0 0-1,-1 0 1,0-1 0,1 0 0,-1-1 0,10-8 0,-3-6-4445</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -2596,7 +3126,7 @@
           <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
         </inkml:channelProperties>
       </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2025-01-04T15:30:31.488"/>
+      <inkml:timestamp xml:id="ts0" timeString="2025-02-22T15:37:41.358"/>
     </inkml:context>
     <inkml:brush xml:id="br0">
       <inkml:brushProperty name="width" value="0.035" units="cm"/>
@@ -2604,7 +3134,12 @@
       <inkml:brushProperty name="color" value="#004F8B"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">3127 179 3282,'0'0'10743,"-6"-10"-9887,-1-4-615,6 9-120,-2 1 0,1-1 0,0 0 0,-1 1 0,0 0-1,0-1 1,0 1 0,-8-6 0,6 6 6,0 0 1,0 1-1,-1 0 1,0 0-1,1 0 0,-1 1 1,0 0-1,0 0 1,-12-2-1,-60-6-75,74 9-25,-406-5 43,230 9-7,-327 19 220,413-16-233,-116-7 0,72-1-25,-141-5-37,-183 5-40,406 9-6,0 2-1,-103 30 0,32-5 139,-108 20 11,234-53-92,0-1-1,0 0 1,0 1 0,0-1 0,0 1-1,0-1 1,1 1 0,-1 0 0,0-1-1,0 1 1,1 0 0,-1-1 0,0 1 0,1 0-1,-1 0 1,1 0 0,-1 0 0,1-1-1,-1 1 1,1 0 0,0 0 0,0 0-1,-1 2 1,-3 34-60,13 34 19,-9-68 49,22 84 178,-5 1 0,-3 1 0,2 97 0,-16-178-171,0-1 0,1 1 0,0-1 0,0 0 0,0 1 0,1-1 0,1 0 0,-1 0 0,5 8 0,-6-12-6,1 0 0,0 1 0,1-1 0,-1 0 0,0 0 0,1-1 1,0 1-1,0-1 0,0 1 0,0-1 0,0 0 0,0 0 0,0 0 0,1 0 0,-1-1 0,1 1 0,-1-1 0,1 0 0,0 0 0,3 0 0,75 8 94,109-2 0,47 3-5,188 46-102,394 31-51,-457-81 74,265 17 20,-594-20-40,28 4 4,0-3 1,67-4-1,-126 0 3,0-1-1,0 0 1,1 1-1,-1-1 0,-1 0 1,1-1-1,0 1 1,0 0-1,0-1 1,-1 0-1,1 0 0,0 0 1,-1 0-1,0 0 1,0 0-1,1 0 0,-1-1 1,0 1-1,-1-1 1,1 0-1,0 1 0,-1-1 1,0 0-1,1 0 1,-1 0-1,0 0 0,-1 0 1,2-6-1,1-8 34,-1-1-1,0 0 1,-2-34-1,0 33-29,1-69-42,-4-113-181,0 169 189,-1 0 0,-1 1 0,-2-1 0,-14-39 0,-27-99 67,32 106-42,-33-162 124,48 220-54,1 5-125,-1 5-399,-1 0 0,1 1 0,-1-1 0,0 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,0-1 0,-6 5 0,4-2-965,-16 19-4767</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">16 89 4626,'0'0'13537,"-10"102"-11325,9-91-2172,-2 23 77,1 1-1,2 0 1,6 48 0,-5-81-121,1 0 1,-1-1-1,0 1 1,1 0 0,-1-1-1,1 0 1,0 1-1,-1-1 1,1 0 0,0 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0-1-1,0 1 1,0-1 0,0 1-1,0-1 1,0 0-1,0 0 1,1 0 0,-1 0-1,0 0 1,2-1-1,58-2 189,-52 1-186,0 0-1,0-1 1,0 0 0,-1-1 0,1 0 0,-1 0 0,0-1 0,0 0 0,-1 0 0,1-1 0,13-13 0,-16 13-26,-1 1 0,0-1 1,0 0-1,-1 0 0,1 0 1,-1 0-1,-1-1 0,1 0 0,-1 1 1,0-1-1,-1-1 0,1 1 1,-1 0-1,-1-1 0,0 1 0,1-12 1,-2 18 12,0 0 1,0 0 0,0 0-1,0 1 1,0-1-1,0 0 1,0 0 0,-1 0-1,1 0 1,0 1-1,-1-1 1,1 0 0,0 0-1,-1 1 1,1-1-1,-1 0 1,1 1 0,-1-1-1,1 0 1,-1 1-1,0-1 1,1 1 0,-1-1-1,0 1 1,1-1-1,-1 1 1,0-1 0,0 1-1,1 0 1,-1-1-1,0 1 1,0 0 0,0 0-1,1-1 1,-1 1-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0-1,1 0 1,-1 1 0,0-1-1,0 0 1,0 0-1,0 1 1,-1 0 0,0-1 11,-1 1 1,1 0 0,0 0 0,0 0 0,-1 0 0,1 1 0,0-1 0,0 0 0,0 1 0,0 0 0,1-1 0,-1 1-1,0 0 1,1 0 0,-1 0 0,-2 4 0,3-4-18,0 1 0,0-1 0,0 1-1,0-1 1,0 1 0,0 0 0,1-1 0,-1 1 0,1 0-1,0 0 1,-1 0 0,1-1 0,1 1 0,-1 0-1,0 0 1,1 0 0,1 3 0,-1-4-1,1 0 0,0-1-1,0 0 1,0 1 0,0-1 0,0 0 0,0 0 0,0 0 0,1 0-1,-1 0 1,0 0 0,0-1 0,1 1 0,-1-1 0,1 0-1,-1 1 1,0-1 0,1 0 0,-1 0 0,4-1 0,10 1-24,-1-1 1,0-1 0,0 0-1,0-1 1,0 0 0,-1-1 0,1-1-1,-1 0 1,19-11 0,-27 13 49,0 0 1,-1-1 0,1 0 0,-1 0 0,0 0-1,0-1 1,0 1 0,-1-1 0,1 0 0,-1-1 0,0 1-1,-1-1 1,0 0 0,1 0 0,-2 0 0,1 0 0,-1 0-1,0-1 1,0 1 0,-1-1 0,1 1 0,-2-1-1,1-9 1,-2 3 353,-1 11-143,-6 24-77,-7 42-99,9-31 21,1-1 1,2 1-1,1 0 1,2 0-1,1 0 1,10 60-1,-8-82-62,1 1 0,1-1 0,0 0 0,0-1 0,1 1-1,0-1 1,1 0 0,0-1 0,1 0 0,0 0-1,0 0 1,1-1 0,16 12 0,-25-20 4,1 1 0,0-1 1,0 1-1,0-1 0,0 1 1,0-1-1,1 1 0,-1-1 1,0 0-1,0 1 0,0-1 0,0 0 1,0 0-1,0 0 0,0 0 1,1 0-1,-1 0 0,0 0 1,0-1-1,0 1 0,0 0 0,0-1 1,0 1-1,0 0 0,0-1 1,1 0-1,0-1 11,-1 1-1,1-1 1,-1 0 0,1 1 0,-1-1-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0-3-1,2-6 13,-1 1 0,-1-1 1,1 0-1,-2-11 0,0 8-126,0-1 1,-2 1-1,1 0 1,-2 0-1,0 0 1,-1 1-1,-9-25 1,10 31 72,0 1 1,-1 0-1,1 0 1,-1 1 0,0-1-1,-1 1 1,0 0 0,1 0-1,-2 0 1,1 0 0,0 1-1,-1 0 1,0 0 0,0 1-1,0-1 1,0 1-1,-1 1 1,-8-3 0,-5 0 125,17 8-749,6-2 532,-1 0 0,1 0-1,0 0 1,0 0 0,0 0 0,0-1-1,0 1 1,0-1 0,-1 0 0,5 0 0,1 1 67,1-1 1,-1-1-1,0 0 1,0 0-1,0 0 1,1-1-1,-1 0 0,0-1 1,-1 0-1,1 0 1,-1 0-1,1-1 1,-1 0-1,0-1 1,0 0-1,-1 0 1,1 0-1,-1-1 1,0 1-1,-1-2 1,1 1-1,-1-1 1,-1 1-1,7-12 1,-7 6 367,0 0 1,-1 0 0,-1 0 0,0 0-1,0 0 1,-1-1 0,-1 1 0,-1-15-1,1 18 776,-3 117-943,1 71 538,3-172-682,0 0 0,0 0 1,0 0-1,1 0 0,0 0 0,0 0 1,1 0-1,0 0 0,0-1 0,1 0 0,6 10 1,-7-12-214,0-1 0,0 0 0,0 1 0,1-1 0,-1-1 0,1 1 0,-1 0 1,1-1-1,0 0 0,0 0 0,0 0 0,1 0 0,-1-1 0,0 1 0,1-1 0,-1 0 0,0 0 1,1-1-1,6 1 0,-9-1-267,-2 0 263,1 0-1,-1 0 0,1 0 1,-1 0-1,1 0 0,-1 0 0,1 0 1,-1 0-1,1 0 0,-1 0 1,1 0-1,-1 0 0,1 0 1,-1-1-1,1 1 0,-1 0 1,0 0-1,1 0 0,-1-1 1,1 1-1,-1 0 0,0-1 1,1 1-1,-1 0 0,1-1 1,-1 1-1,0 0 0,0-1 0,1 1 1,-1 0-1,0-1 0,0 1 1,1-1-1,-1 1 0,0-2 1,1-14-6924</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="138.75">661 351 5202,'0'0'11318,"27"-53"-12439,11 44-1264,-1 0-1089,12 3-4978</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="551.26">1247 141 8548,'0'0'10082,"-19"-2"-9167,-63-3-379,78 5-489,0 0 0,0 0 0,0 0 0,0 1 1,0 0-1,0 0 0,0 0 0,0 0 0,0 0 0,0 1 0,0 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1 1 0,0 0 0,0-1 0,0 1 0,0 0 1,-4 7-1,3-4-27,0 1 1,1-1 0,-1 1 0,2 0-1,-1 0 1,1 0 0,-1 0 0,2 0 0,-2 8-1,3-10-33,-1-1 0,1 1-1,0-1 1,1 1-1,-1-1 1,1 0 0,0 1-1,0-1 1,0 1-1,1-1 1,-1 0-1,1 0 1,0 0 0,0 0-1,0 0 1,1 0-1,0-1 1,-1 1-1,1-1 1,1 0 0,4 5-1,6 3-4,1-1 0,0-1-1,0 0 1,21 8 0,13 8 151,-48-25-134,0 0 1,0 0-1,-1 1 1,1-1-1,0 1 1,-1-1-1,1 0 1,0 1-1,-1-1 1,1 1-1,0-1 1,-1 1-1,1 0 1,-1-1-1,1 1 1,-1 0-1,1-1 1,-1 1-1,0 0 1,1-1-1,-1 1 1,0 0-1,1 0 1,-1-1-1,0 1 1,0 0-1,0 0 1,0 0-1,0-1 1,0 1-1,0 2 1,-1-2 22,0 1 0,0-1 1,0 0-1,0 1 1,0-1-1,-1 0 1,1 0-1,0 1 0,-1-1 1,1 0-1,-1 0 1,1-1-1,-3 2 0,-53 19 356,48-19-448,-15 2-754,24-4 665,-1 0-1,1 0 1,-1 0 0,0 0 0,1 0 0,-1-1 0,1 1 0,-1 0 0,1 0 0,-1-1 0,1 1 0,-1 0 0,1-1 0,0 1 0,-1 0 0,1-1 0,-1 1 0,1-1 0,0 1 0,-1-1 0,1 1 0,0-1 0,0 1-1,-1-1 1,1 1 0,0-1 0,0 1 0,0-1 0,0 0 0,-1 1 0,1-1 0,0 1 0,0-1 0,0 1 0,0-1 0,1-1 0,-1-23-7285</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="738.79">1317 224 9989,'0'0'8724,"0"111"-8372,6-81-80,-6 1-128,11-9-144,5-4-192,0-6-1137,0-6-1360,5-6-1617,1 0-2705</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="905.71">1497 142 7988,'0'0'10484,"-16"-10"-12244,16 35-81,5 0-2977,11-1-4771</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1573.86">1723 292 8516,'0'0'6048,"-20"-1"-3449,-64-3-1049,79 4-1476,0 0 0,0 0 1,0 1-1,1 0 1,-1 0-1,0 0 1,0 0-1,1 1 0,-1 0 1,1 0-1,-1 0 1,1 0-1,0 1 1,0-1-1,0 1 0,0 0 1,0 1-1,1-1 1,-1 1-1,1-1 1,0 1-1,0 0 0,1 0 1,-5 8-1,3-2-47,-1 0 0,1 0 0,1 1 0,0-1 0,1 1-1,0 0 1,0 0 0,0 20 0,2-29-43,0 0 1,1 0-1,-1 0 1,0 1-1,1-1 1,-1 0-1,1 0 1,-1-1-1,1 1 0,0 0 1,0 0-1,0 0 1,0 0-1,0-1 1,1 1-1,-1 0 1,0-1-1,1 1 1,-1-1-1,1 0 0,3 3 1,-1-2-2,0 0 1,0 0-1,1 0 1,-1 0-1,1-1 1,-1 0-1,1 0 1,0 0-1,7 0 1,-3 0-37,0-1 1,0-1-1,0 1 0,0-1 1,0-1-1,-1 0 1,1 0-1,0 0 0,-1-1 1,12-6-1,-5-1-87,-2 0 0,1-2 0,-1 1 1,-1-1-1,0-1 0,-1-1 0,0 1 0,-1-1 0,0-1 0,-1 0 1,-1-1-1,-1 1 0,0-1 0,5-21 0,-1 0 283,-2-1 1,-1 0-1,-3-1 0,0 0 1,-2-48-1,-5 138 1268,0-21-1331,1 1 1,1-1 0,2 1 0,8 42-1,-8-67-104,0 0-1,1 0 0,0 0 0,1 0 1,-1-1-1,1 1 0,0-1 1,0 0-1,1 0 0,-1-1 0,1 1 1,0-1-1,0 0 0,1 0 0,-1-1 1,1 1-1,0-1 0,0-1 1,0 1-1,0-1 0,0 0 0,1 0 1,-1-1-1,1 0 0,8 1 1,-9-1-6,0-1 1,1 1-1,-1-1 1,1 0-1,-1-1 1,1 0-1,-1 0 1,0 0-1,0-1 1,1 0 0,-1 0-1,0 0 1,-1-1-1,1 0 1,0 0-1,-1 0 1,0-1-1,1 0 1,-1 0-1,-1 0 1,1-1-1,-1 0 1,1 1 0,-2-1-1,8-11 1,-10 13 32,0 1 0,1-1 1,-1 0-1,0 0 0,0 0 1,-1 0-1,1-1 0,-1 1 1,1 0-1,-1 0 0,0 0 1,0 0-1,-1 0 0,1-1 1,-1-2-1,0 4 18,1 1 1,-1-1-1,0 1 0,0-1 0,0 1 1,0-1-1,0 1 0,0 0 0,0-1 1,0 1-1,0 0 0,0 0 0,-1 0 0,1 0 1,-1 0-1,1 0 0,0 0 0,-1 0 1,0 1-1,1-1 0,-1 1 0,1-1 1,-1 1-1,0-1 0,1 1 0,-1 0 1,-2 0-1,0-1 6,-1 1 1,1 0-1,0 0 0,-1 1 0,1-1 1,0 1-1,0 0 0,0 0 1,-1 0-1,1 1 0,0-1 0,0 1 1,1 0-1,-1 0 0,0 1 1,1-1-1,-1 1 0,1 0 0,0-1 1,0 2-1,0-1 0,0 0 1,0 0-1,1 1 0,-1 0 0,1-1 1,0 1-1,0 0 0,-1 5 1,-1 2-26,1 0 0,0 0 0,1 1 0,0-1-1,1 1 1,0-1 0,1 1 0,1-1 0,-1 1 0,4 12 0,-3-19-26,0-1 1,1 1-1,0 0 0,0 0 0,0-1 0,1 1 0,-1-1 0,1 0 0,0 0 0,0 0 1,1 0-1,-1 0 0,1-1 0,0 1 0,0-1 0,0 0 0,0-1 0,1 1 0,-1 0 0,1-1 1,-1 0-1,1 0 0,8 1 0,-3 0-521,1 0 0,-1-1 0,1 0 0,-1-1 0,1 0 0,0-1 0,0 0 0,-1-1 0,1 0 0,13-3 0,4-9-4004</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -2624,7 +3159,7 @@
           <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
         </inkml:channelProperties>
       </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2025-01-04T15:32:45.702"/>
+      <inkml:timestamp xml:id="ts0" timeString="2025-02-22T15:37:46.574"/>
     </inkml:context>
     <inkml:brush xml:id="br0">
       <inkml:brushProperty name="width" value="0.035" units="cm"/>
@@ -2632,11 +3167,9 @@
       <inkml:brushProperty name="color" value="#004F8B"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">90 27 4338,'0'0'8660,"0"-17"-3087,-2 41-5506,-1-1 0,0 0 0,-2 1-1,-14 37 1,-3 18-3,12-36-37,4-22-19,1 1-1,0-1 1,-1 38 0,5-63 111,0-4-107,0 0 0,0 0 0,1 0 0,1-16 0,10-33-21,3 0-1,2 1 0,2 1 1,28-57-1,-46 111 8,0 1 0,0-1 0,1 1 0,-1-1 0,0 0 0,0 1 0,0-1 0,1 1 0,-1-1 0,0 1 0,1-1 0,-1 1 0,0-1 0,1 1 0,-1-1 0,0 1 0,1-1 0,-1 1 0,1 0 0,-1-1 0,1 1 0,-1 0 0,1-1 0,-1 1 0,1 0 0,0 0 0,-1 0 0,1-1 0,-1 1 0,1 0 0,-1 0 0,1 0 0,0 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,0 0 0,-1 0 0,1 1 0,-1-1 0,1 0 0,0 0 0,-1 1 0,1-1 0,-1 0 0,1 0 0,-1 1 0,1-1 0,-1 1 0,0-1 0,1 0 0,-1 1 0,1-1 0,-1 1 0,0-1 0,1 2 0,16 31-39,-7-1 107,-1 1-1,-1 0 1,-2 0 0,-2 1 0,0 38 0,-2 32-6579,-4-92 2226,-7-4-2036</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="392.64">55 307 1313,'0'0'12336,"1"-9"-11661,-1 6-669,0-1 1,1 1-1,0 0 1,0-1-1,0 1 1,0-1-1,0 1 1,1 0-1,0 0 1,-1 0-1,1 0 1,3-4-1,1 2-16,-1 0-1,1 0 1,0 0-1,0 1 1,0 0-1,10-5 1,8-4-100,0 0 0,-1-2 0,-1-1 0,-1 0 0,30-31 1,-46 41 122,-1-1-1,0 1 1,0-1 0,-1 0 0,1-1 0,2-9 0,-2-1 4269,-24 274-3505,3-60-444,11-42-516,6-89-7117</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1122.77">268 463 1056,'0'0'2655,"0"-21"309,-2-12-1822,1 4 777,4-50 1,-2 74-1756,0-1-1,0 1 1,1 0-1,0 0 1,-1 0 0,2 1-1,-1-1 1,0 0-1,1 1 1,0-1 0,0 1-1,0 0 1,1 0-1,-1 0 1,1 1 0,0-1-1,0 1 1,0 0 0,1 0-1,-1 0 1,1 1-1,7-4 1,-1 2-36,-1 0 1,1 0-1,0 1 1,0 0-1,0 1 1,0 0-1,0 1 1,0 1-1,16 0 1,-25 0-85,-1 1 0,1 0 0,0-1 0,-1 1 0,0 0 0,1 0 0,-1 0 0,1 0 1,-1 0-1,0 0 0,0 1 0,0-1 0,1 0 0,-1 1 0,0-1 0,-1 0 0,1 1 1,0-1-1,0 1 0,-1 0 0,1-1 0,-1 1 0,1-1 0,-1 1 0,0 0 0,1-1 0,-1 1 1,0 0-1,0 0 0,0-1 0,0 1 0,-1 2 0,1 3 13,-1-1 0,1 1 1,-1-1-1,0 0 0,-1 0 0,1 1 0,-5 9 1,-1-6-18,0-1 0,0 1 0,-1-1 1,0-1-1,-1 0 0,0 0 1,-17 12-1,3-5-5,-1 0 0,-31 13-1,54-27-30,1-1 1,0 0-1,0 0 0,-1 1 0,1-1 0,0 0 0,-1 0 0,1 0 0,0 1 0,-1-1 0,1 0 0,0 0 0,-1 0 0,1 0 1,0 0-1,-1 0 0,1 0 0,0 1 0,-1-1 0,1 0 0,-1 0 0,1 0 0,0-1 0,-1 1 0,1 0 0,-1 0 0,1 0 1,0 0-1,-1 0 0,1 0 0,0 0 0,-1-1 0,1 1 0,0 0 0,-1 0 0,1-1 0,0 1 0,0 0 0,-1 0 0,1-1 1,0 1-1,5-18-158,21-22-467,9 6-305,65-47-1,-65 55 490,0-1 0,47-52 0,-79 76 460,-1 0 0,0 0 0,0 0-1,0 0 1,0 0 0,-1 0-1,1-1 1,-1 1 0,0 0 0,0-1-1,1-7 1,0-20 5072,-2 31-4945,-3 47-71,-10 62 0,-3 21 53,0 49-94,14-170-329,0-10 93,0-27-1,5-48 22,2 50 137,1 0 0,1 1 0,15-36 0,-19 53 27,0 0 1,0 1-1,1-1 1,0 1-1,1 0 1,0 1-1,0-1 1,0 1-1,1 0 1,0 0-1,0 1 1,0-1 0,1 1-1,-1 1 1,12-7-1,-14 10 1,-1-1 0,0 1 0,1 0 0,-1 0 1,1 0-1,-1 0 0,1 1 0,-1 0 0,1-1 0,0 1 0,-1 1 0,1-1 0,-1 0 0,1 1 0,-1 0 1,7 2-1,-8-2 6,0 0 0,0 1 0,0 0 0,-1-1 0,1 1 0,0 0 0,-1 0 0,1 0 0,-1 0 1,0 0-1,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 1 0,-1-1 0,1 0 0,-1 1 1,0-1-1,0 1 0,0-1 0,0 5 0,-1-1 40,0 1 0,0-1 1,0 0-1,-1-1 0,0 1 0,0 0 0,0 0 0,-1-1 1,0 1-1,0-1 0,-1 0 0,1 0 0,-1 0 1,-8 7-1,-9 9-16,-44 33 1,30-26-726,19-16-1151,4-10-4747</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1653.54">800 187 4610,'0'0'10568,"21"4"-9461,64 16-283,-83-19-779,0 0 1,1 0-1,-1 0 0,0 0 0,0 0 1,0 0-1,0 1 0,0-1 0,0 1 1,0 0-1,0-1 0,-1 1 0,1 0 0,-1 0 1,1 0-1,-1 0 0,0 0 0,1 1 1,-1-1-1,0 0 0,1 5 0,-1-1 75,0 1 0,-1 0 0,1-1 0,-1 1 0,-2 12 0,1-1 97,2-15-189,-1 1 1,0 0-1,0-1 1,0 1-1,-1 0 1,1-1 0,-1 1-1,0 0 1,0-1-1,0 1 1,-1-1-1,1 0 1,-1 1-1,0-1 1,1 0 0,-1 0-1,-1 0 1,1 0-1,0 0 1,-1-1-1,0 1 1,1-1-1,-1 1 1,0-1 0,0 0-1,0 0 1,-1 0-1,1-1 1,0 1-1,-1-1 1,1 0-1,-1 0 1,1 0 0,-1 0-1,0-1 1,-4 1-1,8-2-31,-1 0-1,0 0 0,1 0 1,-1 0-1,0 0 0,1 0 1,-1 0-1,1 0 1,0 0-1,-1 0 0,1 0 1,0 0-1,0-1 0,-1 1 1,1 0-1,0 0 1,0 0-1,0 0 0,1-1 1,-1 1-1,0-2 0,5-30-684,-1 25 567,0 0-1,1 0 1,0 1 0,0-1 0,1 1 0,0 0-1,0 1 1,1 0 0,-1 0 0,1 0-1,1 0 1,-1 1 0,1 1 0,0-1 0,13-4-1,-15 8 96,-5 37 1066,-7 65-141,7-100-903,0 0-1,0-1 1,0 1-1,0-1 1,-1 1-1,1-1 1,0 0 0,0 1-1,0-1 1,0 0-1,0 0 1,0 1-1,0-1 1,0 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0-1,0-1 1,2 1-1,23-4 79,-20 2-71,0-1-1,1 0 1,-1 0 0,-1-1-1,1 0 1,0 0 0,-1 0-1,0-1 1,0 0 0,0 0-1,-1 0 1,0 0 0,0-1-1,6-10 1,-5 8 22,-1-1-1,0 0 1,-1 0-1,0-1 1,0 1-1,-1-1 1,0 0 0,-1 1-1,1-17 1,-3 25 2,1 0 0,0-1 1,-1 1-1,1-1 0,-1 1 1,1 0-1,-1 0 0,0-1 1,1 1-1,-1 0 0,0 0 1,0 0-1,0-1 1,0 1-1,0 0 0,0 0 1,0 1-1,0-1 0,-1 0 1,1 0-1,0 0 0,0 1 1,-1-1-1,1 1 0,0-1 1,-1 1-1,1 0 0,-1-1 1,1 1-1,-1 0 0,1 0 1,0 0-1,-1 0 1,-1 0-1,1 0-110,0 0 1,0 0 0,1 1-1,-1-1 1,0 0 0,0 1-1,0 0 1,0-1-1,1 1 1,-1 0 0,0 0-1,-2 1 1,3-1-149,0 0-1,0 0 1,0 0 0,0 0 0,1 0-1,-1 0 1,0 0 0,0 0 0,1 0 0,-1 0-1,1 1 1,-1-1 0,1 0 0,-1 0 0,1 0-1,0 1 1,0-1 0,0 0 0,-1 3-1,5 6-4399,14-8-1145</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2003.84">1367 153 6307,'0'0'13275,"-4"9"-12621,-12 26-280,-2-2 0,-31 45 0,0-1-4127,48-97-10501,-2-20 13486,2 12 1418,1-17 3886,0 36 255,2 19 2245,-1-5-7015,0 0 1,0 0 0,1 1 0,0-1-1,0 0 1,0-1 0,1 1 0,0 0-1,0-1 1,0 1 0,0-1 0,0 0-1,1 0 1,7 6 0,7 4 14,0 0 1,26 14-1,13 10-1285,-56-38 962,0 1-1,-1-1 1,1 1-1,0-1 1,0 1 0,-1 0-1,1-1 1,0 1-1,-1 0 1,1 0-1,-1-1 1,1 1 0,-1 0-1,1 0 1,-1 0-1,0 0 1,1 0 0,-1-1-1,0 1 1,0 0-1,1 2 1,-1 4-6778</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">184 179 3922,'0'0'12622,"-14"-4"-11987,14 4-633,-12-3 96,0 0 1,0 1-1,0 0 0,0 1 1,-20 0-1,29 1-87,0 0-1,0 1 1,0-1-1,1 0 1,-1 1-1,0 0 1,0 0-1,1-1 1,-1 2-1,1-1 1,-1 0-1,1 0 1,-1 1-1,1 0 1,0-1 0,-1 1-1,1 0 1,0 0-1,0 0 1,1 0-1,-1 0 1,0 1-1,1-1 1,-1 0-1,1 1 1,0-1-1,0 1 1,0 0-1,0-1 1,0 1-1,1 0 1,-1 0-1,1-1 1,-1 1-1,1 0 1,1 5-1,-2-4-41,1 0-1,1 0 1,-1 0-1,1 0 1,-1 0 0,1 0-1,0 0 1,0 0-1,1-1 1,-1 1-1,1 0 1,0-1-1,4 6 1,-1-3-47,1 0-1,0 0 1,0-1 0,1 0 0,9 6 0,-6-4-24,0 0 0,-1 0 1,0 1-1,9 9 0,-15-13 65,-1-1 0,1 0-1,-1 1 1,0 0 0,0-1 0,0 1-1,0 0 1,0 0 0,-1 0 0,0 0-1,0 0 1,0 1 0,0-1 0,0 7-1,-2-9 95,0 0-1,0-1 0,0 1 0,0 0 0,-1-1 0,1 1 1,0-1-1,-1 0 0,1 1 0,-1-1 0,1 0 0,-1 0 1,1 0-1,-1 0 0,0 0 0,0 0 0,0 0 0,1-1 0,-1 1 1,0-1-1,0 1 0,-3 0 0,-49 8 939,-8-8-2705,60-10-6710</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1452.67">210 256 8628,'0'0'7505,"4"10"-6673,26 123 934,-26-128-1154,2-14-272,11-34-185,-12 30-137,-1 0 0,2 1 0,11-21 0,-17 33-14,0 0 0,1-1 0,-1 1 0,0 0 0,0 0 0,1-1 0,-1 1 0,0 0 0,1 0 0,-1 0 0,0-1 0,1 1 1,-1 0-1,0 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,0 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,1 0 0,-1 0 0,0 1 0,1-1 0,-1 0 0,1 0 0,-1 0 0,0 1 0,0-1 0,1 0 0,-1 0 0,0 1 0,1-1 0,-1 0 0,0 0 0,0 1 0,0-1 0,1 0 0,-1 1 0,0-1 0,0 0 0,0 1 0,0-1 0,0 1 0,1-1 0,-1 0 0,0 1 0,9 27 165,-7-21 15,35 99 747,-36-105-971,-1 0 0,1 0-1,0 0 1,-1-1 0,1 1 0,0 0-1,-1 0 1,1-1 0,0 1 0,0 0-1,0-1 1,0 1 0,-1-1-1,1 1 1,0-1 0,0 0 0,0 1-1,0-1 1,0 0 0,0 0 0,0 0-1,0 1 1,0-1 0,0 0 0,0 0-1,0-1 1,0 1 0,0 0 0,0 0-1,0 0 1,0-1 0,2 1-1,30-15-2031,19-34-1882,-49 46 3812,0-1 0,0 0-1,-1 0 1,1 1-1,-1-1 1,0-1 0,0 1-1,0 0 1,0 0-1,-1-1 1,0 1 0,0-1-1,1-5 1,0 4 1593,4 13 657,3 13-1102,4 13-389,-11-30-1091,0 0-1,1 0 1,-1 0-1,1 0 1,0 0 0,0 0-1,0-1 1,0 1 0,0-1-1,7 4 1,-8-5 128,1 0 0,-1 0 0,0-1 0,1 1 0,-1 0 0,1-1 0,-1 0 0,1 1 0,-1-1 0,1 0 0,0 0 0,-1 0 0,1-1 0,-1 1 0,1-1 0,4-1 0,-5 1 295,1 0 0,0-1 0,-1 1-1,1-1 1,-1 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,3-4 0,-3 2 387,0 0 0,0 1 0,0-1 1,-1 0-1,0-1 0,0 1 0,0 0 1,0 0-1,-1 0 0,1-1 1,-1 1-1,0 0 0,-1-8 0,1-2 2296,-1 13-2487,1 1 1,0-1-1,-1 0 0,1 0 1,-1 1-1,1-1 1,-1 0-1,1 1 0,-1-1 1,1 1-1,-1-1 0,1 1 1,-1-1-1,0 1 1,1-1-1,-1 1 0,0-1 1,0 1-1,1 0 0,-1-1 1,0 1-1,0 0 1,0 0-1,1 0 0,-1 0 1,0-1-1,0 1 0,0 0 1,1 0-1,-1 1 0,0-1 1,0 0-1,0 0 1,0 0-1,1 0 0,-1 1 1,0-1-1,0 0 0,1 1 1,-2 0-1,-1 0-123,-1-1-1,1 1 0,0 1 1,0-1-1,-1 0 0,1 1 0,0 0 1,1-1-1,-5 4 0,3 1-18,0 0-1,0 0 0,1 0 0,0 0 1,0 0-1,0 1 0,1-1 0,0 1 0,0 0 1,1-1-1,-1 12 0,4-17-109,0 0-1,0 0 0,0-1 1,1 1-1,-1-1 1,0 0-1,0 1 1,1-1-1,-1 0 1,0 0-1,1-1 0,-1 1 1,0 0-1,0-1 1,3-1-1,-1 0-19,0 0-1,0 0 0,0-1 1,0 0-1,-1 1 0,1-2 1,-1 1-1,0 0 1,0-1-1,0 1 0,0-1 1,-1 0-1,1 0 0,-1 0 1,0 0-1,0 0 1,1-5-1,0-1 564,0 0 0,-1 0 1,0 0-1,0 0 0,-1-18 0,-1 43-159,0-6-189,-1 0 1,2-1-1,-1 1 0,1 0 1,4 12-1,-5-19-82,1 1 0,0-1-1,0 0 1,0 0 0,0-1-1,0 1 1,0 0 0,1 0-1,-1 0 1,0-1 0,1 1-1,0-1 1,-1 1 0,1-1-1,0 0 1,0 0 0,-1 1-1,1-1 1,0-1 0,0 1-1,0 0 1,1 0 0,-1-1-1,0 1 1,0-1 0,0 1 0,4-1-1,-1 1-7,1-1 1,-1 1-1,0-1 0,1 0 0,-1 0 1,0-1-1,1 1 0,-1-1 0,0-1 1,0 1-1,0-1 0,0 0 0,0 0 1,0 0-1,0 0 0,-1-1 0,1 0 1,-1 0-1,0 0 0,0-1 0,0 1 1,0-1-1,0 0 0,-1 0 0,0-1 1,0 1-1,0 0 0,0-1 0,-1 0 1,1 0-1,1-7 0,3-10 20,-1 0-1,0-1 1,-2 0-1,-1 0 1,0 0-1,-2-1 1,-1 1-1,-4-37 1,-10 27 39,14 32-54,0 1 0,0-1 0,-1 1 1,1-1-1,0 1 0,0 0 0,-1-1 1,1 1-1,0-1 0,-1 1 0,1 0 1,-1-1-1,1 1 0,-1 0 0,1-1 1,0 1-1,-1 0 0,1 0 0,-1-1 1,1 1-1,-1 0 0,1 0 0,-1 0 1,0 0-1,1 0 0,-1 0 0,1 0 1,-1 0-1,1 0 0,-1 0 0,1 0 0,-1 0 1,1 0-1,-1 0 0,1 0 0,-1 0 1,1 1-1,-1-1 0,1 0 0,-1 0 1,1 1-1,-1-1 0,1 0 0,-1 1 1,1-1-1,0 0 0,-1 1 0,1-1 1,0 1-1,-1-1 0,1 1 0,0-1 1,0 1-1,-1-1 0,1 1 0,0-1 1,0 1-1,0-1 0,0 1 0,-1-1 1,1 1-1,0 0 0,-6 15 35,1 1 0,0 0-1,1-1 1,1 2 0,-2 31-1,4-6 28,5 54-1,-3-93-66,-1 1 1,1 0-1,0-1 0,0 1 1,0-1-1,1 0 0,-1 1 1,1-1-1,0 0 0,0 0 1,1 0-1,-1 0 0,1-1 1,0 1-1,0-1 0,0 1 0,1-1 1,-1 0-1,1 0 0,5 4 1,-6-6-3,0 0 0,0 0 0,0 0 0,0 0-1,0 0 1,1-1 0,-1 1 0,0-1 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,0-1 0,0 0 0,0 1-1,0-1 1,0 0 0,0-1 0,0 1 0,0 0 0,0-1 0,0 0 0,-1 1 0,1-1 0,-1 0 0,1-1 0,-1 1 0,4-5-1,-1 1-7,1-1 0,-1 0 0,0 0-1,-1-1 1,0 1 0,0-1-1,0 0 1,-1 0 0,-1 0 0,1-1-1,1-11 1,0-7-42,-2 1-1,-2-36 1,0 39 20,0 23 59,1-1 0,-1 1 0,0-1 0,0 1 0,0 0 0,0-1 0,0 1 0,0-1 0,0 1-1,0-1 1,0 1 0,-1-1 0,1 1 0,0 0 0,0-1 0,0 1 0,0-1 0,-1 1 0,1 0 0,0-1-1,0 1 1,-1-1 0,1 1 0,0 0 0,-1 0 0,1-1 0,0 1 0,-1 0 0,1-1 0,0 1 0,-1 0 0,1 0-1,-1 0 1,1-1 0,0 1 0,-1 0 0,0 0 0,0 0-2,0 1-1,0-1 0,0 0 1,1 1-1,-1-1 1,0 1-1,0-1 1,1 1-1,-1-1 1,0 1-1,1 0 0,-1-1 1,1 1-1,-1 0 1,1 0-1,-1-1 1,1 1-1,-1 0 1,1 0-1,0 0 1,-1 1-1,-7 24-23,2-1 1,1 1-1,1 0 0,1 0 1,1 1-1,1-1 0,5 43 1,-4-66-162,0-1 1,1 1 0,-1 0-1,1-1 1,-1 1 0,1-1 0,0 0-1,0 1 1,0-1 0,0 0-1,1 1 1,-1-1 0,2 2-1,-1-3-268,-1 0-1,0 0 0,0 0 0,1 0 1,-1 0-1,0 0 0,1-1 0,-1 1 0,1 0 1,-1-1-1,1 1 0,-1-1 0,1 0 0,-1 1 1,2-1-1,18 0-8744</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1977.1">1173 244 11941,'0'0'5232,"-2"10"-5032,-3 29-197,5-38-7,0 0-1,1 0 1,-1-1 0,0 1 0,1 0-1,-1-1 1,0 1 0,1 0 0,-1-1-1,1 1 1,-1 0 0,1-1 0,-1 1-1,1-1 1,0 1 0,-1-1 0,1 1-1,-1-1 1,1 1 0,0-1 0,0 0-1,-1 1 1,1-1 0,0 0 0,0 0-1,-1 0 1,1 1 0,0-1-1,0 0 1,0 0 0,-1 0 0,1 0-1,0 0 1,0-1 0,0 1 0,26-7-48,-24 1 65,-1-1 0,0 1 0,0-1 0,-1 0 0,0 0 0,0 0 0,0 0 0,-1 0 0,-1-12 0,1 11 179,0 8-127,0-1-1,0 1 1,0-1-1,0 1 1,0-1-1,0 1 1,-1-1-1,1 1 1,0-1-1,0 1 1,0-1-1,-1 1 0,1 0 1,0-1-1,0 1 1,-1-1-1,1 1 1,0 0-1,-1-1 1,1 1-1,-1 0 1,1-1-1,0 1 1,-1 0-1,1-1 1,-1 1-1,1 0 1,-1 0-1,1 0 1,-1 0-1,1-1 0,-1 1 1,1 0-1,-1 0 1,1 0-1,-1 0 1,1 0-1,-1 0 1,1 0-1,-1 0 1,1 0-1,-1 0 1,1 1-1,-2-1 1,1 0-27,0 1 0,0-1 0,0 0 0,0 1 0,0-1 0,-1 1-1,1-1 1,0 1 0,0-1 0,0 1 0,0 0 0,1 0 0,-1 0 0,0-1 0,0 1 0,0 0 0,1 0 0,-2 1 0,1 2-126,0-1 0,0 1 0,0-1 0,0 1 0,0 0 0,1-1 0,0 1 0,0 0 0,0-1 0,0 1 0,1-1 0,-1 1-1,1 0 1,0-1 0,1 4 0,-1-5-217,0 0 0,0 0-1,1 0 1,-1 0 0,0 0-1,1-1 1,0 1 0,-1 0 0,1-1-1,0 1 1,0-1 0,-1 0-1,1 0 1,0 0 0,0 0 0,0 0-1,1 0 1,-1 0 0,0-1-1,0 1 1,0-1 0,1 1-1,-1-1 1,4 0 0,8 1-2143,1-1 0,0 0-1,15-3 1,1-6 1497,-30 9 1252,-1 0 1,0 0-1,1 0 0,-1 0 0,0 0 0,1 0 1,-1 0-1,0 0 0,1 0 0,-1 0 0,0 0 1,1 0-1,-1 0 0,0 1 0,1-1 0,-1 0 1,0 0-1,1 0 0,-1 0 0,0 1 0,0-1 1,1 0-1,-1 0 0,0 1 0,0-1 0,1 0 1,-1 0-1,0 1 0,0-1 0,0 0 0,0 0 1,1 1-1,-1-1 0,0 0 0,0 1 0,0-1 1,0 0-1,0 1 0,0-1 0,0 0 0,0 1 1,2 25 2797,-7 21-1700,0-36 371,1-24-296,2-22-694,2 26-828,0-1 1,1 1-1,0 0 0,1-1 1,0 1-1,0 0 1,1 0-1,0 0 1,1 0-1,0 0 1,0 1-1,1 0 0,0 0 1,1 0-1,0 1 1,8-9-1,80-85-5154,-46 52-566</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -2656,7 +3189,7 @@
           <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
         </inkml:channelProperties>
       </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2025-01-04T15:32:56.081"/>
+      <inkml:timestamp xml:id="ts0" timeString="2025-02-22T15:37:44.421"/>
     </inkml:context>
     <inkml:brush xml:id="br0">
       <inkml:brushProperty name="width" value="0.035" units="cm"/>
@@ -2664,7 +3197,11 @@
       <inkml:brushProperty name="color" value="#004F8B"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">236 53 10373,'0'0'10458,"0"-12"-9716,1-15-519,-1 14 924,-6 52-717,-11 71-374,-14 131 14,27-96-24,-4 34-10,8-178-30,0 1-1,0 0 0,0-1 0,0 1 1,0 0-1,0 0 0,-1-1 0,1 1 0,-1 0 1,1-1-1,-1 1 0,0-1 0,1 1 0,-1-1 1,0 1-1,0-1 0,0 0 0,0 1 1,0-1-1,-1 0 0,1 0 0,0 0 0,0 1 1,-1-1-1,1-1 0,-1 1 0,1 0 0,-1 0 1,1-1-1,-1 1 0,0 0 0,1-1 1,-1 0-1,0 1 0,1-1 0,-1 0 0,0 0 1,1 0-1,-1 0 0,0 0 0,-3-1 0,1 0 8,0 0 0,0-1-1,0 0 1,0 0 0,0 0-1,0 0 1,1 0-1,-1-1 1,1 0 0,-1 1-1,1-1 1,0-1-1,0 1 1,-4-6 0,-4-10-20,1-1 0,0 0 1,2 0-1,0-1 0,-9-43 1,21 82-596,13 26 502,-6-25 100,61 96 74,-61-99-61,0 0 0,1-2 0,1 1 0,28 23 0,-39-37-11,0 0 0,0 1 0,0-1 0,-1 0 0,1 0 0,0 0 0,0-1 0,0 1 0,1 0 0,-1-1 1,0 1-1,0-1 0,0 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,0-1 0,0 1 0,0-1 0,0 0 0,0 1 1,0-1-1,0 0 0,0 0 0,0 0 0,0-1 0,0 1 0,2-3 0,4-3 21,1-2-1,-2 1 1,1-1-1,10-17 1,-10 14-5,17-25-246,-2 0 0,-1-2 0,-2 0 0,-2-2 1,-2 0-1,19-70 0,-33 87-774,-3 17-3826</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">111 0 7123,'0'0'9714,"-7"21"-8647,-36 100-575,26-77-232,1 1 0,-10 48 1,26-93-260,0 0 1,0 0-1,0 0 0,0 0 1,0 0-1,-1 0 0,1 0 1,0 0-1,0 0 1,0 0-1,0 0 0,0 0 1,0 0-1,0 0 1,-1 0-1,3-26 48,6-38 27,-3 44-70,-1 2 16,0 0-1,1 0 1,1 0-1,1 1 1,0-1-1,17-26 1,-24 44-8,1-1 1,-1 0-1,0 1 1,1-1-1,-1 1 1,1-1-1,-1 1 1,1 0-1,-1-1 0,1 1 1,-1-1-1,1 1 1,-1 0-1,1-1 1,0 1-1,-1 0 1,1 0-1,-1 0 1,1-1-1,0 1 0,-1 0 1,1 0-1,0 0 1,-1 0-1,1 0 1,0 0-1,-1 0 1,1 0-1,0 0 1,0 1-1,17 16 231,8 37 114,-22-46-205,8 22-264,0 1-1,-2 0 1,-1 0 0,6 38-1,-9 17-8523,-6-69 1823</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="172.72">57 289 10037,'0'0'6066,"86"-77"-7474,-38 65-1153,-5 0-305,6-7-1184,-17 4 497</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="573.28">363 79 208,'0'0'14810,"0"-7"-13202,0-16-784,0 45-458,0 58 349,0 0-513,3 159 215,11-82-3837,-10-144-925,-1-24 3133,0-23 1377,-4-17 519,0 10 602,4-42 1,-2 72-1006,1 1 1,0-1-1,0 1 0,1-1 0,0 1 1,1 0-1,0 0 0,0 1 0,7-11 1,-10 18-264,0 0 0,1 0 0,-1 0 0,0 1 0,1-1 0,-1 0 0,1 1 1,0-1-1,-1 1 0,1-1 0,0 1 0,0 0 0,0 0 0,0-1 1,0 2-1,0-1 0,1 0 0,-1 0 0,0 1 0,0-1 0,1 1 1,-1-1-1,0 1 0,0 0 0,1 0 0,-1 0 0,0 1 0,1-1 1,-1 0-1,0 1 0,4 1 0,-3-1 20,-1 0 0,1 1-1,-1 0 1,0-1 0,1 1 0,-1 0 0,0 0 0,0 0-1,-1 0 1,1 1 0,0-1 0,-1 0 0,1 1-1,-1-1 1,0 1 0,1 0 0,-1-1 0,-1 1 0,1 0-1,0 0 1,-1 0 0,1-1 0,-1 1 0,0 4 0,0 0 32,1 0 1,-2 0-1,1-1 1,-1 1-1,0 0 1,0-1-1,-1 1 1,0 0-1,0-1 1,-1 0-1,0 0 1,0 1-1,0-2 1,-1 1-1,0 0 1,0-1-1,0 1 1,0-1 0,-1-1-1,0 1 1,0 0-1,-10 5 1,9-6-228,-37 24 240,14-19-3766,28-14-756,1-18-2055</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="990.92">525 129 2577,'0'0'15509,"3"14"-15085,19 104 724,6 139 1,-28-187-1299,0-69 230,0-16 467,0-24-487,-2 15-43,2 1 0,1-1 0,6-38 0,-6 57-31,0-1-1,1 1 0,-1 0 1,1 0-1,0 0 0,0 0 1,1 0-1,0 0 0,0 0 1,0 1-1,0-1 0,1 1 1,-1 0-1,1 0 0,0 0 1,0 1-1,1-1 0,-1 1 1,1 0-1,0 1 0,5-4 1,-8 5-3,0 0 1,-1 1 0,1-1 0,0 0 0,0 1 0,-1-1 0,1 1-1,0 0 1,0 0 0,0 0 0,0-1 0,0 2 0,0-1-1,-1 0 1,1 0 0,0 1 0,0-1 0,0 0 0,1 2-1,-2-1-2,0-1-1,0 1 0,0 0 1,0 0-1,0 0 0,0 0 1,0 0-1,-1 1 0,1-1 1,0 0-1,-1 0 0,1 0 1,-1 1-1,1-1 0,-1 0 1,0 0-1,1 1 0,-1-1 1,0 0-1,0 2 0,0 3-9,0 0 0,-1-1 0,0 1 0,0-1 0,0 1 0,0-1 0,-1 1-1,0-1 1,0 0 0,-5 9 0,-3-1-112,0 0-1,0-1 1,-2 0 0,1-1-1,-15 11 1,21-46-13844,14-8 8785</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1241">708 298 3362,'0'0'10231,"20"-4"-9012,68-4-168,-84 9-991,0-1 1,-1 1-1,1 0 0,0 0 0,-1 0 0,1 0 0,-1 1 1,1-1-1,-1 1 0,0 0 0,0 0 0,0 0 0,0 1 0,0-1 1,0 1-1,0-1 0,-1 1 0,1 0 0,-1 0 0,3 5 1,1 3 49,0-1 1,-1 2-1,0-1 1,3 13-1,-8-24-109,3 10 33,-1-1 0,-1 0 1,0 1-1,0-1 0,-1 18 0,0-12 388,-1-15-338,1 0 1,-1 0-1,1-1 0,-1 1 0,1 0 0,-1 0 1,1 0-1,-1-1 0,1 1 0,-1 0 1,1-1-1,0 1 0,-1 0 0,1-1 0,-1 1 1,1-1-1,0 1 0,0-1 0,-1 1 1,1 0-1,0-1 0,0 1 0,-1-1 1,1 1-1,0-1 0,0 0 0,0 0 0,-3-17 42,2-1 0,0 0-1,3-37 1,-1 47-259,0-1 1,1 1-1,0 0 1,1-1 0,0 1-1,0 0 1,1 0 0,0 1-1,9-15 1,-11 20-88,1 0 0,0 0 1,0 0-1,0 0 0,0 0 1,0 1-1,1-1 0,-1 1 1,1 0-1,-1 0 0,1 0 1,0 1-1,0-1 0,4 0 1,39-3-7166,-21 5 542</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -2868,8 +3405,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:J1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView tabSelected="1" topLeftCell="D19" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -2877,7 +3414,7 @@
     <col min="1" max="1" width="8.73046875" customWidth="1"/>
     <col min="2" max="2" width="25" customWidth="1"/>
     <col min="3" max="3" width="8.73046875" customWidth="1"/>
-    <col min="4" max="4" width="20.46484375" customWidth="1"/>
+    <col min="4" max="4" width="112.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="26" width="8.73046875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2963,10 +3500,7 @@
     </row>
     <row r="11" spans="2:10" ht="14.25" x14ac:dyDescent="0.45">
       <c r="B11" s="8"/>
-      <c r="C11" s="9" t="str">
-        <f>VLOOKUP(B8,B5:D8,2,0)</f>
-        <v>Q4 2013</v>
-      </c>
+      <c r="C11" s="9"/>
       <c r="D11" s="26" t="s">
         <v>14</v>
       </c>
@@ -2975,10 +3509,7 @@
     </row>
     <row r="12" spans="2:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B12" s="8"/>
-      <c r="C12" s="9">
-        <f>VLOOKUP(B8,B5:D8,3,0)</f>
-        <v>3000</v>
-      </c>
+      <c r="C12" s="9"/>
       <c r="D12" s="26" t="s">
         <v>15</v>
       </c>
@@ -3013,117 +3544,136 @@
       <c r="F15" s="25"/>
     </row>
     <row r="16" spans="2:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="17" spans="5:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="18" spans="5:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="H18" t="s">
-        <v>4</v>
+    <row r="17" spans="5:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="18" spans="5:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="19" spans="5:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="E19">
+        <f>VLOOKUP(1600,G19:G23,1,1)</f>
+        <v>1000</v>
+      </c>
+      <c r="G19">
+        <v>1500</v>
       </c>
     </row>
-    <row r="19" spans="5:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="H19">
+    <row r="20" spans="5:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="G20">
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="21" spans="5:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="G21">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="22" spans="5:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="G22">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="23" spans="5:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="G23">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="24" spans="5:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="25" spans="5:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="E25">
+        <f>VLOOKUP(1600,_xlfn.ANCHORARRAY(G25),1,1)</f>
         <v>1500</v>
       </c>
-      <c r="J19">
+      <c r="G25" cm="1">
+        <f t="array" ref="G25:G29">_xlfn._xlws.SORT(G19:G23)</f>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="26" spans="5:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="G26">
         <v>1000</v>
       </c>
     </row>
-    <row r="20" spans="5:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="E20">
+    <row r="27" spans="5:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="G27">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="28" spans="5:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="G28">
         <v>1800</v>
       </c>
-      <c r="H20">
+    </row>
+    <row r="29" spans="5:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="G29">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="30" spans="5:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="31" spans="5:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="32" spans="5:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="F32">
+        <f>VLOOKUP("S*",H32:I36,2,1)</f>
+        <v>1500</v>
+      </c>
+      <c r="H32" s="45" t="s">
+        <v>81</v>
+      </c>
+      <c r="I32">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="33" spans="6:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="H33" s="45" t="s">
+        <v>82</v>
+      </c>
+      <c r="I33">
         <v>1000</v>
       </c>
-      <c r="J20">
+    </row>
+    <row r="34" spans="6:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="H34" s="45" t="s">
+        <v>83</v>
+      </c>
+      <c r="I34">
         <v>1500</v>
       </c>
     </row>
-    <row r="21" spans="5:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="H21">
-        <v>2500</v>
-      </c>
-      <c r="J21">
+    <row r="35" spans="6:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="H35" s="45" t="s">
+        <v>84</v>
+      </c>
+      <c r="I35">
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="36" spans="6:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="H36" s="45" t="s">
+        <v>85</v>
+      </c>
+      <c r="I36">
         <v>2000</v>
       </c>
     </row>
-    <row r="22" spans="5:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="H22">
-        <v>2000</v>
-      </c>
-      <c r="J22">
-        <v>2500</v>
+    <row r="37" spans="6:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="38" spans="6:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="39" spans="6:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="40" spans="6:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="41" spans="6:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="F41" t="e">
+        <f>VLOOKUP("*ma*",H32:I36,2,1)</f>
+        <v>#N/A</v>
       </c>
     </row>
-    <row r="23" spans="5:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="H23">
-        <v>5000</v>
-      </c>
-      <c r="J23">
-        <v>3000</v>
+    <row r="42" spans="6:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="43" spans="6:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="F43">
+        <f>VLOOKUP("Sac*",H32:I36,2,1)</f>
+        <v>1500</v>
       </c>
     </row>
-    <row r="24" spans="5:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="H24">
-        <v>3000</v>
-      </c>
-      <c r="J24">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="25" spans="5:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="26" spans="5:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="27" spans="5:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="E27" t="e">
-        <f>VLOOKUP(E20,H19:H24,1,0)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="28" spans="5:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="29" spans="5:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="H29">
-        <f>VLOOKUP(E20,H19:H24,1,1)</f>
-        <v>1000</v>
-      </c>
-      <c r="J29">
-        <f>VLOOKUP(E20,J19:J24,1,1)</f>
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="30" spans="5:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="31" spans="5:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="H31" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="32" spans="5:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="33" spans="2:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B33" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="34" spans="2:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="F34" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="35" spans="2:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="F35" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="36" spans="2:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="37" spans="2:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="38" spans="2:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="39" spans="2:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="40" spans="2:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="41" spans="2:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="42" spans="2:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="43" spans="2:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="44" spans="2:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="45" spans="2:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="46" spans="2:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="47" spans="2:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="48" spans="2:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="44" spans="6:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="45" spans="6:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="46" spans="6:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="47" spans="6:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="48" spans="6:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="49" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="50" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="51" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -8543,8 +9093,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B1:H1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -8658,7 +9208,7 @@
         <v>45</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E11" s="4" t="str">
         <f>INDEX(B2:C7,MATCH(C11,C2:C7,0),1)</f>
@@ -8677,7 +9227,7 @@
         <v>47</v>
       </c>
       <c r="D12" s="17" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E12" s="4" t="str">
         <f>INDEX(B2:C7,MATCH(C12,C2:C7,0),MATCH(B2,B2:C2,0))</f>

</xml_diff>